<commit_message>
Lots of ch4 proofreading
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="names-名前" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4258" uniqueCount="2925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4262" uniqueCount="2927">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -8861,6 +8861,12 @@
   </si>
   <si>
     <t>英語</t>
+  </si>
+  <si>
+    <t>回復</t>
+  </si>
+  <si>
+    <t>Cures</t>
   </si>
 </sst>
 </file>
@@ -9589,8 +9595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -13464,7 +13470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -16705,10 +16711,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
@@ -16949,6 +16955,22 @@
         <v>198</v>
       </c>
     </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="s">
+        <v>2925</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>2926</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>2003</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16961,8 +16983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView topLeftCell="C52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="C20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -22617,7 +22639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
All items and states have been translated!
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4907" uniqueCount="3497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4929" uniqueCount="3519">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -10565,9 +10565,6 @@
     <t>A technique that drains enemy levels in exchange for pleasure.</t>
   </si>
   <si>
-    <t>Faints a foe by massaging their crotch with the soles of her feet.</t>
-  </si>
-  <si>
     <t>A technique that arouses foes by moving sexually and lascivously.</t>
   </si>
   <si>
@@ -10578,6 +10575,75 @@
   </si>
   <si>
     <t>A sigh filled with pheromones that inflicts 2 or more abnormal states.</t>
+  </si>
+  <si>
+    <t>A spear made by woodland sprites. It quietens the user's mind and movements.</t>
+  </si>
+  <si>
+    <t>A staff made by woodland sprites. It quietens the user's mind and movements.</t>
+  </si>
+  <si>
+    <t>A spear with superior durability.</t>
+  </si>
+  <si>
+    <t>A spear that will almost always hit it's mark.</t>
+  </si>
+  <si>
+    <t>A spear coated in poison. Occasionally paralyzes foes.</t>
+  </si>
+  <si>
+    <t>Strikes enemies with a thick log.</t>
+  </si>
+  <si>
+    <t>More powerful than a sword, but less acurrate.</t>
+  </si>
+  <si>
+    <t>A heavy axe. It's rather powerful, although hard to hit with.</t>
+  </si>
+  <si>
+    <t>A danerous skill that faints a foe by massaging their crotch with the soles of her feet.</t>
+  </si>
+  <si>
+    <t>An axe said to fell an opponent in one blow. High crit and power, but terribly inaccurate.</t>
+  </si>
+  <si>
+    <t>Comes with a skill that allows the user to strike twice.</t>
+  </si>
+  <si>
+    <t>A club made from a tree. Kinda cheap.</t>
+  </si>
+  <si>
+    <t>A hammer boasting high power. Has a chance to cut a foe's defence in half.</t>
+  </si>
+  <si>
+    <t>Strikes foes multiple times until dizziness, temporarily stopping movement.</t>
+  </si>
+  <si>
+    <t>A club dotted with spikes. Quite strong.</t>
+  </si>
+  <si>
+    <t>A cheap staff. It's not particualrly expensive.</t>
+  </si>
+  <si>
+    <t>A normal staff of average strength.</t>
+  </si>
+  <si>
+    <t>A high quality staff. It has great strength although it breaks easily.</t>
+  </si>
+  <si>
+    <t>A staff blessed by the goddess. Restores HP every turn when equipped.</t>
+  </si>
+  <si>
+    <t>A staff with a high critical rate.</t>
+  </si>
+  <si>
+    <t>A staff said to ward off sprits.</t>
+  </si>
+  <si>
+    <t>A staff said to offer protection against spirits.</t>
+  </si>
+  <si>
+    <t>A staff said to protect against death. Grants a huge HP boost.</t>
   </si>
 </sst>
 </file>
@@ -22936,16 +23002,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="1" width="22.2109375" customWidth="1"/>
-    <col min="2" max="2" width="68" customWidth="1"/>
+    <col min="2" max="2" width="83.5" customWidth="1"/>
     <col min="3" max="3" width="23.0703125" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
@@ -23502,7 +23568,9 @@
       <c r="C40" s="40" t="s">
         <v>3262</v>
       </c>
-      <c r="D40" s="40"/>
+      <c r="D40" s="40" t="s">
+        <v>3496</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="15">
       <c r="A41" s="40" t="s">
@@ -23514,7 +23582,9 @@
       <c r="C41" s="40" t="s">
         <v>3263</v>
       </c>
-      <c r="D41" s="40"/>
+      <c r="D41" s="40" t="s">
+        <v>3498</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15">
       <c r="A42" s="40" t="s">
@@ -23526,7 +23596,9 @@
       <c r="C42" s="40" t="s">
         <v>3264</v>
       </c>
-      <c r="D42" s="40"/>
+      <c r="D42" s="40" t="s">
+        <v>3499</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15">
       <c r="A43" s="40" t="s">
@@ -23538,7 +23610,9 @@
       <c r="C43" s="40" t="s">
         <v>3265</v>
       </c>
-      <c r="D43" s="40"/>
+      <c r="D43" s="40" t="s">
+        <v>3500</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="15">
       <c r="A44" s="40" t="s">
@@ -23550,7 +23624,9 @@
       <c r="C44" s="40" t="s">
         <v>3266</v>
       </c>
-      <c r="D44" s="40"/>
+      <c r="D44" s="40" t="s">
+        <v>3501</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15">
       <c r="A45" s="40" t="s">
@@ -23562,7 +23638,9 @@
       <c r="C45" s="40" t="s">
         <v>3267</v>
       </c>
-      <c r="D45" s="40"/>
+      <c r="D45" s="40" t="s">
+        <v>3502</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15">
       <c r="A46" s="40" t="s">
@@ -23574,7 +23652,9 @@
       <c r="C46" s="40" t="s">
         <v>3268</v>
       </c>
-      <c r="D46" s="40"/>
+      <c r="D46" s="40" t="s">
+        <v>3503</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15">
       <c r="A47" s="40" t="s">
@@ -23586,7 +23666,9 @@
       <c r="C47" s="40" t="s">
         <v>3269</v>
       </c>
-      <c r="D47" s="40"/>
+      <c r="D47" s="40" t="s">
+        <v>3505</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="15">
       <c r="A48" s="40" t="s">
@@ -23598,7 +23680,9 @@
       <c r="C48" s="40" t="s">
         <v>3270</v>
       </c>
-      <c r="D48" s="40"/>
+      <c r="D48" s="40" t="s">
+        <v>3506</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="15">
       <c r="A49" s="40" t="s">
@@ -23610,7 +23694,9 @@
       <c r="C49" s="40" t="s">
         <v>3271</v>
       </c>
-      <c r="D49" s="40"/>
+      <c r="D49" s="40" t="s">
+        <v>3507</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="15">
       <c r="A50" s="40" t="s">
@@ -23622,7 +23708,9 @@
       <c r="C50" s="40" t="s">
         <v>3272</v>
       </c>
-      <c r="D50" s="40"/>
+      <c r="D50" s="40" t="s">
+        <v>3508</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="15">
       <c r="A51" s="40" t="s">
@@ -23634,7 +23722,9 @@
       <c r="C51" s="40" t="s">
         <v>3273</v>
       </c>
-      <c r="D51" s="40"/>
+      <c r="D51" s="40" t="s">
+        <v>3509</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15">
       <c r="A52" s="40" t="s">
@@ -23646,7 +23736,9 @@
       <c r="C52" s="40" t="s">
         <v>3274</v>
       </c>
-      <c r="D52" s="40"/>
+      <c r="D52" s="40" t="s">
+        <v>3510</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="15">
       <c r="A53" s="40" t="s">
@@ -23658,7 +23750,9 @@
       <c r="C53" s="40" t="s">
         <v>3275</v>
       </c>
-      <c r="D53" s="40"/>
+      <c r="D53" s="40" t="s">
+        <v>3511</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="15">
       <c r="A54" s="40" t="s">
@@ -23670,7 +23764,9 @@
       <c r="C54" s="40" t="s">
         <v>3276</v>
       </c>
-      <c r="D54" s="40"/>
+      <c r="D54" s="40" t="s">
+        <v>3512</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15">
       <c r="A55" s="40" t="s">
@@ -23682,7 +23778,9 @@
       <c r="C55" s="40" t="s">
         <v>3277</v>
       </c>
-      <c r="D55" s="40"/>
+      <c r="D55" s="40" t="s">
+        <v>3513</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15">
       <c r="A56" s="40" t="s">
@@ -23694,7 +23792,9 @@
       <c r="C56" s="40" t="s">
         <v>3278</v>
       </c>
-      <c r="D56" s="40"/>
+      <c r="D56" s="40" t="s">
+        <v>3497</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="15">
       <c r="A57" s="40" t="s">
@@ -23706,7 +23806,9 @@
       <c r="C57" s="40" t="s">
         <v>3279</v>
       </c>
-      <c r="D57" s="40"/>
+      <c r="D57" s="40" t="s">
+        <v>3514</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="15">
       <c r="A58" s="40" t="s">
@@ -23718,7 +23820,9 @@
       <c r="C58" s="40" t="s">
         <v>3280</v>
       </c>
-      <c r="D58" s="40"/>
+      <c r="D58" s="40" t="s">
+        <v>3515</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="15">
       <c r="A59" s="40" t="s">
@@ -23730,7 +23834,9 @@
       <c r="C59" s="40" t="s">
         <v>3281</v>
       </c>
-      <c r="D59" s="40"/>
+      <c r="D59" s="40" t="s">
+        <v>3516</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="15">
       <c r="A60" s="40" t="s">
@@ -23742,7 +23848,9 @@
       <c r="C60" s="40" t="s">
         <v>3282</v>
       </c>
-      <c r="D60" s="40"/>
+      <c r="D60" s="40" t="s">
+        <v>3517</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="15">
       <c r="A61" s="40" t="s">
@@ -23754,7 +23862,9 @@
       <c r="C61" s="40" t="s">
         <v>3283</v>
       </c>
-      <c r="D61" s="40"/>
+      <c r="D61" s="40" t="s">
+        <v>3518</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="15">
       <c r="A62" s="40" t="s">
@@ -24633,7 +24743,7 @@
         <v>3376</v>
       </c>
       <c r="D125" s="40" t="s">
-        <v>3492</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15">
@@ -24647,7 +24757,7 @@
         <v>3341</v>
       </c>
       <c r="D126" s="40" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15">
@@ -24661,7 +24771,7 @@
         <v>3342</v>
       </c>
       <c r="D127" s="40" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15">
@@ -24675,7 +24785,7 @@
         <v>3343</v>
       </c>
       <c r="D128" s="40" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15">
@@ -24689,7 +24799,7 @@
         <v>3344</v>
       </c>
       <c r="D129" s="40" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15">

</xml_diff>

<commit_message>
Ch4 proofreading, and ch5 investigation start
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="names-名前" sheetId="1" r:id="rId1"/>
@@ -10223,9 +10223,6 @@
     <t>The leader of a mercinary group.</t>
   </si>
   <si>
-    <t>Unit becomes love struck and unable to resist seduction.</t>
-  </si>
-  <si>
     <t>HP decreases over 3 turns.</t>
   </si>
   <si>
@@ -10280,9 +10277,6 @@
     <t>Mark of submission to the queen. Serves her to their very limit untill death.</t>
   </si>
   <si>
-    <t>Unit becomes enthralled and vulnerable to pleasure for several turns.</t>
-  </si>
-  <si>
     <t>Serious enthrallment. Unit becomes vulerable and sets Will to 0.</t>
   </si>
   <si>
@@ -10674,6 +10668,12 @@
   </si>
   <si>
     <t>A advanced level breast succubus. All men's reason will melts within her huge soft breasts.</t>
+  </si>
+  <si>
+    <t>Love struck and unable to resist seduction.</t>
+  </si>
+  <si>
+    <t>Enthralled and vulnerable to pleasure for several turns.</t>
   </si>
 </sst>
 </file>
@@ -12506,7 +12506,7 @@
         <v>2305</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>3528</v>
+        <v>3526</v>
       </c>
       <c r="G52" s="23" t="s">
         <v>108</v>
@@ -19780,7 +19780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -23599,7 +23599,7 @@
         <v>3261</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>3494</v>
+        <v>3492</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15">
@@ -23613,7 +23613,7 @@
         <v>3262</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>3496</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15">
@@ -23627,7 +23627,7 @@
         <v>3263</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>3497</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15">
@@ -23641,7 +23641,7 @@
         <v>3264</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>3498</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15">
@@ -23655,7 +23655,7 @@
         <v>3265</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>3499</v>
+        <v>3497</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15">
@@ -23669,7 +23669,7 @@
         <v>3266</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>3500</v>
+        <v>3498</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15">
@@ -23683,7 +23683,7 @@
         <v>3267</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>3501</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15">
@@ -23697,7 +23697,7 @@
         <v>3268</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>3503</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15">
@@ -23711,7 +23711,7 @@
         <v>3269</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>3504</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15">
@@ -23725,7 +23725,7 @@
         <v>3270</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>3505</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15">
@@ -23739,7 +23739,7 @@
         <v>3271</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>3506</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15">
@@ -23753,7 +23753,7 @@
         <v>3272</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>3507</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15">
@@ -23767,7 +23767,7 @@
         <v>3273</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>3508</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15">
@@ -23781,7 +23781,7 @@
         <v>3274</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>3509</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15">
@@ -23795,7 +23795,7 @@
         <v>3275</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>3510</v>
+        <v>3508</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15">
@@ -23809,7 +23809,7 @@
         <v>3276</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>3511</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15">
@@ -23823,7 +23823,7 @@
         <v>3277</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>3495</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15">
@@ -23837,7 +23837,7 @@
         <v>3278</v>
       </c>
       <c r="D57" s="40" t="s">
-        <v>3512</v>
+        <v>3510</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15">
@@ -23851,7 +23851,7 @@
         <v>3279</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>3513</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15">
@@ -23865,7 +23865,7 @@
         <v>3280</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>3514</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15">
@@ -23879,7 +23879,7 @@
         <v>3281</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>3515</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15">
@@ -23893,7 +23893,7 @@
         <v>3282</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>3516</v>
+        <v>3514</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15">
@@ -23907,7 +23907,7 @@
         <v>3283</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>3443</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15">
@@ -23921,7 +23921,7 @@
         <v>3284</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>3444</v>
+        <v>3442</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15">
@@ -23935,7 +23935,7 @@
         <v>3285</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>3442</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15">
@@ -23949,7 +23949,7 @@
         <v>3286</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>3442</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15">
@@ -23963,7 +23963,7 @@
         <v>3287</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>3442</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15">
@@ -23977,7 +23977,7 @@
         <v>3288</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>3445</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15">
@@ -23988,10 +23988,10 @@
         <v>3158</v>
       </c>
       <c r="C68" s="40" t="s">
-        <v>3446</v>
+        <v>3444</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>3447</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15">
@@ -24005,7 +24005,7 @@
         <v>3289</v>
       </c>
       <c r="D69" s="40" t="s">
-        <v>3453</v>
+        <v>3451</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15">
@@ -24019,7 +24019,7 @@
         <v>3290</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>3453</v>
+        <v>3451</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15">
@@ -24033,7 +24033,7 @@
         <v>3291</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>3453</v>
+        <v>3451</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15">
@@ -24047,7 +24047,7 @@
         <v>3292</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>3453</v>
+        <v>3451</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15">
@@ -24061,7 +24061,7 @@
         <v>3293</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>3448</v>
+        <v>3446</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15">
@@ -24075,7 +24075,7 @@
         <v>3294</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>3449</v>
+        <v>3447</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15">
@@ -24089,7 +24089,7 @@
         <v>3306</v>
       </c>
       <c r="D75" s="40" t="s">
-        <v>3450</v>
+        <v>3448</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15">
@@ -24103,7 +24103,7 @@
         <v>3295</v>
       </c>
       <c r="D76" s="40" t="s">
-        <v>3451</v>
+        <v>3449</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15">
@@ -24117,7 +24117,7 @@
         <v>3296</v>
       </c>
       <c r="D77" s="40" t="s">
-        <v>3456</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15">
@@ -24131,7 +24131,7 @@
         <v>3297</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>3456</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15">
@@ -24145,7 +24145,7 @@
         <v>3298</v>
       </c>
       <c r="D79" s="40" t="s">
-        <v>3452</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15">
@@ -24159,7 +24159,7 @@
         <v>3299</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>3452</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15">
@@ -24173,7 +24173,7 @@
         <v>3300</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>3452</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15">
@@ -24187,7 +24187,7 @@
         <v>3301</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>3454</v>
+        <v>3452</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15">
@@ -24201,7 +24201,7 @@
         <v>3376</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>3455</v>
+        <v>3453</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15">
@@ -24213,7 +24213,7 @@
         <v>3302</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>3457</v>
+        <v>3455</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15">
@@ -24225,7 +24225,7 @@
         <v>3303</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>3457</v>
+        <v>3455</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15">
@@ -24237,7 +24237,7 @@
         <v>3304</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>3458</v>
+        <v>3456</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15">
@@ -24249,7 +24249,7 @@
         <v>3305</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>3459</v>
+        <v>3457</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15">
@@ -24263,7 +24263,7 @@
         <v>3307</v>
       </c>
       <c r="D88" s="40" t="s">
-        <v>3461</v>
+        <v>3459</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15">
@@ -24277,7 +24277,7 @@
         <v>3308</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>3460</v>
+        <v>3458</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15">
@@ -24291,7 +24291,7 @@
         <v>3309</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>3462</v>
+        <v>3460</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15">
@@ -24305,7 +24305,7 @@
         <v>3310</v>
       </c>
       <c r="D91" s="40" t="s">
-        <v>3463</v>
+        <v>3461</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15">
@@ -24319,7 +24319,7 @@
         <v>3311</v>
       </c>
       <c r="D92" s="40" t="s">
-        <v>3464</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15">
@@ -24333,7 +24333,7 @@
         <v>3312</v>
       </c>
       <c r="D93" s="40" t="s">
-        <v>3465</v>
+        <v>3463</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15">
@@ -24347,7 +24347,7 @@
         <v>3313</v>
       </c>
       <c r="D94" s="40" t="s">
-        <v>3465</v>
+        <v>3463</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15">
@@ -24359,7 +24359,7 @@
         <v>3314</v>
       </c>
       <c r="D95" s="40" t="s">
-        <v>3466</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15">
@@ -24371,7 +24371,7 @@
         <v>3315</v>
       </c>
       <c r="D96" s="40" t="s">
-        <v>3466</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15">
@@ -24385,7 +24385,7 @@
         <v>3316</v>
       </c>
       <c r="D97" s="40" t="s">
-        <v>3466</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15">
@@ -24397,7 +24397,7 @@
         <v>3317</v>
       </c>
       <c r="D98" s="40" t="s">
-        <v>3467</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15">
@@ -24409,7 +24409,7 @@
         <v>3319</v>
       </c>
       <c r="D99" s="40" t="s">
-        <v>3467</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15">
@@ -24423,7 +24423,7 @@
         <v>3318</v>
       </c>
       <c r="D100" s="40" t="s">
-        <v>3467</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15">
@@ -24437,7 +24437,7 @@
         <v>3320</v>
       </c>
       <c r="D101" s="40" t="s">
-        <v>3468</v>
+        <v>3466</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15">
@@ -24451,7 +24451,7 @@
         <v>3321</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>3469</v>
+        <v>3467</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15">
@@ -24465,7 +24465,7 @@
         <v>3322</v>
       </c>
       <c r="D103" s="40" t="s">
-        <v>3470</v>
+        <v>3468</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15">
@@ -24479,7 +24479,7 @@
         <v>3323</v>
       </c>
       <c r="D104" s="40" t="s">
-        <v>3471</v>
+        <v>3469</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15">
@@ -24493,7 +24493,7 @@
         <v>3324</v>
       </c>
       <c r="D105" s="40" t="s">
-        <v>3472</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15">
@@ -24507,7 +24507,7 @@
         <v>3325</v>
       </c>
       <c r="D106" s="40" t="s">
-        <v>3473</v>
+        <v>3471</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15">
@@ -24521,7 +24521,7 @@
         <v>3326</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>3474</v>
+        <v>3472</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15">
@@ -24535,7 +24535,7 @@
         <v>3373</v>
       </c>
       <c r="D108" s="40" t="s">
-        <v>3474</v>
+        <v>3472</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15">
@@ -24549,7 +24549,7 @@
         <v>3372</v>
       </c>
       <c r="D109" s="40" t="s">
-        <v>3475</v>
+        <v>3473</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15">
@@ -24563,7 +24563,7 @@
         <v>3327</v>
       </c>
       <c r="D110" s="40" t="s">
-        <v>3473</v>
+        <v>3471</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15">
@@ -24577,7 +24577,7 @@
         <v>3328</v>
       </c>
       <c r="D111" s="40" t="s">
-        <v>3476</v>
+        <v>3474</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15">
@@ -24591,7 +24591,7 @@
         <v>3374</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>3477</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15">
@@ -24605,7 +24605,7 @@
         <v>3329</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>3478</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15">
@@ -24619,7 +24619,7 @@
         <v>3330</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>3479</v>
+        <v>3477</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15">
@@ -24633,7 +24633,7 @@
         <v>3331</v>
       </c>
       <c r="D115" s="40" t="s">
-        <v>3480</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15">
@@ -24647,7 +24647,7 @@
         <v>3332</v>
       </c>
       <c r="D116" s="40" t="s">
-        <v>3481</v>
+        <v>3479</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15">
@@ -24661,7 +24661,7 @@
         <v>3344</v>
       </c>
       <c r="D117" s="40" t="s">
-        <v>3482</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15">
@@ -24675,7 +24675,7 @@
         <v>3333</v>
       </c>
       <c r="D118" s="40" t="s">
-        <v>3483</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15">
@@ -24689,7 +24689,7 @@
         <v>3334</v>
       </c>
       <c r="D119" s="40" t="s">
-        <v>3484</v>
+        <v>3482</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15">
@@ -24703,7 +24703,7 @@
         <v>3335</v>
       </c>
       <c r="D120" s="40" t="s">
-        <v>3485</v>
+        <v>3483</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15">
@@ -24717,7 +24717,7 @@
         <v>3336</v>
       </c>
       <c r="D121" s="40" t="s">
-        <v>3486</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15">
@@ -24731,7 +24731,7 @@
         <v>3337</v>
       </c>
       <c r="D122" s="40" t="s">
-        <v>3487</v>
+        <v>3485</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15">
@@ -24745,7 +24745,7 @@
         <v>3338</v>
       </c>
       <c r="D123" s="40" t="s">
-        <v>3488</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15">
@@ -24759,7 +24759,7 @@
         <v>3339</v>
       </c>
       <c r="D124" s="40" t="s">
-        <v>3489</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15">
@@ -24773,7 +24773,7 @@
         <v>3375</v>
       </c>
       <c r="D125" s="40" t="s">
-        <v>3502</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15">
@@ -24787,7 +24787,7 @@
         <v>3340</v>
       </c>
       <c r="D126" s="40" t="s">
-        <v>3490</v>
+        <v>3488</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15">
@@ -24801,7 +24801,7 @@
         <v>3341</v>
       </c>
       <c r="D127" s="40" t="s">
-        <v>3491</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15">
@@ -24815,7 +24815,7 @@
         <v>3342</v>
       </c>
       <c r="D128" s="40" t="s">
-        <v>3492</v>
+        <v>3490</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15">
@@ -24829,7 +24829,7 @@
         <v>3343</v>
       </c>
       <c r="D129" s="40" t="s">
-        <v>3493</v>
+        <v>3491</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15">
@@ -24853,8 +24853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -24891,7 +24891,7 @@
         <v>1926</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>3378</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -24905,7 +24905,7 @@
         <v>1973</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>3379</v>
+        <v>3378</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -24919,7 +24919,7 @@
         <v>1974</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>3380</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -24933,7 +24933,7 @@
         <v>3045</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>3381</v>
+        <v>3380</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -24947,7 +24947,7 @@
         <v>3046</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>3382</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -24961,7 +24961,7 @@
         <v>3047</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>3383</v>
+        <v>3382</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -24975,7 +24975,7 @@
         <v>3065</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>3384</v>
+        <v>3383</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -24989,7 +24989,7 @@
         <v>3048</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>3396</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -25000,10 +25000,10 @@
         <v>2922</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>3387</v>
+        <v>3386</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>3385</v>
+        <v>3384</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -25014,10 +25014,10 @@
         <v>2924</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>3388</v>
+        <v>3387</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>3386</v>
+        <v>3385</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -25031,7 +25031,7 @@
         <v>3070</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>3389</v>
+        <v>3388</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -25045,7 +25045,7 @@
         <v>3069</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>3390</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -25059,7 +25059,7 @@
         <v>3050</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>3391</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -25073,7 +25073,7 @@
         <v>3067</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>3392</v>
+        <v>3391</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -25087,7 +25087,7 @@
         <v>3068</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>3393</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -25101,7 +25101,7 @@
         <v>1944</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>3395</v>
+        <v>3394</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -25115,7 +25115,7 @@
         <v>3066</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>3394</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -25129,7 +25129,7 @@
         <v>3049</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>3397</v>
+        <v>3528</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -25143,7 +25143,7 @@
         <v>3079</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>3398</v>
+        <v>3396</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -25157,7 +25157,7 @@
         <v>3064</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>3399</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -25171,7 +25171,7 @@
         <v>3071</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>3399</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -25185,7 +25185,7 @@
         <v>3080</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>3400</v>
+        <v>3398</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -25199,7 +25199,7 @@
         <v>3081</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>3400</v>
+        <v>3398</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -25210,10 +25210,10 @@
         <v>2948</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>3401</v>
+        <v>3399</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>3402</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -25227,7 +25227,7 @@
         <v>3078</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>3403</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -25241,7 +25241,7 @@
         <v>2042</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>3406</v>
+        <v>3404</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -25255,7 +25255,7 @@
         <v>3074</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>3407</v>
+        <v>3405</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -25269,7 +25269,7 @@
         <v>3075</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>3408</v>
+        <v>3406</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -25280,10 +25280,10 @@
         <v>2958</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>3409</v>
+        <v>3407</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>3410</v>
+        <v>3408</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -25297,7 +25297,7 @@
         <v>2043</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>3404</v>
+        <v>3402</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -25311,7 +25311,7 @@
         <v>3077</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>3411</v>
+        <v>3409</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -25325,7 +25325,7 @@
         <v>2047</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>3413</v>
+        <v>3411</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -25339,7 +25339,7 @@
         <v>3076</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>3412</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -25353,7 +25353,7 @@
         <v>2045</v>
       </c>
       <c r="D35" s="40" t="s">
-        <v>3405</v>
+        <v>3403</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -25367,7 +25367,7 @@
         <v>3073</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>3414</v>
+        <v>3412</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -25381,7 +25381,7 @@
         <v>3072</v>
       </c>
       <c r="D37" s="40" t="s">
-        <v>3415</v>
+        <v>3413</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -25395,7 +25395,7 @@
         <v>3082</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>3416</v>
+        <v>3414</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -25406,10 +25406,10 @@
         <v>2976</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>3417</v>
+        <v>3415</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>3418</v>
+        <v>3416</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -25423,7 +25423,7 @@
         <v>3083</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>3419</v>
+        <v>3417</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -25437,7 +25437,7 @@
         <v>3084</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>3420</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -25451,7 +25451,7 @@
         <v>3085</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>3421</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -25465,7 +25465,7 @@
         <v>3086</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>3422</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -25479,7 +25479,7 @@
         <v>3087</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>3423</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -25493,7 +25493,7 @@
         <v>3088</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>3424</v>
+        <v>3422</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -25507,7 +25507,7 @@
         <v>3089</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>3425</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -25521,7 +25521,7 @@
         <v>3090</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>3426</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -25535,7 +25535,7 @@
         <v>3091</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>3427</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -25549,7 +25549,7 @@
         <v>3092</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>3428</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -25557,10 +25557,10 @@
         <v>168</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>3522</v>
+        <v>3520</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>3517</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -25571,7 +25571,7 @@
         <v>3051</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>3519</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -25582,7 +25582,7 @@
         <v>3052</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>3520</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -25593,7 +25593,7 @@
         <v>3053</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>3521</v>
+        <v>3519</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -25604,7 +25604,7 @@
         <v>3054</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>3523</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -25615,7 +25615,7 @@
         <v>3055</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>3524</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -25626,7 +25626,7 @@
         <v>3056</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>3525</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -25640,7 +25640,7 @@
         <v>3057</v>
       </c>
       <c r="D57" s="40" t="s">
-        <v>3518</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -25654,7 +25654,7 @@
         <v>3093</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>3429</v>
+        <v>3427</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -25668,7 +25668,7 @@
         <v>3058</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>3430</v>
+        <v>3428</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -25682,7 +25682,7 @@
         <v>3094</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>3431</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -25696,7 +25696,7 @@
         <v>3095</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>3431</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -25710,7 +25710,7 @@
         <v>3096</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>3432</v>
+        <v>3430</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -25724,7 +25724,7 @@
         <v>3097</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>3433</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -25738,7 +25738,7 @@
         <v>3098</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>3433</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -25752,7 +25752,7 @@
         <v>3099</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>3433</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -25766,7 +25766,7 @@
         <v>3100</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>3434</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -25780,7 +25780,7 @@
         <v>3101</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>3435</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -25794,7 +25794,7 @@
         <v>3102</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>3436</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -25808,10 +25808,10 @@
         <v>3103</v>
       </c>
       <c r="D69" s="40" t="s">
-        <v>3438</v>
+        <v>3436</v>
       </c>
       <c r="E69" s="40" t="s">
-        <v>3437</v>
+        <v>3435</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -25822,7 +25822,7 @@
         <v>3059</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>3526</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -25833,7 +25833,7 @@
         <v>3060</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>3527</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -25847,7 +25847,7 @@
         <v>3061</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>3439</v>
+        <v>3437</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -25861,7 +25861,7 @@
         <v>3062</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>3440</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -25875,7 +25875,7 @@
         <v>3063</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>3441</v>
+        <v>3439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Goodness Mizuhide has a lot of exposition dialogue
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="names-名前" sheetId="1" r:id="rId1"/>
@@ -24853,7 +24853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -26149,8 +26149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>

</xml_diff>

<commit_message>
Big updates for ch5
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="names-名前" sheetId="1" r:id="rId1"/>
@@ -9224,9 +9224,6 @@
     <t>Paralysis</t>
   </si>
   <si>
-    <t>Betrayal</t>
-  </si>
-  <si>
     <t>Queen's Slave</t>
   </si>
   <si>
@@ -9278,9 +9275,6 @@
     <t>Masturbation Frenzy</t>
   </si>
   <si>
-    <t>Betrayal+</t>
-  </si>
-  <si>
     <t>Accelerate</t>
   </si>
   <si>
@@ -10526,12 +10520,6 @@
     <t>Drains a foe's strength by rubbing their face against the queen's breasts.</t>
   </si>
   <si>
-    <t>Skillfully melts a man with unrivaled handjob techniques.</t>
-  </si>
-  <si>
-    <t>Melts a man into mindlessness with the caress of her mouth.</t>
-  </si>
-  <si>
     <t>Pleasures men by rubbing her smooth feet around their penis.</t>
   </si>
   <si>
@@ -10550,9 +10538,6 @@
     <t>An irresistable paizuri that drains men of the will to fight.</t>
   </si>
   <si>
-    <t>A sigh filled with pheromones that inflicts 2 or more abnormal states.</t>
-  </si>
-  <si>
     <t>A spear made by woodland sprites. It quietens the user's mind and movements.</t>
   </si>
   <si>
@@ -10752,6 +10737,21 @@
   </si>
   <si>
     <t>A advanced level breast succubus. All men's reason will melt within her huge soft breasts.</t>
+  </si>
+  <si>
+    <t>Treachery</t>
+  </si>
+  <si>
+    <t>Treachery+</t>
+  </si>
+  <si>
+    <t>A pheromone filled sigh that inflicts 2 or more abnormal states.</t>
+  </si>
+  <si>
+    <t>A caressing mouth that melts a man into mindlessness.</t>
+  </si>
+  <si>
+    <t>An unrivaled handjob technique that skillfully melts any man.</t>
   </si>
 </sst>
 </file>
@@ -11481,7 +11481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
@@ -11739,7 +11739,7 @@
         <v>2264</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>3368</v>
+        <v>3366</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>32</v>
@@ -11761,7 +11761,7 @@
         <v>2265</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>3367</v>
+        <v>3365</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>34</v>
@@ -11783,7 +11783,7 @@
         <v>2266</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>3369</v>
+        <v>3367</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>36</v>
@@ -12368,7 +12368,7 @@
         <v>2284</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>3553</v>
+        <v>3548</v>
       </c>
       <c r="G43" s="36" t="s">
         <v>89</v>
@@ -12437,7 +12437,7 @@
         <v>2227</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>3524</v>
+        <v>3519</v>
       </c>
       <c r="F46" s="23" t="s">
         <v>2649</v>
@@ -12560,7 +12560,7 @@
         <v>2300</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>3366</v>
+        <v>3364</v>
       </c>
       <c r="G51" s="23" t="s">
         <v>105</v>
@@ -12584,7 +12584,7 @@
         <v>2304</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>3554</v>
+        <v>3549</v>
       </c>
       <c r="G52" s="23" t="s">
         <v>108</v>
@@ -19858,7 +19858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -19895,7 +19895,7 @@
         <v>3037</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>3528</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15">
@@ -19909,7 +19909,7 @@
         <v>2318</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>3526</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15">
@@ -19923,7 +19923,7 @@
         <v>3036</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>3527</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15">
@@ -19951,7 +19951,7 @@
         <v>3038</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>3529</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15">
@@ -19965,7 +19965,7 @@
         <v>2319</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>3530</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15">
@@ -19979,7 +19979,7 @@
         <v>3039</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>3531</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15">
@@ -19993,7 +19993,7 @@
         <v>2805</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>3532</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15">
@@ -20007,7 +20007,7 @@
         <v>3040</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>3532</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15">
@@ -20021,7 +20021,7 @@
         <v>2320</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>3535</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15">
@@ -20035,7 +20035,7 @@
         <v>3042</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15">
@@ -20049,7 +20049,7 @@
         <v>3041</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>3534</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15">
@@ -20090,10 +20090,10 @@
         <v>2864</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>3360</v>
+        <v>3358</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>3536</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15">
@@ -20104,10 +20104,10 @@
         <v>2866</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>3361</v>
+        <v>3359</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>3537</v>
+        <v>3532</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15">
@@ -20118,10 +20118,10 @@
         <v>2868</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>3363</v>
+        <v>3361</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>3538</v>
+        <v>3533</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15">
@@ -20132,10 +20132,10 @@
         <v>2870</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>3362</v>
+        <v>3360</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>3539</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15">
@@ -20146,10 +20146,10 @@
         <v>2872</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>3364</v>
+        <v>3362</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>3540</v>
+        <v>3535</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15">
@@ -20163,7 +20163,7 @@
         <v>2039</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>3541</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15">
@@ -20174,10 +20174,10 @@
         <v>2874</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>3365</v>
+        <v>3363</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>3541</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15">
@@ -20188,10 +20188,10 @@
         <v>2877</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>3343</v>
+        <v>3341</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>3542</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15">
@@ -20205,7 +20205,7 @@
         <v>2036</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>3542</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15">
@@ -20216,10 +20216,10 @@
         <v>2877</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>3344</v>
+        <v>3342</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>3542</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15">
@@ -20230,10 +20230,10 @@
         <v>2881</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>3345</v>
+        <v>3343</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>3543</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15">
@@ -20244,10 +20244,10 @@
         <v>2881</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>3346</v>
+        <v>3344</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>3543</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15">
@@ -20258,10 +20258,10 @@
         <v>2881</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>3347</v>
+        <v>3345</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>3543</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15">
@@ -20272,10 +20272,10 @@
         <v>2885</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>3348</v>
+        <v>3346</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>3544</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15">
@@ -20286,10 +20286,10 @@
         <v>2885</v>
       </c>
       <c r="C31" s="40" t="s">
-        <v>3349</v>
+        <v>3347</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>3544</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15">
@@ -20300,10 +20300,10 @@
         <v>2885</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>3350</v>
+        <v>3348</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>3544</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15">
@@ -20314,10 +20314,10 @@
         <v>2888</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>3351</v>
+        <v>3349</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>3545</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15">
@@ -20331,7 +20331,7 @@
         <v>2270</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>3546</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15">
@@ -20345,7 +20345,7 @@
         <v>2035</v>
       </c>
       <c r="D35" s="40" t="s">
-        <v>3547</v>
+        <v>3542</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15">
@@ -20356,10 +20356,10 @@
         <v>2893</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>3352</v>
+        <v>3350</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>3548</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15">
@@ -20373,7 +20373,7 @@
         <v>2038</v>
       </c>
       <c r="D37" s="40" t="s">
-        <v>3549</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15">
@@ -20384,10 +20384,10 @@
         <v>2896</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>3353</v>
+        <v>3351</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>3550</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15">
@@ -20401,7 +20401,7 @@
         <v>2271</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>3551</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15">
@@ -20412,10 +20412,10 @@
         <v>2897</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>3354</v>
+        <v>3352</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>3551</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15">
@@ -20426,10 +20426,10 @@
         <v>2899</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>3355</v>
+        <v>3353</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>3552</v>
+        <v>3547</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15">
@@ -20440,10 +20440,10 @@
         <v>2899</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>3552</v>
+        <v>3547</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15">
@@ -20460,7 +20460,7 @@
       </c>
       <c r="B44" s="40"/>
       <c r="C44" s="40" t="s">
-        <v>3357</v>
+        <v>3355</v>
       </c>
       <c r="D44" s="40"/>
     </row>
@@ -20470,7 +20470,7 @@
       </c>
       <c r="B45" s="40"/>
       <c r="C45" s="40" t="s">
-        <v>3358</v>
+        <v>3356</v>
       </c>
       <c r="D45" s="40"/>
     </row>
@@ -20480,7 +20480,7 @@
       </c>
       <c r="B46" s="40"/>
       <c r="C46" s="40" t="s">
-        <v>3359</v>
+        <v>3357</v>
       </c>
       <c r="D46" s="40"/>
     </row>
@@ -20494,7 +20494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G143"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
@@ -23182,8 +23182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15"/>
@@ -23740,1022 +23740,1022 @@
     </row>
     <row r="40" spans="1:4" ht="15">
       <c r="A40" s="40" t="s">
-        <v>3102</v>
+        <v>3100</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>3103</v>
+        <v>3101</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>3259</v>
+        <v>3257</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>3488</v>
+        <v>3483</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15">
       <c r="A41" s="40" t="s">
-        <v>3104</v>
+        <v>3102</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>3105</v>
+        <v>3103</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>3260</v>
+        <v>3258</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>3490</v>
+        <v>3485</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15">
       <c r="A42" s="40" t="s">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>3261</v>
+        <v>3259</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>3491</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15">
       <c r="A43" s="40" t="s">
-        <v>3108</v>
+        <v>3106</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>3109</v>
+        <v>3107</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>3262</v>
+        <v>3260</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>3492</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15">
       <c r="A44" s="40" t="s">
-        <v>3110</v>
+        <v>3108</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>3111</v>
+        <v>3109</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>3263</v>
+        <v>3261</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>3493</v>
+        <v>3488</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15">
       <c r="A45" s="40" t="s">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>3264</v>
+        <v>3262</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>3494</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15">
       <c r="A46" s="40" t="s">
-        <v>3114</v>
+        <v>3112</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>3115</v>
+        <v>3113</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>3265</v>
+        <v>3263</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>3495</v>
+        <v>3490</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15">
       <c r="A47" s="40" t="s">
-        <v>3116</v>
+        <v>3114</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>3117</v>
+        <v>3115</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>3266</v>
+        <v>3264</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>3497</v>
+        <v>3492</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15">
       <c r="A48" s="40" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
       <c r="B48" s="40" t="s">
         <v>1727</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>3267</v>
+        <v>3265</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>3498</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15">
       <c r="A49" s="40" t="s">
-        <v>3119</v>
+        <v>3117</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>3120</v>
+        <v>3118</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>3268</v>
+        <v>3266</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>3499</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15">
       <c r="A50" s="40" t="s">
-        <v>3121</v>
+        <v>3119</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>3122</v>
+        <v>3120</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>3269</v>
+        <v>3267</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>3500</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15">
       <c r="A51" s="40" t="s">
-        <v>3123</v>
+        <v>3121</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>3124</v>
+        <v>3122</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>3270</v>
+        <v>3268</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>3501</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15">
       <c r="A52" s="40" t="s">
-        <v>3125</v>
+        <v>3123</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>3126</v>
+        <v>3124</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>3271</v>
+        <v>3269</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>3502</v>
+        <v>3497</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15">
       <c r="A53" s="40" t="s">
-        <v>3127</v>
+        <v>3125</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>3128</v>
+        <v>3126</v>
       </c>
       <c r="C53" s="40" t="s">
-        <v>3272</v>
+        <v>3270</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>3503</v>
+        <v>3498</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15">
       <c r="A54" s="40" t="s">
-        <v>3129</v>
+        <v>3127</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>3130</v>
+        <v>3128</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>3273</v>
+        <v>3271</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>3504</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15">
       <c r="A55" s="40" t="s">
-        <v>3131</v>
+        <v>3129</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>3132</v>
+        <v>3130</v>
       </c>
       <c r="C55" s="40" t="s">
-        <v>3274</v>
+        <v>3272</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>3505</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15">
       <c r="A56" s="40" t="s">
-        <v>3133</v>
+        <v>3131</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>3134</v>
+        <v>3132</v>
       </c>
       <c r="C56" s="40" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>3489</v>
+        <v>3484</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15">
       <c r="A57" s="40" t="s">
-        <v>3135</v>
+        <v>3133</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>3136</v>
+        <v>3134</v>
       </c>
       <c r="C57" s="40" t="s">
-        <v>3276</v>
+        <v>3274</v>
       </c>
       <c r="D57" s="40" t="s">
-        <v>3506</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15">
       <c r="A58" s="40" t="s">
-        <v>3137</v>
+        <v>3135</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>3138</v>
+        <v>3136</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>3277</v>
+        <v>3275</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>3507</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15">
       <c r="A59" s="40" t="s">
-        <v>3139</v>
+        <v>3137</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>3140</v>
+        <v>3138</v>
       </c>
       <c r="C59" s="40" t="s">
-        <v>3278</v>
+        <v>3276</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>3508</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15">
       <c r="A60" s="40" t="s">
-        <v>3141</v>
+        <v>3139</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>3142</v>
+        <v>3140</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>3279</v>
+        <v>3277</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>3509</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15">
       <c r="A61" s="40" t="s">
-        <v>3143</v>
+        <v>3141</v>
       </c>
       <c r="B61" s="40" t="s">
-        <v>3144</v>
+        <v>3142</v>
       </c>
       <c r="C61" s="40" t="s">
-        <v>3280</v>
+        <v>3278</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>3510</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15">
       <c r="A62" s="40" t="s">
-        <v>3145</v>
+        <v>3143</v>
       </c>
       <c r="B62" s="40" t="s">
-        <v>3146</v>
+        <v>3144</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>3281</v>
+        <v>3279</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>3438</v>
+        <v>3436</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15">
       <c r="A63" s="40" t="s">
-        <v>3147</v>
+        <v>3145</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>3148</v>
+        <v>3146</v>
       </c>
       <c r="C63" s="40" t="s">
-        <v>3282</v>
+        <v>3280</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>3439</v>
+        <v>3437</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15">
       <c r="A64" s="40" t="s">
-        <v>3149</v>
+        <v>3147</v>
       </c>
       <c r="B64" s="40" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="C64" s="40" t="s">
-        <v>3283</v>
+        <v>3281</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>3437</v>
+        <v>3435</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15">
       <c r="A65" s="40" t="s">
-        <v>3151</v>
+        <v>3149</v>
       </c>
       <c r="B65" s="40" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="C65" s="40" t="s">
-        <v>3284</v>
+        <v>3282</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>3437</v>
+        <v>3435</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15">
       <c r="A66" s="40" t="s">
-        <v>3152</v>
+        <v>3150</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>3285</v>
+        <v>3283</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>3437</v>
+        <v>3435</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15">
       <c r="A67" s="40" t="s">
-        <v>3153</v>
+        <v>3151</v>
       </c>
       <c r="B67" s="40" t="s">
-        <v>3154</v>
+        <v>3152</v>
       </c>
       <c r="C67" s="40" t="s">
-        <v>3286</v>
+        <v>3284</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>3440</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15">
       <c r="A68" s="40" t="s">
-        <v>3155</v>
+        <v>3153</v>
       </c>
       <c r="B68" s="40" t="s">
-        <v>3156</v>
+        <v>3154</v>
       </c>
       <c r="C68" s="40" t="s">
-        <v>3441</v>
+        <v>3439</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>3442</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15">
       <c r="A69" s="40" t="s">
-        <v>3157</v>
+        <v>3155</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="C69" s="40" t="s">
-        <v>3287</v>
+        <v>3285</v>
       </c>
       <c r="D69" s="40" t="s">
-        <v>3447</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15">
       <c r="A70" s="40" t="s">
-        <v>3158</v>
+        <v>3156</v>
       </c>
       <c r="B70" s="40" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="C70" s="40" t="s">
-        <v>3288</v>
+        <v>3286</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>3447</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15">
       <c r="A71" s="40" t="s">
-        <v>3159</v>
+        <v>3157</v>
       </c>
       <c r="B71" s="40" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="C71" s="40" t="s">
-        <v>3289</v>
+        <v>3287</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>3447</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15">
       <c r="A72" s="40" t="s">
-        <v>3160</v>
+        <v>3158</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>3150</v>
+        <v>3148</v>
       </c>
       <c r="C72" s="40" t="s">
-        <v>3290</v>
+        <v>3288</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>3447</v>
+        <v>3445</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15">
       <c r="A73" s="40" t="s">
-        <v>3161</v>
+        <v>3159</v>
       </c>
       <c r="B73" s="40" t="s">
-        <v>3162</v>
+        <v>3160</v>
       </c>
       <c r="C73" s="40" t="s">
-        <v>3291</v>
+        <v>3289</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>3443</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15">
       <c r="A74" s="40" t="s">
-        <v>3163</v>
+        <v>3161</v>
       </c>
       <c r="B74" s="40" t="s">
-        <v>3164</v>
+        <v>3162</v>
       </c>
       <c r="C74" s="40" t="s">
-        <v>3292</v>
+        <v>3290</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>3525</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15">
       <c r="A75" s="40" t="s">
-        <v>3165</v>
+        <v>3163</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>3166</v>
+        <v>3164</v>
       </c>
       <c r="C75" s="40" t="s">
-        <v>3304</v>
+        <v>3302</v>
       </c>
       <c r="D75" s="40" t="s">
-        <v>3444</v>
+        <v>3442</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15">
       <c r="A76" s="40" t="s">
-        <v>3167</v>
+        <v>3165</v>
       </c>
       <c r="B76" s="40" t="s">
-        <v>3168</v>
+        <v>3166</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>3293</v>
+        <v>3291</v>
       </c>
       <c r="D76" s="40" t="s">
-        <v>3445</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15">
       <c r="A77" s="40" t="s">
-        <v>3169</v>
+        <v>3167</v>
       </c>
       <c r="B77" s="40" t="s">
-        <v>3170</v>
+        <v>3168</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>3294</v>
+        <v>3292</v>
       </c>
       <c r="D77" s="40" t="s">
-        <v>3450</v>
+        <v>3448</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15">
       <c r="A78" s="40" t="s">
-        <v>3171</v>
+        <v>3169</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>3170</v>
+        <v>3168</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>3295</v>
+        <v>3293</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>3450</v>
+        <v>3448</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15">
       <c r="A79" s="40" t="s">
-        <v>3172</v>
+        <v>3170</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>3170</v>
+        <v>3168</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>3296</v>
+        <v>3294</v>
       </c>
       <c r="D79" s="40" t="s">
-        <v>3446</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15">
       <c r="A80" s="40" t="s">
-        <v>3173</v>
+        <v>3171</v>
       </c>
       <c r="B80" s="40" t="s">
-        <v>3170</v>
+        <v>3168</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>3446</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15">
       <c r="A81" s="40" t="s">
-        <v>3174</v>
+        <v>3172</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>3170</v>
+        <v>3168</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>3298</v>
+        <v>3296</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>3446</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15">
       <c r="A82" s="40" t="s">
-        <v>3175</v>
+        <v>3173</v>
       </c>
       <c r="B82" s="40" t="s">
-        <v>3176</v>
+        <v>3174</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>3299</v>
+        <v>3297</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>3448</v>
+        <v>3446</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15">
       <c r="A83" s="40" t="s">
-        <v>3177</v>
+        <v>3175</v>
       </c>
       <c r="B83" s="40" t="s">
-        <v>3178</v>
+        <v>3176</v>
       </c>
       <c r="C83" s="40" t="s">
-        <v>3374</v>
+        <v>3372</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>3449</v>
+        <v>3447</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15">
       <c r="A84" s="40" t="s">
-        <v>3179</v>
+        <v>3177</v>
       </c>
       <c r="B84" s="40"/>
       <c r="C84" s="40" t="s">
-        <v>3300</v>
+        <v>3298</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>3451</v>
+        <v>3449</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15">
       <c r="A85" s="40" t="s">
-        <v>3180</v>
+        <v>3178</v>
       </c>
       <c r="B85" s="40"/>
       <c r="C85" s="40" t="s">
-        <v>3301</v>
+        <v>3299</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>3451</v>
+        <v>3449</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15">
       <c r="A86" s="40" t="s">
-        <v>3181</v>
+        <v>3179</v>
       </c>
       <c r="B86" s="40"/>
       <c r="C86" s="40" t="s">
-        <v>3302</v>
+        <v>3300</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>3452</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15">
       <c r="A87" s="40" t="s">
-        <v>3182</v>
+        <v>3180</v>
       </c>
       <c r="B87" s="40"/>
       <c r="C87" s="40" t="s">
-        <v>3303</v>
+        <v>3301</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>3453</v>
+        <v>3451</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15">
       <c r="A88" s="40" t="s">
-        <v>3183</v>
+        <v>3181</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>3184</v>
+        <v>3182</v>
       </c>
       <c r="C88" s="40" t="s">
-        <v>3305</v>
+        <v>3303</v>
       </c>
       <c r="D88" s="40" t="s">
-        <v>3455</v>
+        <v>3453</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15">
       <c r="A89" s="40" t="s">
-        <v>3185</v>
+        <v>3183</v>
       </c>
       <c r="B89" s="40" t="s">
-        <v>3184</v>
+        <v>3182</v>
       </c>
       <c r="C89" s="40" t="s">
-        <v>3306</v>
+        <v>3304</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>3454</v>
+        <v>3452</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15">
       <c r="A90" s="40" t="s">
-        <v>3186</v>
+        <v>3184</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>3187</v>
+        <v>3185</v>
       </c>
       <c r="C90" s="40" t="s">
-        <v>3307</v>
+        <v>3305</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>3456</v>
+        <v>3454</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15">
       <c r="A91" s="40" t="s">
-        <v>3188</v>
+        <v>3186</v>
       </c>
       <c r="B91" s="40" t="s">
-        <v>3189</v>
+        <v>3187</v>
       </c>
       <c r="C91" s="40" t="s">
-        <v>3308</v>
+        <v>3306</v>
       </c>
       <c r="D91" s="40" t="s">
-        <v>3457</v>
+        <v>3455</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15">
       <c r="A92" s="40" t="s">
-        <v>3190</v>
+        <v>3188</v>
       </c>
       <c r="B92" s="40" t="s">
-        <v>3191</v>
+        <v>3189</v>
       </c>
       <c r="C92" s="40" t="s">
-        <v>3309</v>
+        <v>3307</v>
       </c>
       <c r="D92" s="40" t="s">
-        <v>3458</v>
+        <v>3456</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15">
       <c r="A93" s="40" t="s">
-        <v>3192</v>
+        <v>3190</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>3193</v>
+        <v>3191</v>
       </c>
       <c r="C93" s="40" t="s">
-        <v>3310</v>
+        <v>3308</v>
       </c>
       <c r="D93" s="40" t="s">
-        <v>3459</v>
+        <v>3457</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15">
       <c r="A94" s="40" t="s">
-        <v>3194</v>
+        <v>3192</v>
       </c>
       <c r="B94" s="40" t="s">
-        <v>3195</v>
+        <v>3193</v>
       </c>
       <c r="C94" s="40" t="s">
-        <v>3311</v>
+        <v>3309</v>
       </c>
       <c r="D94" s="40" t="s">
-        <v>3459</v>
+        <v>3457</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15">
       <c r="A95" s="40" t="s">
-        <v>3196</v>
+        <v>3194</v>
       </c>
       <c r="B95" s="40"/>
       <c r="C95" s="40" t="s">
-        <v>3312</v>
+        <v>3310</v>
       </c>
       <c r="D95" s="40" t="s">
-        <v>3460</v>
+        <v>3458</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15">
       <c r="A96" s="40" t="s">
-        <v>3197</v>
+        <v>3195</v>
       </c>
       <c r="B96" s="40"/>
       <c r="C96" s="40" t="s">
-        <v>3313</v>
+        <v>3311</v>
       </c>
       <c r="D96" s="40" t="s">
-        <v>3460</v>
+        <v>3458</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15">
       <c r="A97" s="40" t="s">
-        <v>3198</v>
+        <v>3196</v>
       </c>
       <c r="B97" s="40" t="s">
-        <v>3199</v>
+        <v>3197</v>
       </c>
       <c r="C97" s="40" t="s">
-        <v>3314</v>
+        <v>3312</v>
       </c>
       <c r="D97" s="40" t="s">
-        <v>3460</v>
+        <v>3458</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15">
       <c r="A98" s="40" t="s">
-        <v>3200</v>
+        <v>3198</v>
       </c>
       <c r="B98" s="40"/>
       <c r="C98" s="40" t="s">
-        <v>3315</v>
+        <v>3313</v>
       </c>
       <c r="D98" s="40" t="s">
-        <v>3461</v>
+        <v>3459</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15">
       <c r="A99" s="40" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
       <c r="B99" s="40"/>
       <c r="C99" s="40" t="s">
-        <v>3317</v>
+        <v>3315</v>
       </c>
       <c r="D99" s="40" t="s">
-        <v>3461</v>
+        <v>3459</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15">
       <c r="A100" s="40" t="s">
-        <v>3202</v>
+        <v>3200</v>
       </c>
       <c r="B100" s="40" t="s">
-        <v>3203</v>
+        <v>3201</v>
       </c>
       <c r="C100" s="40" t="s">
-        <v>3316</v>
+        <v>3314</v>
       </c>
       <c r="D100" s="40" t="s">
-        <v>3461</v>
+        <v>3459</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15">
       <c r="A101" s="40" t="s">
-        <v>3204</v>
+        <v>3202</v>
       </c>
       <c r="B101" s="40" t="s">
-        <v>3205</v>
+        <v>3203</v>
       </c>
       <c r="C101" s="40" t="s">
-        <v>3318</v>
+        <v>3316</v>
       </c>
       <c r="D101" s="40" t="s">
-        <v>3462</v>
+        <v>3460</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15">
       <c r="A102" s="40" t="s">
-        <v>3206</v>
+        <v>3204</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>3199</v>
+        <v>3197</v>
       </c>
       <c r="C102" s="40" t="s">
-        <v>3319</v>
+        <v>3317</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>3463</v>
+        <v>3461</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15">
       <c r="A103" s="40" t="s">
-        <v>3207</v>
+        <v>3205</v>
       </c>
       <c r="B103" s="40" t="s">
-        <v>3208</v>
+        <v>3206</v>
       </c>
       <c r="C103" s="40" t="s">
-        <v>3320</v>
+        <v>3318</v>
       </c>
       <c r="D103" s="40" t="s">
-        <v>3464</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15">
       <c r="A104" s="40" t="s">
-        <v>3209</v>
+        <v>3207</v>
       </c>
       <c r="B104" s="40" t="s">
-        <v>3210</v>
+        <v>3208</v>
       </c>
       <c r="C104" s="40" t="s">
-        <v>3321</v>
+        <v>3319</v>
       </c>
       <c r="D104" s="40" t="s">
-        <v>3465</v>
+        <v>3463</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15">
       <c r="A105" s="40" t="s">
-        <v>3211</v>
+        <v>3209</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="C105" s="40" t="s">
-        <v>3322</v>
+        <v>3320</v>
       </c>
       <c r="D105" s="40" t="s">
-        <v>3466</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15">
       <c r="A106" s="40" t="s">
-        <v>3213</v>
+        <v>3211</v>
       </c>
       <c r="B106" s="40" t="s">
-        <v>3214</v>
+        <v>3212</v>
       </c>
       <c r="C106" s="40" t="s">
-        <v>3323</v>
+        <v>3321</v>
       </c>
       <c r="D106" s="40" t="s">
-        <v>3467</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15">
       <c r="A107" s="40" t="s">
-        <v>3215</v>
+        <v>3213</v>
       </c>
       <c r="B107" s="40" t="s">
-        <v>3216</v>
+        <v>3214</v>
       </c>
       <c r="C107" s="40" t="s">
-        <v>3324</v>
+        <v>3322</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>3468</v>
+        <v>3466</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15">
       <c r="A108" s="40" t="s">
-        <v>3217</v>
+        <v>3215</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>3216</v>
+        <v>3214</v>
       </c>
       <c r="C108" s="40" t="s">
-        <v>3371</v>
+        <v>3369</v>
       </c>
       <c r="D108" s="40" t="s">
-        <v>3468</v>
+        <v>3466</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15">
       <c r="A109" s="40" t="s">
-        <v>3218</v>
+        <v>3216</v>
       </c>
       <c r="B109" s="40" t="s">
-        <v>3219</v>
+        <v>3217</v>
       </c>
       <c r="C109" s="40" t="s">
-        <v>3370</v>
+        <v>3368</v>
       </c>
       <c r="D109" s="40" t="s">
-        <v>3469</v>
+        <v>3467</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15">
       <c r="A110" s="40" t="s">
-        <v>3220</v>
+        <v>3218</v>
       </c>
       <c r="B110" s="40" t="s">
-        <v>3221</v>
+        <v>3219</v>
       </c>
       <c r="C110" s="40" t="s">
-        <v>3325</v>
+        <v>3323</v>
       </c>
       <c r="D110" s="40" t="s">
-        <v>3467</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15">
       <c r="A111" s="40" t="s">
-        <v>3222</v>
+        <v>3220</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>3223</v>
+        <v>3221</v>
       </c>
       <c r="C111" s="40" t="s">
-        <v>3326</v>
+        <v>3324</v>
       </c>
       <c r="D111" s="40" t="s">
-        <v>3470</v>
+        <v>3468</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15">
       <c r="A112" s="40" t="s">
-        <v>3224</v>
+        <v>3222</v>
       </c>
       <c r="B112" s="40" t="s">
-        <v>3225</v>
+        <v>3223</v>
       </c>
       <c r="C112" s="40" t="s">
-        <v>3372</v>
+        <v>3370</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>3471</v>
+        <v>3469</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15">
       <c r="A113" s="40" t="s">
-        <v>3226</v>
+        <v>3224</v>
       </c>
       <c r="B113" s="40" t="s">
-        <v>3227</v>
+        <v>3225</v>
       </c>
       <c r="C113" s="40" t="s">
-        <v>3327</v>
+        <v>3325</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>3472</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15">
@@ -24763,223 +24763,223 @@
         <v>810</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>3228</v>
+        <v>3226</v>
       </c>
       <c r="C114" s="40" t="s">
-        <v>3328</v>
+        <v>3326</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>3473</v>
+        <v>3471</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15">
       <c r="A115" s="40" t="s">
-        <v>3229</v>
+        <v>3227</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>3230</v>
+        <v>3228</v>
       </c>
       <c r="C115" s="40" t="s">
-        <v>3329</v>
+        <v>3327</v>
       </c>
       <c r="D115" s="40" t="s">
-        <v>3474</v>
+        <v>3472</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15">
       <c r="A116" s="40" t="s">
-        <v>3231</v>
+        <v>3229</v>
       </c>
       <c r="B116" s="40" t="s">
-        <v>3232</v>
+        <v>3230</v>
       </c>
       <c r="C116" s="40" t="s">
-        <v>3330</v>
+        <v>3328</v>
       </c>
       <c r="D116" s="40" t="s">
-        <v>3475</v>
+        <v>3473</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15">
       <c r="A117" s="40" t="s">
-        <v>3233</v>
+        <v>3231</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>3234</v>
+        <v>3232</v>
       </c>
       <c r="C117" s="40" t="s">
-        <v>3342</v>
+        <v>3340</v>
       </c>
       <c r="D117" s="40" t="s">
-        <v>3476</v>
+        <v>3474</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15">
       <c r="A118" s="40" t="s">
-        <v>3235</v>
+        <v>3233</v>
       </c>
       <c r="B118" s="40" t="s">
-        <v>3236</v>
+        <v>3234</v>
       </c>
       <c r="C118" s="40" t="s">
-        <v>3331</v>
+        <v>3329</v>
       </c>
       <c r="D118" s="40" t="s">
-        <v>3477</v>
+        <v>3475</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15">
       <c r="A119" s="40" t="s">
-        <v>3237</v>
+        <v>3235</v>
       </c>
       <c r="B119" s="40" t="s">
-        <v>3238</v>
+        <v>3236</v>
       </c>
       <c r="C119" s="40" t="s">
-        <v>3332</v>
+        <v>3330</v>
       </c>
       <c r="D119" s="40" t="s">
-        <v>3478</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15">
       <c r="A120" s="40" t="s">
-        <v>3239</v>
+        <v>3237</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>3240</v>
+        <v>3238</v>
       </c>
       <c r="C120" s="40" t="s">
-        <v>3333</v>
+        <v>3331</v>
       </c>
       <c r="D120" s="40" t="s">
-        <v>3479</v>
+        <v>3554</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15">
       <c r="A121" s="40" t="s">
-        <v>3241</v>
+        <v>3239</v>
       </c>
       <c r="B121" s="40" t="s">
-        <v>3242</v>
+        <v>3240</v>
       </c>
       <c r="C121" s="40" t="s">
-        <v>3334</v>
+        <v>3332</v>
       </c>
       <c r="D121" s="40" t="s">
-        <v>3480</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15">
       <c r="A122" s="40" t="s">
-        <v>3243</v>
+        <v>3241</v>
       </c>
       <c r="B122" s="40" t="s">
-        <v>3244</v>
+        <v>3242</v>
       </c>
       <c r="C122" s="40" t="s">
-        <v>3335</v>
+        <v>3333</v>
       </c>
       <c r="D122" s="40" t="s">
-        <v>3481</v>
+        <v>3477</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15">
       <c r="A123" s="40" t="s">
-        <v>3245</v>
+        <v>3243</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>3246</v>
+        <v>3244</v>
       </c>
       <c r="C123" s="40" t="s">
-        <v>3336</v>
+        <v>3334</v>
       </c>
       <c r="D123" s="40" t="s">
-        <v>3482</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15">
       <c r="A124" s="40" t="s">
-        <v>3247</v>
+        <v>3245</v>
       </c>
       <c r="B124" s="40" t="s">
-        <v>3248</v>
+        <v>3246</v>
       </c>
       <c r="C124" s="40" t="s">
-        <v>3337</v>
+        <v>3335</v>
       </c>
       <c r="D124" s="40" t="s">
-        <v>3483</v>
+        <v>3479</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15">
       <c r="A125" s="40" t="s">
-        <v>3249</v>
+        <v>3247</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>3250</v>
+        <v>3248</v>
       </c>
       <c r="C125" s="40" t="s">
-        <v>3373</v>
+        <v>3371</v>
       </c>
       <c r="D125" s="40" t="s">
-        <v>3496</v>
+        <v>3491</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15">
       <c r="A126" s="40" t="s">
-        <v>3251</v>
+        <v>3249</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>3252</v>
+        <v>3250</v>
       </c>
       <c r="C126" s="40" t="s">
-        <v>3338</v>
+        <v>3336</v>
       </c>
       <c r="D126" s="40" t="s">
-        <v>3484</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15">
       <c r="A127" s="40" t="s">
-        <v>3253</v>
+        <v>3251</v>
       </c>
       <c r="B127" s="40" t="s">
-        <v>3254</v>
+        <v>3252</v>
       </c>
       <c r="C127" s="40" t="s">
-        <v>3339</v>
+        <v>3337</v>
       </c>
       <c r="D127" s="40" t="s">
-        <v>3485</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15">
       <c r="A128" s="40" t="s">
-        <v>3255</v>
+        <v>3253</v>
       </c>
       <c r="B128" s="40" t="s">
-        <v>3256</v>
+        <v>3254</v>
       </c>
       <c r="C128" s="40" t="s">
-        <v>3340</v>
+        <v>3338</v>
       </c>
       <c r="D128" s="40" t="s">
-        <v>3486</v>
+        <v>3482</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15">
       <c r="A129" s="40" t="s">
-        <v>3257</v>
+        <v>3255</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>3258</v>
+        <v>3256</v>
       </c>
       <c r="C129" s="40" t="s">
-        <v>3341</v>
+        <v>3339</v>
       </c>
       <c r="D129" s="40" t="s">
-        <v>3487</v>
+        <v>3552</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15">
@@ -25003,8 +25003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -25041,7 +25041,7 @@
         <v>1926</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>3522</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -25055,7 +25055,7 @@
         <v>1973</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>3375</v>
+        <v>3373</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -25069,7 +25069,7 @@
         <v>1974</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>3376</v>
+        <v>3374</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -25083,7 +25083,7 @@
         <v>3043</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>3377</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -25097,7 +25097,7 @@
         <v>3044</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>3378</v>
+        <v>3376</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -25108,10 +25108,10 @@
         <v>2914</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>3045</v>
+        <v>3550</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>3379</v>
+        <v>3377</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -25122,10 +25122,10 @@
         <v>2916</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>3063</v>
+        <v>3551</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>3380</v>
+        <v>3378</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -25136,10 +25136,10 @@
         <v>2918</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>3046</v>
+        <v>3045</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>3392</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -25150,10 +25150,10 @@
         <v>2920</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>3383</v>
+        <v>3381</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>3381</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -25164,10 +25164,10 @@
         <v>2922</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>3384</v>
+        <v>3382</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>3382</v>
+        <v>3380</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -25178,10 +25178,10 @@
         <v>2924</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>3068</v>
+        <v>3066</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>3385</v>
+        <v>3383</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -25192,10 +25192,10 @@
         <v>2926</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>3067</v>
+        <v>3065</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>3386</v>
+        <v>3384</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -25206,10 +25206,10 @@
         <v>2928</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>3048</v>
+        <v>3047</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>3387</v>
+        <v>3385</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -25220,10 +25220,10 @@
         <v>2930</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>3065</v>
+        <v>3063</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>3388</v>
+        <v>3386</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -25234,10 +25234,10 @@
         <v>2932</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>3066</v>
+        <v>3064</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>3389</v>
+        <v>3387</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -25251,7 +25251,7 @@
         <v>1944</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>3391</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -25262,10 +25262,10 @@
         <v>2936</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>3064</v>
+        <v>3062</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>3390</v>
+        <v>3388</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -25276,10 +25276,10 @@
         <v>2937</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>3047</v>
+        <v>3046</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>3523</v>
+        <v>3518</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -25290,10 +25290,10 @@
         <v>2939</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>3077</v>
+        <v>3075</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>3393</v>
+        <v>3391</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -25304,10 +25304,10 @@
         <v>2940</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>3062</v>
+        <v>3061</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>3394</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -25318,10 +25318,10 @@
         <v>2940</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>3069</v>
+        <v>3067</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>3394</v>
+        <v>3392</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -25332,10 +25332,10 @@
         <v>2943</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>3078</v>
+        <v>3076</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>3395</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -25346,10 +25346,10 @@
         <v>2943</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>3079</v>
+        <v>3077</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>3395</v>
+        <v>3393</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -25360,10 +25360,10 @@
         <v>2946</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>3396</v>
+        <v>3394</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>3397</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -25374,10 +25374,10 @@
         <v>2948</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>3076</v>
+        <v>3074</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>3398</v>
+        <v>3396</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -25391,7 +25391,7 @@
         <v>2042</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>3401</v>
+        <v>3399</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -25402,10 +25402,10 @@
         <v>2952</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>3072</v>
+        <v>3070</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>3402</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -25416,10 +25416,10 @@
         <v>2954</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>3073</v>
+        <v>3071</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>3403</v>
+        <v>3401</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -25430,10 +25430,10 @@
         <v>2956</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>3404</v>
+        <v>3402</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>3405</v>
+        <v>3403</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -25447,7 +25447,7 @@
         <v>2043</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>3399</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -25458,10 +25458,10 @@
         <v>2960</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>3075</v>
+        <v>3073</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>3406</v>
+        <v>3404</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -25475,7 +25475,7 @@
         <v>2047</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>3408</v>
+        <v>3406</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -25486,10 +25486,10 @@
         <v>2964</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>3074</v>
+        <v>3072</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>3407</v>
+        <v>3405</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -25503,7 +25503,7 @@
         <v>2045</v>
       </c>
       <c r="D35" s="40" t="s">
-        <v>3400</v>
+        <v>3398</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -25514,10 +25514,10 @@
         <v>2968</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>3071</v>
+        <v>3069</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>3409</v>
+        <v>3407</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -25528,10 +25528,10 @@
         <v>2970</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>3070</v>
+        <v>3068</v>
       </c>
       <c r="D37" s="40" t="s">
-        <v>3410</v>
+        <v>3408</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -25542,10 +25542,10 @@
         <v>2972</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>3080</v>
+        <v>3078</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>3411</v>
+        <v>3409</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -25556,10 +25556,10 @@
         <v>2974</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>3412</v>
+        <v>3410</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>3413</v>
+        <v>3411</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -25570,10 +25570,10 @@
         <v>2976</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>3081</v>
+        <v>3079</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>3414</v>
+        <v>3412</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -25584,10 +25584,10 @@
         <v>2978</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>3415</v>
+        <v>3413</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -25598,10 +25598,10 @@
         <v>2980</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>3083</v>
+        <v>3081</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>3416</v>
+        <v>3414</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -25612,10 +25612,10 @@
         <v>2982</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>3084</v>
+        <v>3082</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>3417</v>
+        <v>3415</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -25626,10 +25626,10 @@
         <v>2984</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>3085</v>
+        <v>3083</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>3418</v>
+        <v>3416</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -25640,10 +25640,10 @@
         <v>2986</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>3086</v>
+        <v>3084</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>3419</v>
+        <v>3417</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -25654,10 +25654,10 @@
         <v>2988</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>3087</v>
+        <v>3085</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>3420</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -25668,10 +25668,10 @@
         <v>2990</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>3088</v>
+        <v>3086</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>3421</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -25682,10 +25682,10 @@
         <v>2992</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>3089</v>
+        <v>3087</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>3422</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -25696,10 +25696,10 @@
         <v>2994</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>3090</v>
+        <v>3088</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>3423</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -25707,10 +25707,10 @@
         <v>168</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>3516</v>
+        <v>3511</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>3511</v>
+        <v>3506</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -25718,10 +25718,10 @@
         <v>2995</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>3049</v>
+        <v>3048</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>3513</v>
+        <v>3508</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -25729,10 +25729,10 @@
         <v>2996</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>3050</v>
+        <v>3049</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>3514</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -25740,10 +25740,10 @@
         <v>2997</v>
       </c>
       <c r="C53" s="40" t="s">
-        <v>3051</v>
+        <v>3050</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>3515</v>
+        <v>3510</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -25751,10 +25751,10 @@
         <v>2998</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>3052</v>
+        <v>3051</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>3517</v>
+        <v>3512</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -25762,10 +25762,10 @@
         <v>2999</v>
       </c>
       <c r="C55" s="40" t="s">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>3518</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -25773,10 +25773,10 @@
         <v>3000</v>
       </c>
       <c r="C56" s="40" t="s">
-        <v>3054</v>
+        <v>3053</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>3519</v>
+        <v>3514</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -25787,10 +25787,10 @@
         <v>3002</v>
       </c>
       <c r="C57" s="40" t="s">
-        <v>3055</v>
+        <v>3054</v>
       </c>
       <c r="D57" s="40" t="s">
-        <v>3512</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -25801,10 +25801,10 @@
         <v>3004</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>3091</v>
+        <v>3089</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>3424</v>
+        <v>3422</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -25815,10 +25815,10 @@
         <v>3006</v>
       </c>
       <c r="C59" s="40" t="s">
-        <v>3056</v>
+        <v>3055</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>3425</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -25829,10 +25829,10 @@
         <v>3007</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>3092</v>
+        <v>3090</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>3426</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -25843,10 +25843,10 @@
         <v>3007</v>
       </c>
       <c r="C61" s="40" t="s">
-        <v>3093</v>
+        <v>3091</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>3426</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -25857,10 +25857,10 @@
         <v>3010</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>3094</v>
+        <v>3092</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>3427</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -25871,10 +25871,10 @@
         <v>3012</v>
       </c>
       <c r="C63" s="40" t="s">
-        <v>3095</v>
+        <v>3093</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>3428</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -25885,10 +25885,10 @@
         <v>3012</v>
       </c>
       <c r="C64" s="40" t="s">
-        <v>3096</v>
+        <v>3094</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>3428</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -25899,10 +25899,10 @@
         <v>3012</v>
       </c>
       <c r="C65" s="40" t="s">
-        <v>3097</v>
+        <v>3095</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>3428</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -25913,10 +25913,10 @@
         <v>3015</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>3098</v>
+        <v>3096</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>3429</v>
+        <v>3427</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -25927,10 +25927,10 @@
         <v>3017</v>
       </c>
       <c r="C67" s="40" t="s">
-        <v>3099</v>
+        <v>3097</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>3430</v>
+        <v>3428</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -25941,10 +25941,10 @@
         <v>3019</v>
       </c>
       <c r="C68" s="40" t="s">
-        <v>3100</v>
+        <v>3098</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>3431</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -25955,13 +25955,13 @@
         <v>3021</v>
       </c>
       <c r="C69" s="40" t="s">
-        <v>3101</v>
+        <v>3099</v>
       </c>
       <c r="D69" s="40" t="s">
-        <v>3433</v>
+        <v>3431</v>
       </c>
       <c r="E69" s="40" t="s">
-        <v>3432</v>
+        <v>3430</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -25969,10 +25969,10 @@
         <v>3022</v>
       </c>
       <c r="C70" s="40" t="s">
-        <v>3057</v>
+        <v>3056</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>3520</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -25980,10 +25980,10 @@
         <v>3023</v>
       </c>
       <c r="C71" s="40" t="s">
-        <v>3058</v>
+        <v>3057</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>3521</v>
+        <v>3516</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -25994,10 +25994,10 @@
         <v>3025</v>
       </c>
       <c r="C72" s="40" t="s">
-        <v>3059</v>
+        <v>3058</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>3434</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -26008,10 +26008,10 @@
         <v>3027</v>
       </c>
       <c r="C73" s="40" t="s">
-        <v>3060</v>
+        <v>3059</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>3435</v>
+        <v>3433</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -26022,10 +26022,10 @@
         <v>3029</v>
       </c>
       <c r="C74" s="40" t="s">
-        <v>3061</v>
+        <v>3060</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>3436</v>
+        <v>3434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ch6 end events translating
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -35,14 +35,14 @@
     <sheet name="常見生詞" sheetId="19" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'names-名前'!$A$1:$H$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'names-名前'!$A$1:$H$76</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5075" uniqueCount="3597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5078" uniqueCount="3600">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -10879,6 +10879,15 @@
   </si>
   <si>
     <t>CC Certificate</t>
+  </si>
+  <si>
+    <t>Kurowa</t>
+  </si>
+  <si>
+    <t>ミラージュ</t>
+  </si>
+  <si>
+    <t>Mirage</t>
   </si>
 </sst>
 </file>
@@ -11964,7 +11973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
@@ -22417,17 +22426,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="12.0703125" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="66.5703125" customWidth="1"/>
+    <col min="4" max="4" width="75" customWidth="1"/>
     <col min="5" max="5" width="15.35546875" customWidth="1"/>
     <col min="6" max="6" width="54.5" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
@@ -22962,28 +22971,18 @@
       <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" ht="15">
-      <c r="A29" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>2204</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>2266</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>2303</v>
-      </c>
-      <c r="G29" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H29" s="23"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40" t="s">
+        <v>3598</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40" t="s">
+        <v>3599</v>
+      </c>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:8" ht="15">
       <c r="A30" s="23" t="s">
@@ -22993,19 +22992,19 @@
         <v>63</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>2302</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>67</v>
+        <v>2303</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="H30" s="23"/>
     </row>
@@ -23017,15 +23016,19 @@
         <v>63</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="23"/>
+        <v>66</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>2205</v>
+      </c>
       <c r="E31" s="23" t="s">
-        <v>2268</v>
-      </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23" t="s">
-        <v>69</v>
+        <v>2267</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>2302</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="H31" s="23"/>
     </row>
@@ -23034,22 +23037,18 @@
         <v>62</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>2206</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D32" s="23"/>
       <c r="E32" s="23" t="s">
-        <v>2269</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>2783</v>
-      </c>
+        <v>2268</v>
+      </c>
+      <c r="F32" s="23"/>
       <c r="G32" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H32" s="23"/>
     </row>
@@ -23061,19 +23060,19 @@
         <v>7</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>2617</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>73</v>
+        <v>2783</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="H33" s="23"/>
     </row>
@@ -23085,87 +23084,87 @@
         <v>7</v>
       </c>
       <c r="C34" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>2207</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>2270</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>2617</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="23"/>
+    </row>
+    <row r="35" spans="1:8" ht="15">
+      <c r="A35" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D35" s="23" t="s">
         <v>2208</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E35" s="23" t="s">
         <v>2271</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F35" s="23" t="s">
         <v>2618</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G35" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="H34" s="23"/>
-    </row>
-    <row r="35" spans="1:8" ht="15">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40" t="s">
+      <c r="H35" s="23"/>
+    </row>
+    <row r="36" spans="1:8" ht="15">
+      <c r="A36" s="40"/>
+      <c r="B36" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C36" s="40" t="s">
         <v>2787</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D36" s="40" t="s">
         <v>2784</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E36" s="40" t="s">
         <v>3562</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F36" s="40" t="s">
         <v>2786</v>
       </c>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-    </row>
-    <row r="36" spans="1:8" ht="15">
-      <c r="A36" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>2209</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>2272</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>2782</v>
-      </c>
-      <c r="G36" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="H36" s="23"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
     </row>
     <row r="37" spans="1:8" ht="15">
       <c r="A37" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>2275</v>
+        <v>2272</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>2619</v>
+        <v>2782</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H37" s="23"/>
     </row>
@@ -23180,13 +23179,13 @@
         <v>78</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>2275</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>2633</v>
+        <v>2619</v>
       </c>
       <c r="G38" s="23" t="s">
         <v>79</v>
@@ -23201,19 +23200,19 @@
         <v>23</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>2586</v>
+        <v>2275</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>2620</v>
+        <v>2633</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H39" s="23"/>
     </row>
@@ -23225,19 +23224,19 @@
         <v>23</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>2273</v>
+        <v>2586</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H40" s="23"/>
     </row>
@@ -23249,19 +23248,19 @@
         <v>23</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H41" s="23"/>
     </row>
@@ -23270,22 +23269,22 @@
         <v>62</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>2265</v>
+        <v>2274</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="G42" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H42" s="23"/>
     </row>
@@ -23297,19 +23296,19 @@
         <v>10</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>2276</v>
-      </c>
-      <c r="F43" s="40" t="s">
-        <v>3571</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>89</v>
+        <v>2265</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>2623</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="H43" s="23"/>
     </row>
@@ -23321,19 +23320,19 @@
         <v>10</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="F44" s="40" t="s">
-        <v>3569</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>91</v>
+        <v>3571</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>89</v>
       </c>
       <c r="H44" s="23"/>
     </row>
@@ -23345,19 +23344,19 @@
         <v>10</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>2278</v>
-      </c>
-      <c r="F45" s="23" t="s">
-        <v>3575</v>
+        <v>2277</v>
+      </c>
+      <c r="F45" s="40" t="s">
+        <v>3569</v>
       </c>
       <c r="G45" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H45" s="23"/>
     </row>
@@ -23366,22 +23365,22 @@
         <v>62</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>3477</v>
+        <v>2278</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>2625</v>
+        <v>3575</v>
       </c>
       <c r="G46" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H46" s="23"/>
     </row>
@@ -23393,19 +23392,19 @@
         <v>15</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>2293</v>
+        <v>3477</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="G47" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H47" s="23"/>
     </row>
@@ -23417,19 +23416,19 @@
         <v>15</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>3591</v>
+        <v>2293</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H48" s="23"/>
     </row>
@@ -23441,19 +23440,19 @@
         <v>15</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>2294</v>
+        <v>3591</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="G49" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H49" s="23"/>
     </row>
@@ -23465,19 +23464,19 @@
         <v>15</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>2299</v>
+        <v>2294</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="G50" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H50" s="23"/>
     </row>
@@ -23489,19 +23488,19 @@
         <v>15</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>2292</v>
+        <v>2299</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>3325</v>
+        <v>2629</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H51" s="23"/>
     </row>
@@ -23510,22 +23509,22 @@
         <v>62</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>2295</v>
-      </c>
-      <c r="F52" s="40" t="s">
-        <v>3570</v>
+        <v>2292</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>3325</v>
       </c>
       <c r="G52" s="23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H52" s="23"/>
     </row>
@@ -23534,22 +23533,22 @@
         <v>62</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>1916</v>
+        <v>2225</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>2296</v>
-      </c>
-      <c r="F53" s="23" t="s">
-        <v>2630</v>
+        <v>2295</v>
+      </c>
+      <c r="F53" s="40" t="s">
+        <v>3570</v>
       </c>
       <c r="G53" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H53" s="23"/>
     </row>
@@ -23564,13 +23563,13 @@
         <v>110</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>2226</v>
+        <v>1916</v>
       </c>
       <c r="E54" s="23" t="s">
         <v>2296</v>
       </c>
-      <c r="F54" s="40" t="s">
-        <v>3572</v>
+      <c r="F54" s="23" t="s">
+        <v>2630</v>
       </c>
       <c r="G54" s="23" t="s">
         <v>111</v>
@@ -23585,19 +23584,19 @@
         <v>109</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>2297</v>
-      </c>
-      <c r="F55" s="23" t="s">
-        <v>2632</v>
+        <v>2296</v>
+      </c>
+      <c r="F55" s="40" t="s">
+        <v>3572</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H55" s="23"/>
     </row>
@@ -23609,17 +23608,19 @@
         <v>109</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>3592</v>
-      </c>
-      <c r="F56" s="23"/>
+        <v>2297</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>2632</v>
+      </c>
       <c r="G56" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H56" s="23"/>
     </row>
@@ -23631,17 +23632,17 @@
         <v>109</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>2298</v>
+        <v>3592</v>
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H57" s="23"/>
     </row>
@@ -23650,48 +23651,48 @@
         <v>62</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>2284</v>
+        <v>2298</v>
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H58" s="23"/>
     </row>
     <row r="59" spans="1:8" ht="15">
       <c r="A59" s="23" t="s">
-        <v>1917</v>
+        <v>62</v>
       </c>
       <c r="B59" s="23" t="s">
         <v>118</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>1918</v>
+        <v>2230</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>2290</v>
+        <v>2284</v>
       </c>
       <c r="F59" s="23"/>
       <c r="G59" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H59" s="23"/>
     </row>
     <row r="60" spans="1:8" ht="15">
       <c r="A60" s="23" t="s">
-        <v>62</v>
+        <v>1917</v>
       </c>
       <c r="B60" s="23" t="s">
         <v>118</v>
@@ -23700,7 +23701,7 @@
         <v>121</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>2231</v>
+        <v>1918</v>
       </c>
       <c r="E60" s="23" t="s">
         <v>2290</v>
@@ -23719,17 +23720,17 @@
         <v>118</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="F61" s="23"/>
       <c r="G61" s="23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H61" s="23"/>
     </row>
@@ -23741,17 +23742,17 @@
         <v>118</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>2289</v>
+        <v>2291</v>
       </c>
       <c r="F62" s="23"/>
       <c r="G62" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H62" s="23"/>
     </row>
@@ -23763,15 +23764,17 @@
         <v>118</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>2234</v>
-      </c>
-      <c r="E63" s="23"/>
+        <v>2233</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>2289</v>
+      </c>
       <c r="F63" s="23"/>
       <c r="G63" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H63" s="23"/>
     </row>
@@ -23780,20 +23783,20 @@
         <v>62</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>1919</v>
+        <v>118</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>2272</v>
+        <v>3597</v>
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="23" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="H64" s="23"/>
     </row>
@@ -23802,20 +23805,20 @@
         <v>62</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>118</v>
+        <v>1919</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>2236</v>
+        <v>2235</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>2285</v>
+        <v>2272</v>
       </c>
       <c r="F65" s="23"/>
       <c r="G65" s="23" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
       <c r="H65" s="23"/>
     </row>
@@ -23824,20 +23827,20 @@
         <v>62</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
       <c r="F66" s="23"/>
       <c r="G66" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H66" s="23"/>
     </row>
@@ -23849,17 +23852,17 @@
         <v>131</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D67" s="23" t="s">
         <v>2237</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="F67" s="23"/>
       <c r="G67" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H67" s="23"/>
     </row>
@@ -23871,17 +23874,17 @@
         <v>131</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="E68" s="23" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="F68" s="23"/>
       <c r="G68" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H68" s="23"/>
     </row>
@@ -23893,17 +23896,17 @@
         <v>131</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>2282</v>
+        <v>2288</v>
       </c>
       <c r="F69" s="23"/>
       <c r="G69" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H69" s="23"/>
     </row>
@@ -23915,17 +23918,17 @@
         <v>131</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="F70" s="23"/>
       <c r="G70" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H70" s="23"/>
     </row>
@@ -23937,17 +23940,17 @@
         <v>131</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>2280</v>
+        <v>2283</v>
       </c>
       <c r="F71" s="23"/>
       <c r="G71" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H71" s="23"/>
     </row>
@@ -23956,18 +23959,20 @@
         <v>62</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D72" s="23"/>
+        <v>142</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>2241</v>
+      </c>
       <c r="E72" s="23" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="F72" s="23"/>
       <c r="G72" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H72" s="23"/>
     </row>
@@ -23979,17 +23984,15 @@
         <v>144</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="D73" s="23" t="s">
-        <v>2242</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D73" s="23"/>
       <c r="E73" s="23" t="s">
-        <v>2279</v>
+        <v>2281</v>
       </c>
       <c r="F73" s="23"/>
       <c r="G73" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H73" s="23"/>
     </row>
@@ -23998,20 +24001,20 @@
         <v>62</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D74" s="23" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>2300</v>
+        <v>2279</v>
       </c>
       <c r="F74" s="23"/>
       <c r="G74" s="23" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H74" s="23"/>
     </row>
@@ -24023,22 +24026,44 @@
         <v>149</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="E75" s="23" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
       <c r="F75" s="23"/>
       <c r="G75" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H75" s="23"/>
+    </row>
+    <row r="76" spans="1:8" ht="15">
+      <c r="A76" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>2301</v>
+      </c>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="H75" s="23"/>
+      <c r="H76" s="23"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H75"/>
+  <autoFilter ref="A1:H76"/>
   <phoneticPr fontId="7"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Final updates for ch6 public release
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6049" uniqueCount="4402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6057" uniqueCount="4403">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -13311,6 +13311,9 @@
   </si>
   <si>
     <t>A corpse brought to life by magic. Not particularly strong.</t>
+  </si>
+  <si>
+    <t>Enemies</t>
   </si>
 </sst>
 </file>
@@ -14073,10 +14076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -14136,16 +14139,10 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="40" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>2233</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>2288</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>3610</v>
+        <v>4271</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="58"/>
@@ -14153,16 +14150,10 @@
     </row>
     <row r="6" spans="1:7" ht="15.9">
       <c r="A6" s="40" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>2234</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>2289</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>3611</v>
+        <v>2255</v>
       </c>
       <c r="E6" s="56"/>
       <c r="F6" s="56"/>
@@ -14170,246 +14161,130 @@
     </row>
     <row r="7" spans="1:7" ht="15.9">
       <c r="A7" s="40" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>2209</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>3436</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>3583</v>
+        <v>2256</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="57"/>
       <c r="G7" s="57"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>2210</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>2281</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>2605</v>
-      </c>
       <c r="E8" s="55"/>
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>2212</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>2282</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>2607</v>
-      </c>
       <c r="E9" s="55"/>
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>4271</v>
-      </c>
       <c r="E10" s="55"/>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>4400</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>2244</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>4401</v>
-      </c>
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
     </row>
     <row r="12" spans="1:7" ht="15.9">
-      <c r="A12" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>4395</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>2243</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>4396</v>
-      </c>
       <c r="E12" s="57"/>
       <c r="F12" s="57"/>
       <c r="G12" s="57"/>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="51" t="s">
-        <v>3612</v>
-      </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-    </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="40" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>3613</v>
-      </c>
-      <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="F15" s="55"/>
       <c r="G15" s="55"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
       <c r="E16" s="55"/>
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="40" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>3614</v>
-      </c>
-      <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55"/>
       <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
+      <c r="A18" s="51" t="s">
+        <v>3612</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="55"/>
       <c r="F18" s="55"/>
       <c r="G18" s="55"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="29" t="s">
-        <v>992</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>993</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>994</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>3512</v>
-      </c>
+      <c r="A19" s="55"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="55"/>
       <c r="F19" s="55"/>
       <c r="G19" s="55"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="29"/>
+      <c r="A20" s="40" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>1027</v>
+      </c>
       <c r="C20" s="40" t="s">
-        <v>996</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>2740</v>
-      </c>
+        <v>3613</v>
+      </c>
+      <c r="D20" s="55"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="40" t="s">
-        <v>4116</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>2029</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>4117</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>4122</v>
-      </c>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="55"/>
       <c r="G21" s="55"/>
     </row>
     <row r="22" spans="1:7">
+      <c r="A22" s="40" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>1037</v>
+      </c>
       <c r="C22" s="40" t="s">
-        <v>4118</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>4120</v>
-      </c>
+        <v>3614</v>
+      </c>
+      <c r="D22" s="55"/>
       <c r="E22" s="55"/>
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="C23" s="40" t="s">
-        <v>4119</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>4121</v>
-      </c>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="55"/>
       <c r="F23" s="55"/>
       <c r="G23" s="55"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="40" t="s">
-        <v>907</v>
+      <c r="A24" s="29" t="s">
+        <v>992</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>946</v>
+        <v>993</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>947</v>
+        <v>994</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>2724</v>
+        <v>3512</v>
       </c>
       <c r="E24" s="55"/>
       <c r="F24" s="55"/>
@@ -14417,94 +14292,137 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="29"/>
-      <c r="B25" s="40" t="s">
-        <v>949</v>
-      </c>
       <c r="C25" s="40" t="s">
-        <v>950</v>
+        <v>996</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>2726</v>
+        <v>2740</v>
       </c>
       <c r="E25" s="55"/>
       <c r="F25" s="55"/>
       <c r="G25" s="55"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="29"/>
+      <c r="A26" s="40" t="s">
+        <v>4116</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>2029</v>
+      </c>
       <c r="C26" s="40" t="s">
-        <v>952</v>
+        <v>4117</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>2725</v>
+        <v>4122</v>
       </c>
       <c r="E26" s="55"/>
       <c r="F26" s="55"/>
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="29"/>
-      <c r="B27" s="40" t="s">
-        <v>954</v>
-      </c>
       <c r="C27" s="40" t="s">
-        <v>955</v>
+        <v>4118</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>3511</v>
+        <v>4120</v>
       </c>
       <c r="E27" s="55"/>
       <c r="F27" s="55"/>
       <c r="G27" s="55"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="29"/>
-      <c r="B28" s="40" t="s">
-        <v>957</v>
-      </c>
       <c r="C28" s="40" t="s">
-        <v>958</v>
+        <v>4119</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>2727</v>
+        <v>4121</v>
       </c>
       <c r="E28" s="55"/>
       <c r="F28" s="55"/>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="29"/>
+      <c r="A29" s="40" t="s">
+        <v>907</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>946</v>
+      </c>
       <c r="C29" s="40" t="s">
-        <v>959</v>
+        <v>947</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>2728</v>
+        <v>2724</v>
       </c>
       <c r="E29" s="55"/>
       <c r="F29" s="55"/>
       <c r="G29" s="55"/>
     </row>
     <row r="30" spans="1:7">
+      <c r="A30" s="29"/>
+      <c r="B30" s="40" t="s">
+        <v>949</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>950</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>2726</v>
+      </c>
       <c r="E30" s="55"/>
       <c r="F30" s="55"/>
       <c r="G30" s="55"/>
     </row>
     <row r="31" spans="1:7">
+      <c r="A31" s="29"/>
+      <c r="C31" s="40" t="s">
+        <v>952</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>2725</v>
+      </c>
       <c r="E31" s="55"/>
       <c r="F31" s="55"/>
       <c r="G31" s="55"/>
     </row>
     <row r="32" spans="1:7">
+      <c r="A32" s="29"/>
+      <c r="B32" s="40" t="s">
+        <v>954</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>955</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>3511</v>
+      </c>
       <c r="E32" s="55"/>
       <c r="F32" s="55"/>
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="1:7">
+      <c r="A33" s="29"/>
+      <c r="B33" s="40" t="s">
+        <v>957</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>958</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>2727</v>
+      </c>
       <c r="E33" s="55"/>
       <c r="F33" s="55"/>
       <c r="G33" s="55"/>
     </row>
     <row r="34" spans="1:7">
+      <c r="A34" s="29"/>
+      <c r="C34" s="40" t="s">
+        <v>959</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>2728</v>
+      </c>
       <c r="E34" s="55"/>
       <c r="F34" s="55"/>
       <c r="G34" s="55"/>
@@ -14636,6 +14554,126 @@
       </c>
       <c r="D51" s="40" t="s">
         <v>4401</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.9">
+      <c r="A52" s="40" t="s">
+        <v>3562</v>
+      </c>
+      <c r="B52" s="61" t="s">
+        <v>3564</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>3563</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="51" t="s">
+        <v>4402</v>
+      </c>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" s="40" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>2234</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>2289</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>2209</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>3436</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>2210</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>2212</v>
+      </c>
+      <c r="C59" s="40" t="s">
+        <v>2282</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" s="40" t="s">
+        <v>4400</v>
+      </c>
+      <c r="C60" s="40" t="s">
+        <v>2244</v>
+      </c>
+      <c r="D60" s="40" t="s">
+        <v>4401</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>4395</v>
+      </c>
+      <c r="C61" s="40" t="s">
+        <v>2243</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>4396</v>
       </c>
     </row>
   </sheetData>
@@ -25280,8 +25318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:F12"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -33112,8 +33150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>

</xml_diff>

<commit_message>
lots of ch7 translated
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6056" uniqueCount="4415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6085" uniqueCount="4415">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -14113,8 +14113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -14349,52 +14349,144 @@
       </c>
     </row>
     <row r="21" spans="1:7">
+      <c r="A21" s="29" t="s">
+        <v>926</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>927</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>928</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>2717</v>
+      </c>
       <c r="E21" s="55"/>
       <c r="F21" s="55"/>
       <c r="G21" s="55"/>
     </row>
     <row r="22" spans="1:7">
+      <c r="A22" s="29"/>
+      <c r="C22" s="40" t="s">
+        <v>930</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>2718</v>
+      </c>
       <c r="E22" s="55"/>
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:7">
+      <c r="A23" s="29" t="s">
+        <v>926</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>931</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>932</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>2720</v>
+      </c>
       <c r="E23" s="55"/>
       <c r="F23" s="55"/>
       <c r="G23" s="55"/>
     </row>
     <row r="24" spans="1:7">
+      <c r="A24" s="29"/>
+      <c r="C24" s="40" t="s">
+        <v>934</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>2719</v>
+      </c>
       <c r="E24" s="55"/>
       <c r="F24" s="55"/>
       <c r="G24" s="55"/>
     </row>
     <row r="25" spans="1:7">
+      <c r="A25" s="29" t="s">
+        <v>926</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>936</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>937</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>2720</v>
+      </c>
       <c r="E25" s="55"/>
       <c r="F25" s="55"/>
       <c r="G25" s="55"/>
     </row>
     <row r="26" spans="1:7">
+      <c r="A26" s="29"/>
+      <c r="C26" s="40" t="s">
+        <v>939</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>2721</v>
+      </c>
       <c r="E26" s="55"/>
       <c r="F26" s="55"/>
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:7">
+      <c r="A27" s="29"/>
+      <c r="B27" s="40" t="s">
+        <v>941</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>937</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>2720</v>
+      </c>
       <c r="E27" s="55"/>
       <c r="F27" s="55"/>
       <c r="G27" s="55"/>
     </row>
     <row r="28" spans="1:7">
+      <c r="A28" s="29"/>
+      <c r="C28" s="40" t="s">
+        <v>939</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>2721</v>
+      </c>
       <c r="E28" s="55"/>
       <c r="F28" s="55"/>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" s="41"/>
+      <c r="A29" s="29" t="s">
+        <v>926</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>942</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>943</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>2722</v>
+      </c>
       <c r="E29" s="55"/>
       <c r="F29" s="55"/>
       <c r="G29" s="55"/>
     </row>
     <row r="30" spans="1:7">
+      <c r="A30" s="29"/>
+      <c r="C30" s="40" t="s">
+        <v>934</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>2719</v>
+      </c>
       <c r="E30" s="55"/>
       <c r="F30" s="55"/>
       <c r="G30" s="55"/>
@@ -19142,8 +19234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:E74"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -25281,7 +25373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F42" sqref="C42:F42"/>
     </sheetView>
   </sheetViews>
@@ -27851,7 +27943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F306"/>
   <sheetViews>
-    <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="FU62" sqref="FU62"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chapter 8 spare dialogue complete
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091" tabRatio="627" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7725" uniqueCount="4796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7751" uniqueCount="4813">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -13525,9 +13525,6 @@
     <t>Investigate 情報收集</t>
   </si>
   <si>
-    <t>Items アイテム</t>
-  </si>
-  <si>
     <t>Guard (Battle Saves)</t>
   </si>
   <si>
@@ -13558,9 +13555,6 @@
     <t>Inflicts Charm on Aroused foes. Range 2.</t>
   </si>
   <si>
-    <t>Sexual Aroma</t>
-  </si>
-  <si>
     <t>Enemy Type 2: Junior Student B</t>
   </si>
   <si>
@@ -13795,9 +13789,6 @@
     <t>Fascination</t>
   </si>
   <si>
-    <t>Charmed</t>
-  </si>
-  <si>
     <t>Aphrodasiac lotion that adds a 30% chance for attacks to charm foes.</t>
   </si>
   <si>
@@ -14504,6 +14495,66 @@
   </si>
   <si>
     <t>Makes foes fall in love during combat.</t>
+  </si>
+  <si>
+    <t>Ignore Luminara's advice</t>
+  </si>
+  <si>
+    <t>Deactivate the Holy Sword</t>
+  </si>
+  <si>
+    <t>Endure Temptation</t>
+  </si>
+  <si>
+    <t>Stare intently</t>
+  </si>
+  <si>
+    <t>Look away</t>
+  </si>
+  <si>
+    <t>Let your desires think for you</t>
+  </si>
+  <si>
+    <t>I want her feet to step over my penis…</t>
+  </si>
+  <si>
+    <t>No! I must resist!</t>
+  </si>
+  <si>
+    <t>I want to suck on her breasts…</t>
+  </si>
+  <si>
+    <t>Observe her carefully</t>
+  </si>
+  <si>
+    <t>Jump right in for the kill</t>
+  </si>
+  <si>
+    <t>Just relax</t>
+  </si>
+  <si>
+    <t>Muster your willpower and attack</t>
+  </si>
+  <si>
+    <t>I can't move…</t>
+  </si>
+  <si>
+    <t>Do as she says</t>
+  </si>
+  <si>
+    <t>Relax as she pumps your penis between her tits</t>
+  </si>
+  <si>
+    <t>Muster your willpower to defy her</t>
+  </si>
+  <si>
+    <t>I can't disobey her…</t>
+  </si>
+  <si>
+    <t>Somehow manage to shake her off</t>
+  </si>
+  <si>
+    <t>Let your body relax</t>
   </si>
 </sst>
 </file>
@@ -15257,8 +15308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -15433,7 +15484,7 @@
         <v>4467</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>4473</v>
+        <v>4472</v>
       </c>
       <c r="F8" s="59"/>
       <c r="G8" s="45"/>
@@ -15465,10 +15516,10 @@
         <v>2631</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>4475</v>
+        <v>4474</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>4477</v>
+        <v>4476</v>
       </c>
       <c r="G9" s="48"/>
       <c r="H9" s="67" t="s">
@@ -15493,10 +15544,10 @@
         <v>2630</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>4474</v>
+        <v>4473</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>4476</v>
+        <v>4475</v>
       </c>
       <c r="G10" s="45"/>
       <c r="H10" s="67" t="s">
@@ -15671,7 +15722,7 @@
         <v>4321</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>4478</v>
+        <v>4477</v>
       </c>
       <c r="G16" s="45"/>
       <c r="H16" s="67" t="s">
@@ -15734,7 +15785,18 @@
       <c r="L18" s="45"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="D19" s="59"/>
+      <c r="A19" s="31" t="s">
+        <v>914</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>4469</v>
+      </c>
       <c r="G19" s="45"/>
       <c r="H19" s="67" t="s">
         <v>3544</v>
@@ -15751,7 +15813,18 @@
       <c r="L19" s="45"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="D20" s="59"/>
+      <c r="A20" s="31" t="s">
+        <v>945</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>4470</v>
+      </c>
       <c r="G20" s="45"/>
       <c r="H20" s="67" t="s">
         <v>3546</v>
@@ -15768,6 +15841,7 @@
       <c r="L20" s="45"/>
     </row>
     <row r="21" spans="1:12">
+      <c r="A21" s="23"/>
       <c r="D21" s="59"/>
       <c r="G21" s="56"/>
       <c r="H21" s="67" t="s">
@@ -15819,18 +15893,6 @@
       <c r="L23" s="45"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="31" t="s">
-        <v>914</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>1426</v>
-      </c>
-      <c r="D24" s="59" t="s">
-        <v>4470</v>
-      </c>
       <c r="G24" s="57"/>
       <c r="H24" s="67" t="s">
         <v>3554</v>
@@ -15847,18 +15909,6 @@
       <c r="L24" s="45"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="31" t="s">
-        <v>945</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>1452</v>
-      </c>
-      <c r="D25" s="59" t="s">
-        <v>4471</v>
-      </c>
       <c r="G25" s="45"/>
       <c r="H25" s="67" t="s">
         <v>3556</v>
@@ -15875,8 +15925,6 @@
       <c r="L25" s="45"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="23"/>
-      <c r="D26" s="59"/>
       <c r="G26" s="56"/>
       <c r="H26" s="67" t="s">
         <v>3557</v>
@@ -15911,9 +15959,7 @@
       <c r="L27" s="45"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="37" t="s">
-        <v>4469</v>
-      </c>
+      <c r="A28" s="37"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
       <c r="D28" s="61"/>
@@ -15935,18 +15981,10 @@
       <c r="L28" s="45"/>
     </row>
     <row r="29" spans="1:12" ht="15.9">
-      <c r="A29" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>1903</v>
-      </c>
-      <c r="D29" s="62" t="s">
-        <v>2043</v>
-      </c>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="62"/>
       <c r="E29" s="60"/>
       <c r="F29" s="59"/>
       <c r="G29" s="48"/>
@@ -15965,18 +16003,10 @@
       <c r="L29" s="45"/>
     </row>
     <row r="30" spans="1:12" ht="15.9">
-      <c r="A30" s="13" t="s">
-        <v>788</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>789</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>4480</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>4479</v>
-      </c>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="60"/>
       <c r="F30" s="59"/>
       <c r="G30" s="48"/>
@@ -15995,9 +16025,7 @@
       <c r="L30" s="45"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="37" t="s">
-        <v>2533</v>
-      </c>
+      <c r="A31" s="37"/>
       <c r="D31" s="59"/>
       <c r="E31" s="60"/>
       <c r="F31" s="59"/>
@@ -16017,18 +16045,6 @@
       <c r="L31" s="45"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>2787</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>4559</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>3343</v>
-      </c>
       <c r="E32" s="60"/>
       <c r="F32" s="59"/>
       <c r="G32" s="45"/>
@@ -17081,7 +17097,7 @@
         <v>3648</v>
       </c>
       <c r="K80" s="66" t="s">
-        <v>4482</v>
+        <v>4480</v>
       </c>
       <c r="L80" s="45"/>
     </row>
@@ -17103,7 +17119,7 @@
         <v>3650</v>
       </c>
       <c r="K81" s="66" t="s">
-        <v>4483</v>
+        <v>4481</v>
       </c>
       <c r="L81" s="45"/>
     </row>
@@ -17125,7 +17141,7 @@
         <v>3652</v>
       </c>
       <c r="K82" s="66" t="s">
-        <v>4484</v>
+        <v>4482</v>
       </c>
       <c r="L82" s="45"/>
     </row>
@@ -17147,7 +17163,7 @@
         <v>3654</v>
       </c>
       <c r="K83" s="66" t="s">
-        <v>4485</v>
+        <v>4483</v>
       </c>
       <c r="L83" s="45"/>
     </row>
@@ -17169,7 +17185,7 @@
         <v>3656</v>
       </c>
       <c r="K84" s="66" t="s">
-        <v>4486</v>
+        <v>4484</v>
       </c>
       <c r="L84" s="45"/>
     </row>
@@ -17191,7 +17207,7 @@
         <v>3658</v>
       </c>
       <c r="K85" s="66" t="s">
-        <v>4487</v>
+        <v>4485</v>
       </c>
       <c r="L85" s="45"/>
     </row>
@@ -17212,7 +17228,7 @@
         <v>3660</v>
       </c>
       <c r="K86" s="66" t="s">
-        <v>4488</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -17232,7 +17248,7 @@
         <v>3661</v>
       </c>
       <c r="K87" s="66" t="s">
-        <v>4489</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -17401,7 +17417,7 @@
         <v>3673</v>
       </c>
       <c r="K97" s="66" t="s">
-        <v>4490</v>
+        <v>4488</v>
       </c>
     </row>
     <row r="98" spans="8:11">
@@ -17415,7 +17431,7 @@
         <v>3674</v>
       </c>
       <c r="K98" s="66" t="s">
-        <v>4493</v>
+        <v>4491</v>
       </c>
     </row>
     <row r="99" spans="8:11">
@@ -17423,13 +17439,13 @@
         <v>3513</v>
       </c>
       <c r="I99" s="66" t="s">
-        <v>4492</v>
+        <v>4490</v>
       </c>
       <c r="J99" s="66" t="s">
         <v>3675</v>
       </c>
       <c r="K99" s="66" t="s">
-        <v>4491</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="100" spans="8:11">
@@ -17443,7 +17459,7 @@
         <v>3677</v>
       </c>
       <c r="K100" s="66" t="s">
-        <v>4494</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="101" spans="8:11">
@@ -17457,7 +17473,7 @@
         <v>3679</v>
       </c>
       <c r="K101" s="66" t="s">
-        <v>4495</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="102" spans="8:11">
@@ -17471,7 +17487,7 @@
         <v>3681</v>
       </c>
       <c r="K102" s="66" t="s">
-        <v>4496</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="103" spans="8:11">
@@ -17485,7 +17501,7 @@
         <v>3683</v>
       </c>
       <c r="K103" s="66" t="s">
-        <v>4497</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="104" spans="8:11">
@@ -17499,7 +17515,7 @@
         <v>3685</v>
       </c>
       <c r="K104" s="66" t="s">
-        <v>4499</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="105" spans="8:11">
@@ -17513,7 +17529,7 @@
         <v>3687</v>
       </c>
       <c r="K105" s="66" t="s">
-        <v>4500</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="106" spans="8:11">
@@ -17527,7 +17543,7 @@
         <v>3689</v>
       </c>
       <c r="K106" s="66" t="s">
-        <v>4501</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="107" spans="8:11">
@@ -17541,7 +17557,7 @@
         <v>3691</v>
       </c>
       <c r="K107" s="66" t="s">
-        <v>4502</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="108" spans="8:11">
@@ -17555,7 +17571,7 @@
         <v>3692</v>
       </c>
       <c r="K108" s="66" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="109" spans="8:11">
@@ -17569,7 +17585,7 @@
         <v>3694</v>
       </c>
       <c r="K109" s="66" t="s">
-        <v>4504</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="110" spans="8:11">
@@ -17583,7 +17599,7 @@
         <v>3696</v>
       </c>
       <c r="K110" s="66" t="s">
-        <v>4505</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="111" spans="8:11">
@@ -17597,7 +17613,7 @@
         <v>3698</v>
       </c>
       <c r="K111" s="66" t="s">
-        <v>4506</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="112" spans="8:11">
@@ -17611,7 +17627,7 @@
         <v>3700</v>
       </c>
       <c r="K112" s="66" t="s">
-        <v>4507</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="113" spans="8:11">
@@ -17625,7 +17641,7 @@
         <v>3702</v>
       </c>
       <c r="K113" s="66" t="s">
-        <v>4508</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="114" spans="8:11">
@@ -17639,7 +17655,7 @@
         <v>3704</v>
       </c>
       <c r="K114" s="66" t="s">
-        <v>4509</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="115" spans="8:11">
@@ -17653,7 +17669,7 @@
         <v>3705</v>
       </c>
       <c r="K115" s="66" t="s">
-        <v>4510</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="116" spans="8:11">
@@ -17667,7 +17683,7 @@
         <v>3706</v>
       </c>
       <c r="K116" s="66" t="s">
-        <v>4511</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="117" spans="8:11">
@@ -17681,7 +17697,7 @@
         <v>3707</v>
       </c>
       <c r="K117" s="66" t="s">
-        <v>4512</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="118" spans="8:11">
@@ -17695,7 +17711,7 @@
         <v>3708</v>
       </c>
       <c r="K118" s="66" t="s">
-        <v>4513</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="119" spans="8:11">
@@ -17709,7 +17725,7 @@
         <v>3710</v>
       </c>
       <c r="K119" s="66" t="s">
-        <v>4514</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="120" spans="8:11">
@@ -17723,7 +17739,7 @@
         <v>3710</v>
       </c>
       <c r="K120" s="66" t="s">
-        <v>4514</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="121" spans="8:11">
@@ -17737,7 +17753,7 @@
         <v>3712</v>
       </c>
       <c r="K121" s="66" t="s">
-        <v>4515</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="122" spans="8:11">
@@ -17751,7 +17767,7 @@
         <v>3714</v>
       </c>
       <c r="K122" s="66" t="s">
-        <v>4516</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="123" spans="8:11">
@@ -17765,7 +17781,7 @@
         <v>3716</v>
       </c>
       <c r="K123" s="66" t="s">
-        <v>4517</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="124" spans="8:11">
@@ -17779,7 +17795,7 @@
         <v>3718</v>
       </c>
       <c r="K124" s="66" t="s">
-        <v>4518</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="125" spans="8:11">
@@ -17793,7 +17809,7 @@
         <v>3720</v>
       </c>
       <c r="K125" s="66" t="s">
-        <v>4519</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="126" spans="8:11">
@@ -17807,7 +17823,7 @@
         <v>3722</v>
       </c>
       <c r="K126" s="66" t="s">
-        <v>4520</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="127" spans="8:11">
@@ -17821,7 +17837,7 @@
         <v>3723</v>
       </c>
       <c r="K127" s="66" t="s">
-        <v>4521</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="128" spans="8:11">
@@ -17835,7 +17851,7 @@
         <v>3723</v>
       </c>
       <c r="K128" s="66" t="s">
-        <v>4521</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="129" spans="8:11">
@@ -17849,7 +17865,7 @@
         <v>3724</v>
       </c>
       <c r="K129" s="66" t="s">
-        <v>4522</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="130" spans="8:11">
@@ -17863,7 +17879,7 @@
         <v>3725</v>
       </c>
       <c r="K130" s="66" t="s">
-        <v>4523</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="131" spans="8:11">
@@ -17877,7 +17893,7 @@
         <v>3727</v>
       </c>
       <c r="K131" s="66" t="s">
-        <v>4524</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="132" spans="8:11">
@@ -17891,7 +17907,7 @@
         <v>3729</v>
       </c>
       <c r="K132" s="66" t="s">
-        <v>4525</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="133" spans="8:11">
@@ -17905,7 +17921,7 @@
         <v>3731</v>
       </c>
       <c r="K133" s="66" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="134" spans="8:11">
@@ -17919,7 +17935,7 @@
         <v>3733</v>
       </c>
       <c r="K134" s="66" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="135" spans="8:11">
@@ -17933,7 +17949,7 @@
         <v>3735</v>
       </c>
       <c r="K135" s="66" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="136" spans="8:11">
@@ -17947,7 +17963,7 @@
         <v>3737</v>
       </c>
       <c r="K136" s="66" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="137" spans="8:11">
@@ -17961,7 +17977,7 @@
         <v>3739</v>
       </c>
       <c r="K137" s="66" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="138" spans="8:11">
@@ -17975,7 +17991,7 @@
         <v>3741</v>
       </c>
       <c r="K138" s="66" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="139" spans="8:11">
@@ -17983,13 +17999,13 @@
         <v>3742</v>
       </c>
       <c r="I139" s="66" t="s">
-        <v>4529</v>
+        <v>4527</v>
       </c>
       <c r="J139" s="66" t="s">
         <v>3743</v>
       </c>
       <c r="K139" s="66" t="s">
-        <v>4535</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="140" spans="8:11">
@@ -17997,13 +18013,13 @@
         <v>3744</v>
       </c>
       <c r="I140" s="66" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="J140" s="66" t="s">
         <v>3745</v>
       </c>
       <c r="K140" s="66" t="s">
-        <v>4536</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="141" spans="8:11">
@@ -18011,13 +18027,13 @@
         <v>3746</v>
       </c>
       <c r="I141" s="66" t="s">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="J141" s="66" t="s">
         <v>3747</v>
       </c>
       <c r="K141" s="66" t="s">
-        <v>4537</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="142" spans="8:11">
@@ -18025,13 +18041,13 @@
         <v>3748</v>
       </c>
       <c r="I142" s="66" t="s">
-        <v>4532</v>
+        <v>4530</v>
       </c>
       <c r="J142" s="66" t="s">
         <v>3749</v>
       </c>
       <c r="K142" s="66" t="s">
-        <v>4538</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="143" spans="8:11">
@@ -18039,13 +18055,13 @@
         <v>3750</v>
       </c>
       <c r="I143" s="66" t="s">
-        <v>4533</v>
+        <v>4531</v>
       </c>
       <c r="J143" s="66" t="s">
         <v>3751</v>
       </c>
       <c r="K143" s="66" t="s">
-        <v>4539</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="144" spans="8:11">
@@ -18053,13 +18069,13 @@
         <v>3752</v>
       </c>
       <c r="I144" s="66" t="s">
-        <v>4527</v>
+        <v>4525</v>
       </c>
       <c r="J144" s="66" t="s">
         <v>3753</v>
       </c>
       <c r="K144" s="66" t="s">
-        <v>4540</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="145" spans="8:11">
@@ -18067,13 +18083,13 @@
         <v>3726</v>
       </c>
       <c r="I145" s="66" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="J145" s="66" t="s">
         <v>3727</v>
       </c>
       <c r="K145" s="66" t="s">
-        <v>4524</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="146" spans="8:11">
@@ -18081,13 +18097,13 @@
         <v>3754</v>
       </c>
       <c r="I146" s="66" t="s">
-        <v>4541</v>
+        <v>4539</v>
       </c>
       <c r="J146" s="66" t="s">
         <v>3755</v>
       </c>
       <c r="K146" s="66" t="s">
-        <v>4542</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="147" spans="8:11">
@@ -18101,7 +18117,7 @@
         <v>3757</v>
       </c>
       <c r="K147" s="66" t="s">
-        <v>4543</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="148" spans="8:11">
@@ -18115,7 +18131,7 @@
         <v>3759</v>
       </c>
       <c r="K148" s="66" t="s">
-        <v>4545</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="149" spans="8:11">
@@ -18129,7 +18145,7 @@
         <v>3761</v>
       </c>
       <c r="K149" s="66" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="150" spans="8:11">
@@ -18143,7 +18159,7 @@
         <v>3763</v>
       </c>
       <c r="K150" s="66" t="s">
-        <v>4546</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="151" spans="8:11">
@@ -18157,7 +18173,7 @@
         <v>3765</v>
       </c>
       <c r="K151" s="66" t="s">
-        <v>4547</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="152" spans="8:11">
@@ -18171,7 +18187,7 @@
         <v>3767</v>
       </c>
       <c r="K152" s="66" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="153" spans="8:11">
@@ -18185,7 +18201,7 @@
         <v>3769</v>
       </c>
       <c r="K153" s="66" t="s">
-        <v>4549</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="154" spans="8:11">
@@ -18199,7 +18215,7 @@
         <v>3771</v>
       </c>
       <c r="K154" s="66" t="s">
-        <v>4550</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="155" spans="8:11">
@@ -18213,7 +18229,7 @@
         <v>3773</v>
       </c>
       <c r="K155" s="66" t="s">
-        <v>4551</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="156" spans="8:11">
@@ -18227,7 +18243,7 @@
         <v>3775</v>
       </c>
       <c r="K156" s="66" t="s">
-        <v>4552</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="157" spans="8:11">
@@ -18241,7 +18257,7 @@
         <v>3777</v>
       </c>
       <c r="K157" s="66" t="s">
-        <v>4553</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="158" spans="8:11">
@@ -18255,7 +18271,7 @@
         <v>3778</v>
       </c>
       <c r="K158" s="66" t="s">
-        <v>4554</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="159" spans="8:11">
@@ -18269,7 +18285,7 @@
         <v>3780</v>
       </c>
       <c r="K159" s="66" t="s">
-        <v>4555</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="160" spans="8:11">
@@ -18283,7 +18299,7 @@
         <v>3782</v>
       </c>
       <c r="K160" s="66" t="s">
-        <v>4556</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="161" spans="8:11">
@@ -18297,7 +18313,7 @@
         <v>3784</v>
       </c>
       <c r="K161" s="66" t="s">
-        <v>4557</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="162" spans="8:11">
@@ -18311,7 +18327,7 @@
         <v>3786</v>
       </c>
       <c r="K162" s="66" t="s">
-        <v>4556</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="163" spans="8:11">
@@ -18325,7 +18341,7 @@
         <v>3787</v>
       </c>
       <c r="K163" s="66" t="s">
-        <v>4560</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="164" spans="8:11">
@@ -18339,7 +18355,7 @@
         <v>3789</v>
       </c>
       <c r="K164" s="66" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="165" spans="8:11">
@@ -18353,7 +18369,7 @@
         <v>3789</v>
       </c>
       <c r="K165" s="66" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="166" spans="8:11">
@@ -18367,7 +18383,7 @@
         <v>3789</v>
       </c>
       <c r="K166" s="66" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="167" spans="8:11">
@@ -18381,7 +18397,7 @@
         <v>3789</v>
       </c>
       <c r="K167" s="66" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="168" spans="8:11">
@@ -18395,7 +18411,7 @@
         <v>3789</v>
       </c>
       <c r="K168" s="66" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="169" spans="8:11">
@@ -18409,7 +18425,7 @@
         <v>3791</v>
       </c>
       <c r="K169" s="66" t="s">
-        <v>4562</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="170" spans="8:11">
@@ -18417,13 +18433,13 @@
         <v>3792</v>
       </c>
       <c r="I170" s="66" t="s">
-        <v>4563</v>
+        <v>4560</v>
       </c>
       <c r="J170" s="66" t="s">
         <v>3793</v>
       </c>
       <c r="K170" s="66" t="s">
-        <v>4564</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="171" spans="8:11">
@@ -18437,7 +18453,7 @@
         <v>3795</v>
       </c>
       <c r="K171" s="66" t="s">
-        <v>4569</v>
+        <v>4566</v>
       </c>
     </row>
     <row r="172" spans="8:11">
@@ -18451,7 +18467,7 @@
         <v>3797</v>
       </c>
       <c r="K172" s="66" t="s">
-        <v>4568</v>
+        <v>4565</v>
       </c>
     </row>
     <row r="173" spans="8:11">
@@ -18465,7 +18481,7 @@
         <v>3799</v>
       </c>
       <c r="K173" s="66" t="s">
-        <v>4567</v>
+        <v>4564</v>
       </c>
     </row>
     <row r="174" spans="8:11">
@@ -18479,7 +18495,7 @@
         <v>3801</v>
       </c>
       <c r="K174" s="66" t="s">
-        <v>4566</v>
+        <v>4563</v>
       </c>
     </row>
     <row r="175" spans="8:11">
@@ -18493,7 +18509,7 @@
         <v>3803</v>
       </c>
       <c r="K175" s="66" t="s">
-        <v>4565</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="176" spans="8:11">
@@ -18507,7 +18523,7 @@
         <v>3805</v>
       </c>
       <c r="K176" s="66" t="s">
-        <v>4575</v>
+        <v>4572</v>
       </c>
     </row>
     <row r="177" spans="8:11">
@@ -18521,7 +18537,7 @@
         <v>3807</v>
       </c>
       <c r="K177" s="66" t="s">
-        <v>4570</v>
+        <v>4567</v>
       </c>
     </row>
     <row r="178" spans="8:11">
@@ -18535,7 +18551,7 @@
         <v>3809</v>
       </c>
       <c r="K178" s="66" t="s">
-        <v>4571</v>
+        <v>4568</v>
       </c>
     </row>
     <row r="179" spans="8:11">
@@ -18549,7 +18565,7 @@
         <v>3795</v>
       </c>
       <c r="K179" s="66" t="s">
-        <v>4569</v>
+        <v>4566</v>
       </c>
     </row>
     <row r="180" spans="8:11">
@@ -18563,7 +18579,7 @@
         <v>3803</v>
       </c>
       <c r="K180" s="66" t="s">
-        <v>4565</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="181" spans="8:11">
@@ -18577,7 +18593,7 @@
         <v>3807</v>
       </c>
       <c r="K181" s="66" t="s">
-        <v>4570</v>
+        <v>4567</v>
       </c>
     </row>
     <row r="182" spans="8:11">
@@ -18591,7 +18607,7 @@
         <v>3809</v>
       </c>
       <c r="K182" s="66" t="s">
-        <v>4571</v>
+        <v>4568</v>
       </c>
     </row>
     <row r="183" spans="8:11">
@@ -18605,7 +18621,7 @@
         <v>3811</v>
       </c>
       <c r="K183" s="66" t="s">
-        <v>4572</v>
+        <v>4569</v>
       </c>
     </row>
     <row r="184" spans="8:11">
@@ -18613,13 +18629,13 @@
         <v>3812</v>
       </c>
       <c r="I184" s="66" t="s">
-        <v>4573</v>
+        <v>4570</v>
       </c>
       <c r="J184" s="66" t="s">
         <v>3813</v>
       </c>
       <c r="K184" s="66" t="s">
-        <v>4574</v>
+        <v>4571</v>
       </c>
     </row>
     <row r="185" spans="8:11">
@@ -18629,7 +18645,7 @@
         <v>3813</v>
       </c>
       <c r="K185" s="66" t="s">
-        <v>4574</v>
+        <v>4571</v>
       </c>
     </row>
     <row r="186" spans="8:11">
@@ -18683,7 +18699,7 @@
         <v>3818</v>
       </c>
       <c r="K190" s="66" t="s">
-        <v>4576</v>
+        <v>4573</v>
       </c>
     </row>
     <row r="191" spans="8:11">
@@ -18697,7 +18713,7 @@
         <v>3820</v>
       </c>
       <c r="K191" s="66" t="s">
-        <v>4577</v>
+        <v>4574</v>
       </c>
     </row>
     <row r="192" spans="8:11">
@@ -18801,7 +18817,7 @@
         <v>3828</v>
       </c>
       <c r="K199" s="66" t="s">
-        <v>4791</v>
+        <v>4788</v>
       </c>
     </row>
     <row r="200" spans="8:11">
@@ -18815,7 +18831,7 @@
         <v>3828</v>
       </c>
       <c r="K200" s="66" t="s">
-        <v>4791</v>
+        <v>4788</v>
       </c>
     </row>
     <row r="201" spans="8:11">
@@ -18871,7 +18887,7 @@
         <v>3833</v>
       </c>
       <c r="K204" s="66" t="s">
-        <v>4792</v>
+        <v>4789</v>
       </c>
     </row>
     <row r="205" spans="8:11">
@@ -18885,7 +18901,7 @@
         <v>3835</v>
       </c>
       <c r="K205" s="66" t="s">
-        <v>4793</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="206" spans="8:11">
@@ -18899,7 +18915,7 @@
         <v>3835</v>
       </c>
       <c r="K206" s="66" t="s">
-        <v>4793</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="207" spans="8:11">
@@ -18913,7 +18929,7 @@
         <v>3835</v>
       </c>
       <c r="K207" s="66" t="s">
-        <v>4793</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="208" spans="8:11">
@@ -18927,7 +18943,7 @@
         <v>3838</v>
       </c>
       <c r="K208" s="66" t="s">
-        <v>4794</v>
+        <v>4791</v>
       </c>
     </row>
     <row r="209" spans="8:11">
@@ -18941,7 +18957,7 @@
         <v>3840</v>
       </c>
       <c r="K209" s="66" t="s">
-        <v>4795</v>
+        <v>4792</v>
       </c>
     </row>
     <row r="210" spans="8:11">
@@ -18955,7 +18971,7 @@
         <v>3840</v>
       </c>
       <c r="K210" s="66" t="s">
-        <v>4795</v>
+        <v>4792</v>
       </c>
     </row>
     <row r="211" spans="8:11">
@@ -19509,7 +19525,7 @@
       </c>
       <c r="J264" s="66"/>
       <c r="K264" s="66" t="s">
-        <v>4498</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="265" spans="8:11">
@@ -19839,7 +19855,7 @@
         <v>3942</v>
       </c>
       <c r="I288" s="66" t="s">
-        <v>4534</v>
+        <v>4532</v>
       </c>
       <c r="J288" s="66" t="s">
         <v>3943</v>
@@ -23968,7 +23984,7 @@
         <v>1900</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>4479</v>
+        <v>4478</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>790</v>
@@ -28219,8 +28235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B396"/>
   <sheetViews>
-    <sheetView topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="C340" sqref="C340"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="G395" sqref="G395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.6"/>
@@ -29739,7 +29755,7 @@
         <v>1393</v>
       </c>
       <c r="B240" s="31" t="s">
-        <v>4472</v>
+        <v>4471</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -29768,23 +29784,23 @@
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="53" t="s">
-        <v>4473</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="53" t="s">
-        <v>4475</v>
+        <v>4474</v>
       </c>
       <c r="B248" s="31" t="s">
-        <v>4477</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="31" t="s">
-        <v>4474</v>
+        <v>4473</v>
       </c>
       <c r="B249" s="31" t="s">
-        <v>4476</v>
+        <v>4475</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -29885,7 +29901,7 @@
         <v>4321</v>
       </c>
       <c r="B267" s="31" t="s">
-        <v>4478</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -30357,304 +30373,424 @@
         <v>4377</v>
       </c>
     </row>
-    <row r="337" spans="1:1">
+    <row r="337" spans="1:2">
       <c r="A337" s="68" t="s">
+        <v>4754</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" s="68" t="s">
+        <v>4755</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
+      <c r="A339" s="68" t="s">
+        <v>4756</v>
+      </c>
+      <c r="B339" s="31" t="s">
+        <v>4794</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
+      <c r="A340" s="68" t="s">
         <v>4757</v>
       </c>
-    </row>
-    <row r="338" spans="1:1">
-      <c r="A338" s="68" t="s">
-        <v>4758</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1">
-      <c r="A339" s="68" t="s">
-        <v>4759</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1">
-      <c r="A340" s="68" t="s">
-        <v>4760</v>
-      </c>
-    </row>
-    <row r="341" spans="1:1">
+      <c r="B340" s="31" t="s">
+        <v>4793</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2">
       <c r="A341" s="68" t="s">
         <v>1372</v>
       </c>
     </row>
-    <row r="342" spans="1:1">
+    <row r="342" spans="1:2">
       <c r="A342" s="68" t="s">
-        <v>4761</v>
-      </c>
-    </row>
-    <row r="343" spans="1:1">
+        <v>4758</v>
+      </c>
+      <c r="B342" s="31" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
       <c r="A343" s="68" t="s">
-        <v>4762</v>
-      </c>
-    </row>
-    <row r="344" spans="1:1">
+        <v>4759</v>
+      </c>
+      <c r="B343" s="31" t="s">
+        <v>4795</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
       <c r="A344" s="68" t="s">
         <v>1331</v>
       </c>
     </row>
-    <row r="345" spans="1:1">
+    <row r="345" spans="1:2">
       <c r="A345" s="68" t="s">
-        <v>4763</v>
-      </c>
-    </row>
-    <row r="346" spans="1:1">
+        <v>4760</v>
+      </c>
+      <c r="B345" s="31" t="s">
+        <v>4796</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
       <c r="A346" s="68" t="s">
-        <v>4764</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1">
+        <v>4761</v>
+      </c>
+      <c r="B346" s="31" t="s">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
       <c r="A347" s="68" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="348" spans="1:1">
+    <row r="348" spans="1:2">
       <c r="A348" s="68" t="s">
-        <v>4765</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1">
+        <v>4762</v>
+      </c>
+      <c r="B348" s="31" t="s">
+        <v>4798</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
       <c r="A349" s="68" t="s">
-        <v>4766</v>
-      </c>
-    </row>
-    <row r="350" spans="1:1">
+        <v>4763</v>
+      </c>
+      <c r="B349" s="31" t="s">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2">
       <c r="A350" s="68" t="s">
         <v>1370</v>
       </c>
     </row>
-    <row r="351" spans="1:1">
+    <row r="351" spans="1:2">
       <c r="A351" s="68" t="s">
-        <v>4767</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1">
+        <v>4764</v>
+      </c>
+      <c r="B351" s="66" t="s">
+        <v>4799</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
       <c r="A352" s="68" t="s">
+        <v>4763</v>
+      </c>
+      <c r="B352" s="66" t="s">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" s="68" t="s">
+        <v>4765</v>
+      </c>
+      <c r="B353" s="66" t="s">
+        <v>4801</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="A354" s="68" t="s">
         <v>4766</v>
       </c>
     </row>
-    <row r="353" spans="1:1">
-      <c r="A353" s="68" t="s">
-        <v>4768</v>
-      </c>
-    </row>
-    <row r="354" spans="1:1">
-      <c r="A354" s="68" t="s">
-        <v>4769</v>
-      </c>
-    </row>
-    <row r="355" spans="1:1">
+    <row r="355" spans="1:2">
       <c r="A355" s="68" t="s">
-        <v>4767</v>
-      </c>
-    </row>
-    <row r="356" spans="1:1">
+        <v>4764</v>
+      </c>
+      <c r="B355" s="31" t="s">
+        <v>4799</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
       <c r="A356" s="68" t="s">
-        <v>4766</v>
-      </c>
-    </row>
-    <row r="357" spans="1:1">
+        <v>4763</v>
+      </c>
+      <c r="B356" s="31" t="s">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
       <c r="A357" s="68" t="s">
-        <v>4768</v>
-      </c>
-    </row>
-    <row r="358" spans="1:1">
+        <v>4765</v>
+      </c>
+      <c r="B357" s="31" t="s">
+        <v>4801</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
       <c r="A358" s="68" t="s">
         <v>1386</v>
       </c>
     </row>
-    <row r="359" spans="1:1">
+    <row r="359" spans="1:2">
       <c r="A359" s="68" t="s">
-        <v>4770</v>
-      </c>
-    </row>
-    <row r="360" spans="1:1">
+        <v>4767</v>
+      </c>
+      <c r="B359" s="31" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
       <c r="A360" s="68" t="s">
-        <v>4771</v>
-      </c>
-    </row>
-    <row r="361" spans="1:1">
+        <v>4768</v>
+      </c>
+      <c r="B360" s="31" t="s">
+        <v>4803</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
       <c r="A361" s="68" t="s">
         <v>1391</v>
       </c>
     </row>
-    <row r="362" spans="1:1">
+    <row r="362" spans="1:2">
       <c r="A362" s="68" t="s">
-        <v>4772</v>
-      </c>
-    </row>
-    <row r="363" spans="1:1">
+        <v>4769</v>
+      </c>
+      <c r="B362" s="31" t="s">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
       <c r="A363" s="68" t="s">
-        <v>4773</v>
-      </c>
-    </row>
-    <row r="364" spans="1:1">
+        <v>4770</v>
+      </c>
+      <c r="B363" s="31" t="s">
+        <v>4805</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
       <c r="A364" s="68" t="s">
         <v>1365</v>
       </c>
     </row>
-    <row r="365" spans="1:1">
+    <row r="365" spans="1:2">
       <c r="A365" s="68" t="s">
-        <v>4774</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1">
+        <v>4771</v>
+      </c>
+      <c r="B365" s="31" t="s">
+        <v>4806</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
       <c r="A366" s="68" t="s">
-        <v>4773</v>
-      </c>
-    </row>
-    <row r="367" spans="1:1">
+        <v>4770</v>
+      </c>
+      <c r="B366" s="66" t="s">
+        <v>4805</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
       <c r="A367" s="68" t="s">
         <v>1362</v>
       </c>
     </row>
-    <row r="368" spans="1:1">
+    <row r="368" spans="1:2">
       <c r="A368" s="68" t="s">
-        <v>4775</v>
-      </c>
-    </row>
-    <row r="369" spans="1:1">
+        <v>4772</v>
+      </c>
+      <c r="B368" s="31" t="s">
+        <v>4807</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
       <c r="A369" s="68" t="s">
+        <v>4770</v>
+      </c>
+      <c r="B369" s="66" t="s">
+        <v>4805</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" s="68" t="s">
         <v>4773</v>
       </c>
     </row>
-    <row r="370" spans="1:1">
-      <c r="A370" s="68" t="s">
-        <v>4776</v>
-      </c>
-    </row>
-    <row r="371" spans="1:1">
+    <row r="371" spans="1:2">
       <c r="A371" s="68" t="s">
-        <v>4775</v>
-      </c>
-    </row>
-    <row r="372" spans="1:1">
+        <v>4772</v>
+      </c>
+      <c r="B371" s="66" t="s">
+        <v>4807</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
       <c r="A372" s="68" t="s">
-        <v>4773</v>
-      </c>
-    </row>
-    <row r="373" spans="1:1">
+        <v>4770</v>
+      </c>
+      <c r="B372" s="66" t="s">
+        <v>4805</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
       <c r="A373" s="68" t="s">
         <v>1394</v>
       </c>
     </row>
-    <row r="374" spans="1:1">
+    <row r="374" spans="1:2">
       <c r="A374" s="68" t="s">
-        <v>4777</v>
-      </c>
-    </row>
-    <row r="375" spans="1:1">
+        <v>4774</v>
+      </c>
+      <c r="B374" s="31" t="s">
+        <v>4808</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
       <c r="A375" s="68" t="s">
-        <v>4778</v>
-      </c>
-    </row>
-    <row r="376" spans="1:1">
+        <v>4775</v>
+      </c>
+      <c r="B375" s="31" t="s">
+        <v>4372</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
       <c r="A376" s="68" t="s">
         <v>1390</v>
       </c>
     </row>
-    <row r="377" spans="1:1">
+    <row r="377" spans="1:2">
       <c r="A377" s="68" t="s">
+        <v>4776</v>
+      </c>
+      <c r="B377" s="66" t="s">
+        <v>4808</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" s="68" t="s">
+        <v>4777</v>
+      </c>
+      <c r="B378" s="66" t="s">
+        <v>4372</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" s="68" t="s">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" s="68" t="s">
         <v>4779</v>
       </c>
-    </row>
-    <row r="378" spans="1:1">
-      <c r="A378" s="68" t="s">
+      <c r="B380" s="31" t="s">
+        <v>4810</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" s="68" t="s">
         <v>4780</v>
       </c>
-    </row>
-    <row r="379" spans="1:1">
-      <c r="A379" s="68" t="s">
+      <c r="B381" s="66" t="s">
+        <v>4809</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" s="68" t="s">
         <v>4781</v>
       </c>
     </row>
-    <row r="380" spans="1:1">
-      <c r="A380" s="68" t="s">
+    <row r="383" spans="1:2">
+      <c r="A383" s="68" t="s">
+        <v>4779</v>
+      </c>
+      <c r="B383" s="31" t="s">
+        <v>4810</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" s="68" t="s">
+        <v>4780</v>
+      </c>
+      <c r="B384" s="66" t="s">
+        <v>4809</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2">
+      <c r="A385" s="68" t="s">
         <v>4782</v>
       </c>
     </row>
-    <row r="381" spans="1:1">
-      <c r="A381" s="68" t="s">
+    <row r="386" spans="1:2">
+      <c r="A386" s="68" t="s">
         <v>4783</v>
       </c>
-    </row>
-    <row r="382" spans="1:1">
-      <c r="A382" s="68" t="s">
+      <c r="B386" s="66" t="s">
+        <v>4812</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" s="68" t="s">
         <v>4784</v>
       </c>
-    </row>
-    <row r="383" spans="1:1">
-      <c r="A383" s="68" t="s">
-        <v>4782</v>
-      </c>
-    </row>
-    <row r="384" spans="1:1">
-      <c r="A384" s="68" t="s">
-        <v>4783</v>
-      </c>
-    </row>
-    <row r="385" spans="1:1">
-      <c r="A385" s="68" t="s">
-        <v>4785</v>
-      </c>
-    </row>
-    <row r="386" spans="1:1">
-      <c r="A386" s="68" t="s">
-        <v>4786</v>
-      </c>
-    </row>
-    <row r="387" spans="1:1">
-      <c r="A387" s="68" t="s">
-        <v>4787</v>
-      </c>
-    </row>
-    <row r="388" spans="1:1">
+      <c r="B387" s="66" t="s">
+        <v>4811</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
       <c r="A388" s="68" t="s">
         <v>1352</v>
       </c>
     </row>
-    <row r="389" spans="1:1">
+    <row r="389" spans="1:2">
       <c r="A389" s="68" t="s">
-        <v>4786</v>
-      </c>
-    </row>
-    <row r="390" spans="1:1">
+        <v>4783</v>
+      </c>
+      <c r="B389" s="31" t="s">
+        <v>4812</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
       <c r="A390" s="68" t="s">
-        <v>4787</v>
-      </c>
-    </row>
-    <row r="391" spans="1:1">
+        <v>4784</v>
+      </c>
+      <c r="B390" s="31" t="s">
+        <v>4811</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
       <c r="A391" s="68" t="s">
         <v>1379</v>
       </c>
     </row>
-    <row r="392" spans="1:1">
+    <row r="392" spans="1:2">
       <c r="A392" s="68" t="s">
-        <v>4788</v>
-      </c>
-    </row>
-    <row r="393" spans="1:1">
+        <v>4785</v>
+      </c>
+      <c r="B392" s="31" t="s">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
       <c r="A393" s="68" t="s">
-        <v>4789</v>
-      </c>
-    </row>
-    <row r="394" spans="1:1">
+        <v>4786</v>
+      </c>
+      <c r="B393" s="31" t="s">
+        <v>4364</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
       <c r="A394" s="68" t="s">
-        <v>4790</v>
-      </c>
-    </row>
-    <row r="395" spans="1:1">
+        <v>4787</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
       <c r="A395" s="68" t="s">
-        <v>4788</v>
-      </c>
-    </row>
-    <row r="396" spans="1:1">
+        <v>4785</v>
+      </c>
+      <c r="B395" s="66" t="s">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
       <c r="A396" s="68" t="s">
-        <v>4789</v>
+        <v>4786</v>
+      </c>
+      <c r="B396" s="66" t="s">
+        <v>4364</v>
       </c>
     </row>
   </sheetData>
@@ -32433,7 +32569,7 @@
         <v>2180</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>4756</v>
+        <v>4753</v>
       </c>
       <c r="G38" s="14" t="s">
         <v>77</v>
@@ -35188,7 +35324,7 @@
         <v>3648</v>
       </c>
       <c r="D79" s="31" t="s">
-        <v>4482</v>
+        <v>4480</v>
       </c>
       <c r="E79" s="31"/>
       <c r="F79" s="31"/>
@@ -35204,7 +35340,7 @@
         <v>3650</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>4483</v>
+        <v>4481</v>
       </c>
       <c r="E80" s="31"/>
       <c r="F80" s="31"/>
@@ -35220,7 +35356,7 @@
         <v>3652</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>4484</v>
+        <v>4482</v>
       </c>
       <c r="E81" s="31"/>
       <c r="F81" s="31"/>
@@ -35236,7 +35372,7 @@
         <v>3654</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>4485</v>
+        <v>4483</v>
       </c>
       <c r="E82" s="31"/>
       <c r="F82" s="31"/>
@@ -35252,7 +35388,7 @@
         <v>3656</v>
       </c>
       <c r="D83" s="31" t="s">
-        <v>4486</v>
+        <v>4484</v>
       </c>
       <c r="E83" s="31"/>
       <c r="F83" s="31"/>
@@ -35268,7 +35404,7 @@
         <v>3658</v>
       </c>
       <c r="D84" s="31" t="s">
-        <v>4487</v>
+        <v>4485</v>
       </c>
       <c r="E84" s="31"/>
       <c r="F84" s="31"/>
@@ -35284,7 +35420,7 @@
         <v>3660</v>
       </c>
       <c r="D85" s="31" t="s">
-        <v>4488</v>
+        <v>4486</v>
       </c>
       <c r="E85" s="31"/>
       <c r="F85" s="31"/>
@@ -35300,7 +35436,7 @@
         <v>3661</v>
       </c>
       <c r="D86" s="31" t="s">
-        <v>4489</v>
+        <v>4487</v>
       </c>
       <c r="E86" s="31"/>
       <c r="F86" s="31"/>
@@ -35460,7 +35596,7 @@
         <v>3673</v>
       </c>
       <c r="D96" s="31" t="s">
-        <v>4490</v>
+        <v>4488</v>
       </c>
       <c r="E96" s="31"/>
       <c r="F96" s="31"/>
@@ -35476,7 +35612,7 @@
         <v>3674</v>
       </c>
       <c r="D97" s="31" t="s">
-        <v>4493</v>
+        <v>4491</v>
       </c>
       <c r="E97" s="31"/>
       <c r="F97" s="31"/>
@@ -35486,13 +35622,13 @@
         <v>3513</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>4492</v>
+        <v>4490</v>
       </c>
       <c r="C98" s="31" t="s">
         <v>3675</v>
       </c>
       <c r="D98" s="31" t="s">
-        <v>4491</v>
+        <v>4489</v>
       </c>
       <c r="E98" s="31"/>
       <c r="F98" s="31"/>
@@ -35508,7 +35644,7 @@
         <v>3677</v>
       </c>
       <c r="D99" s="31" t="s">
-        <v>4494</v>
+        <v>4492</v>
       </c>
       <c r="E99" s="31"/>
       <c r="F99" s="31"/>
@@ -35524,7 +35660,7 @@
         <v>3679</v>
       </c>
       <c r="D100" s="31" t="s">
-        <v>4495</v>
+        <v>4493</v>
       </c>
       <c r="E100" s="31"/>
       <c r="F100" s="31"/>
@@ -35540,7 +35676,7 @@
         <v>3681</v>
       </c>
       <c r="D101" s="31" t="s">
-        <v>4496</v>
+        <v>4494</v>
       </c>
       <c r="E101" s="31"/>
       <c r="F101" s="31"/>
@@ -35556,7 +35692,7 @@
         <v>3683</v>
       </c>
       <c r="D102" s="31" t="s">
-        <v>4497</v>
+        <v>4495</v>
       </c>
       <c r="E102" s="31"/>
       <c r="F102" s="31"/>
@@ -35572,7 +35708,7 @@
         <v>3685</v>
       </c>
       <c r="D103" s="31" t="s">
-        <v>4499</v>
+        <v>4497</v>
       </c>
       <c r="E103" s="31"/>
       <c r="F103" s="31"/>
@@ -35588,7 +35724,7 @@
         <v>3687</v>
       </c>
       <c r="D104" s="31" t="s">
-        <v>4500</v>
+        <v>4498</v>
       </c>
       <c r="E104" s="31"/>
       <c r="F104" s="31"/>
@@ -35604,7 +35740,7 @@
         <v>3689</v>
       </c>
       <c r="D105" s="31" t="s">
-        <v>4501</v>
+        <v>4499</v>
       </c>
       <c r="E105" s="31"/>
       <c r="F105" s="31"/>
@@ -35620,7 +35756,7 @@
         <v>3691</v>
       </c>
       <c r="D106" s="31" t="s">
-        <v>4502</v>
+        <v>4500</v>
       </c>
       <c r="E106" s="31"/>
       <c r="F106" s="31"/>
@@ -35636,7 +35772,7 @@
         <v>3692</v>
       </c>
       <c r="D107" s="31" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="E107" s="31"/>
       <c r="F107" s="31"/>
@@ -35652,7 +35788,7 @@
         <v>3694</v>
       </c>
       <c r="D108" s="31" t="s">
-        <v>4504</v>
+        <v>4502</v>
       </c>
       <c r="E108" s="31"/>
       <c r="F108" s="31"/>
@@ -35668,7 +35804,7 @@
         <v>3696</v>
       </c>
       <c r="D109" s="31" t="s">
-        <v>4505</v>
+        <v>4503</v>
       </c>
       <c r="E109" s="31"/>
       <c r="F109" s="31"/>
@@ -35684,7 +35820,7 @@
         <v>3698</v>
       </c>
       <c r="D110" s="31" t="s">
-        <v>4506</v>
+        <v>4504</v>
       </c>
       <c r="E110" s="31"/>
       <c r="F110" s="31"/>
@@ -35700,7 +35836,7 @@
         <v>3700</v>
       </c>
       <c r="D111" s="31" t="s">
-        <v>4507</v>
+        <v>4505</v>
       </c>
       <c r="E111" s="31"/>
       <c r="F111" s="31"/>
@@ -35716,7 +35852,7 @@
         <v>3702</v>
       </c>
       <c r="D112" s="31" t="s">
-        <v>4508</v>
+        <v>4506</v>
       </c>
       <c r="E112" s="31"/>
       <c r="F112" s="31"/>
@@ -35732,7 +35868,7 @@
         <v>3704</v>
       </c>
       <c r="D113" s="31" t="s">
-        <v>4509</v>
+        <v>4507</v>
       </c>
       <c r="E113" s="31"/>
       <c r="F113" s="31"/>
@@ -35748,7 +35884,7 @@
         <v>3705</v>
       </c>
       <c r="D114" s="31" t="s">
-        <v>4510</v>
+        <v>4508</v>
       </c>
       <c r="E114" s="31"/>
       <c r="F114" s="31"/>
@@ -35764,7 +35900,7 @@
         <v>3706</v>
       </c>
       <c r="D115" s="31" t="s">
-        <v>4511</v>
+        <v>4509</v>
       </c>
       <c r="E115" s="31"/>
       <c r="F115" s="31"/>
@@ -35780,7 +35916,7 @@
         <v>3707</v>
       </c>
       <c r="D116" s="31" t="s">
-        <v>4512</v>
+        <v>4510</v>
       </c>
       <c r="E116" s="31"/>
       <c r="F116" s="31"/>
@@ -35796,7 +35932,7 @@
         <v>3708</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>4513</v>
+        <v>4511</v>
       </c>
       <c r="E117" s="31"/>
       <c r="F117" s="31"/>
@@ -35812,7 +35948,7 @@
         <v>3710</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>4514</v>
+        <v>4512</v>
       </c>
       <c r="E118" s="31"/>
       <c r="F118" s="31"/>
@@ -35828,7 +35964,7 @@
         <v>3710</v>
       </c>
       <c r="D119" s="31" t="s">
-        <v>4514</v>
+        <v>4512</v>
       </c>
       <c r="E119" s="31"/>
       <c r="F119" s="31"/>
@@ -35844,7 +35980,7 @@
         <v>3712</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>4515</v>
+        <v>4513</v>
       </c>
       <c r="E120" s="31"/>
       <c r="F120" s="31"/>
@@ -35860,7 +35996,7 @@
         <v>3714</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>4516</v>
+        <v>4514</v>
       </c>
       <c r="E121" s="31"/>
       <c r="F121" s="31"/>
@@ -35876,7 +36012,7 @@
         <v>3716</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>4517</v>
+        <v>4515</v>
       </c>
       <c r="E122" s="31"/>
       <c r="F122" s="31"/>
@@ -35892,7 +36028,7 @@
         <v>3718</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>4518</v>
+        <v>4516</v>
       </c>
       <c r="E123" s="31"/>
       <c r="F123" s="31"/>
@@ -35908,7 +36044,7 @@
         <v>3720</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>4519</v>
+        <v>4517</v>
       </c>
       <c r="E124" s="31"/>
       <c r="F124" s="31"/>
@@ -35924,7 +36060,7 @@
         <v>3722</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>4520</v>
+        <v>4518</v>
       </c>
       <c r="E125" s="31"/>
       <c r="F125" s="31"/>
@@ -35940,7 +36076,7 @@
         <v>3723</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>4521</v>
+        <v>4519</v>
       </c>
       <c r="E126" s="31"/>
       <c r="F126" s="31"/>
@@ -35956,7 +36092,7 @@
         <v>3723</v>
       </c>
       <c r="D127" s="31" t="s">
-        <v>4521</v>
+        <v>4519</v>
       </c>
       <c r="E127" s="31"/>
       <c r="F127" s="31"/>
@@ -35972,7 +36108,7 @@
         <v>3724</v>
       </c>
       <c r="D128" s="31" t="s">
-        <v>4522</v>
+        <v>4520</v>
       </c>
       <c r="E128" s="31"/>
       <c r="F128" s="31"/>
@@ -35988,7 +36124,7 @@
         <v>3725</v>
       </c>
       <c r="D129" s="31" t="s">
-        <v>4523</v>
+        <v>4521</v>
       </c>
       <c r="E129" s="31"/>
       <c r="F129" s="31"/>
@@ -36004,7 +36140,7 @@
         <v>3727</v>
       </c>
       <c r="D130" s="31" t="s">
-        <v>4524</v>
+        <v>4522</v>
       </c>
       <c r="E130" s="31"/>
       <c r="F130" s="31"/>
@@ -36020,7 +36156,7 @@
         <v>3729</v>
       </c>
       <c r="D131" s="31" t="s">
-        <v>4525</v>
+        <v>4523</v>
       </c>
       <c r="E131" s="31"/>
       <c r="F131" s="31"/>
@@ -36036,7 +36172,7 @@
         <v>3731</v>
       </c>
       <c r="D132" s="31" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
       <c r="E132" s="31"/>
       <c r="F132" s="31"/>
@@ -36052,7 +36188,7 @@
         <v>3733</v>
       </c>
       <c r="D133" s="31" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
       <c r="E133" s="31"/>
       <c r="F133" s="31"/>
@@ -36068,7 +36204,7 @@
         <v>3735</v>
       </c>
       <c r="D134" s="31" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
       <c r="E134" s="31"/>
       <c r="F134" s="31"/>
@@ -36084,7 +36220,7 @@
         <v>3737</v>
       </c>
       <c r="D135" s="31" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
       <c r="E135" s="31"/>
       <c r="F135" s="31"/>
@@ -36100,7 +36236,7 @@
         <v>3739</v>
       </c>
       <c r="D136" s="31" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
       <c r="E136" s="31"/>
       <c r="F136" s="31"/>
@@ -36116,7 +36252,7 @@
         <v>3741</v>
       </c>
       <c r="D137" s="31" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
       <c r="E137" s="31"/>
       <c r="F137" s="31"/>
@@ -36126,13 +36262,13 @@
         <v>3742</v>
       </c>
       <c r="B138" s="31" t="s">
-        <v>4529</v>
+        <v>4527</v>
       </c>
       <c r="C138" s="31" t="s">
         <v>3743</v>
       </c>
       <c r="D138" s="31" t="s">
-        <v>4535</v>
+        <v>4533</v>
       </c>
       <c r="E138" s="31"/>
       <c r="F138" s="31"/>
@@ -36142,13 +36278,13 @@
         <v>3744</v>
       </c>
       <c r="B139" s="31" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="C139" s="31" t="s">
         <v>3745</v>
       </c>
       <c r="D139" s="31" t="s">
-        <v>4536</v>
+        <v>4534</v>
       </c>
       <c r="E139" s="31"/>
       <c r="F139" s="31"/>
@@ -36158,13 +36294,13 @@
         <v>3746</v>
       </c>
       <c r="B140" s="31" t="s">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="C140" s="31" t="s">
         <v>3747</v>
       </c>
       <c r="D140" s="31" t="s">
-        <v>4537</v>
+        <v>4535</v>
       </c>
       <c r="E140" s="31"/>
       <c r="F140" s="31"/>
@@ -36174,13 +36310,13 @@
         <v>3748</v>
       </c>
       <c r="B141" s="31" t="s">
-        <v>4532</v>
+        <v>4530</v>
       </c>
       <c r="C141" s="31" t="s">
         <v>3749</v>
       </c>
       <c r="D141" s="31" t="s">
-        <v>4538</v>
+        <v>4536</v>
       </c>
       <c r="E141" s="31"/>
       <c r="F141" s="31"/>
@@ -36190,13 +36326,13 @@
         <v>3750</v>
       </c>
       <c r="B142" s="31" t="s">
-        <v>4533</v>
+        <v>4531</v>
       </c>
       <c r="C142" s="31" t="s">
         <v>3751</v>
       </c>
       <c r="D142" s="31" t="s">
-        <v>4539</v>
+        <v>4537</v>
       </c>
       <c r="E142" s="31"/>
       <c r="F142" s="31"/>
@@ -36206,13 +36342,13 @@
         <v>3752</v>
       </c>
       <c r="B143" s="31" t="s">
-        <v>4527</v>
+        <v>4525</v>
       </c>
       <c r="C143" s="31" t="s">
         <v>3753</v>
       </c>
       <c r="D143" s="31" t="s">
-        <v>4540</v>
+        <v>4538</v>
       </c>
       <c r="E143" s="31"/>
       <c r="F143" s="31"/>
@@ -36222,13 +36358,13 @@
         <v>3726</v>
       </c>
       <c r="B144" s="31" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="C144" s="31" t="s">
         <v>3727</v>
       </c>
       <c r="D144" s="31" t="s">
-        <v>4524</v>
+        <v>4522</v>
       </c>
       <c r="E144" s="31"/>
       <c r="F144" s="31"/>
@@ -36238,13 +36374,13 @@
         <v>3754</v>
       </c>
       <c r="B145" s="31" t="s">
-        <v>4541</v>
+        <v>4539</v>
       </c>
       <c r="C145" s="31" t="s">
         <v>3755</v>
       </c>
       <c r="D145" s="31" t="s">
-        <v>4542</v>
+        <v>4540</v>
       </c>
       <c r="E145" s="31"/>
       <c r="F145" s="31"/>
@@ -36260,7 +36396,7 @@
         <v>3757</v>
       </c>
       <c r="D146" s="31" t="s">
-        <v>4543</v>
+        <v>4541</v>
       </c>
       <c r="E146" s="31"/>
       <c r="F146" s="31"/>
@@ -36276,7 +36412,7 @@
         <v>3759</v>
       </c>
       <c r="D147" s="31" t="s">
-        <v>4545</v>
+        <v>4543</v>
       </c>
       <c r="E147" s="31"/>
       <c r="F147" s="31"/>
@@ -36292,7 +36428,7 @@
         <v>3761</v>
       </c>
       <c r="D148" s="31" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="E148" s="31"/>
       <c r="F148" s="31"/>
@@ -36308,7 +36444,7 @@
         <v>3763</v>
       </c>
       <c r="D149" s="31" t="s">
-        <v>4546</v>
+        <v>4544</v>
       </c>
       <c r="E149" s="31"/>
       <c r="F149" s="31"/>
@@ -36324,7 +36460,7 @@
         <v>3765</v>
       </c>
       <c r="D150" s="31" t="s">
-        <v>4547</v>
+        <v>4545</v>
       </c>
       <c r="E150" s="31"/>
       <c r="F150" s="31"/>
@@ -36340,7 +36476,7 @@
         <v>3767</v>
       </c>
       <c r="D151" s="31" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="E151" s="31"/>
       <c r="F151" s="31"/>
@@ -36356,7 +36492,7 @@
         <v>3769</v>
       </c>
       <c r="D152" s="31" t="s">
-        <v>4549</v>
+        <v>4547</v>
       </c>
       <c r="E152" s="31"/>
       <c r="F152" s="31"/>
@@ -36372,7 +36508,7 @@
         <v>3771</v>
       </c>
       <c r="D153" s="31" t="s">
-        <v>4550</v>
+        <v>4548</v>
       </c>
       <c r="E153" s="31"/>
       <c r="F153" s="31"/>
@@ -36388,7 +36524,7 @@
         <v>3773</v>
       </c>
       <c r="D154" s="31" t="s">
-        <v>4551</v>
+        <v>4549</v>
       </c>
       <c r="E154" s="31"/>
       <c r="F154" s="31"/>
@@ -36404,7 +36540,7 @@
         <v>3775</v>
       </c>
       <c r="D155" s="31" t="s">
-        <v>4552</v>
+        <v>4550</v>
       </c>
       <c r="E155" s="31"/>
       <c r="F155" s="31"/>
@@ -36420,7 +36556,7 @@
         <v>3777</v>
       </c>
       <c r="D156" s="31" t="s">
-        <v>4553</v>
+        <v>4551</v>
       </c>
       <c r="E156" s="31"/>
       <c r="F156" s="31"/>
@@ -36436,7 +36572,7 @@
         <v>3778</v>
       </c>
       <c r="D157" s="31" t="s">
-        <v>4554</v>
+        <v>4552</v>
       </c>
       <c r="E157" s="31"/>
       <c r="F157" s="31"/>
@@ -36452,7 +36588,7 @@
         <v>3780</v>
       </c>
       <c r="D158" s="31" t="s">
-        <v>4555</v>
+        <v>4553</v>
       </c>
       <c r="E158" s="31"/>
       <c r="F158" s="31"/>
@@ -36468,7 +36604,7 @@
         <v>3782</v>
       </c>
       <c r="D159" s="31" t="s">
-        <v>4556</v>
+        <v>4554</v>
       </c>
       <c r="E159" s="31"/>
       <c r="F159" s="31"/>
@@ -36484,7 +36620,7 @@
         <v>3784</v>
       </c>
       <c r="D160" s="31" t="s">
-        <v>4557</v>
+        <v>4555</v>
       </c>
       <c r="E160" s="31"/>
       <c r="F160" s="31"/>
@@ -36500,7 +36636,7 @@
         <v>3786</v>
       </c>
       <c r="D161" s="31" t="s">
-        <v>4556</v>
+        <v>4554</v>
       </c>
       <c r="E161" s="31"/>
       <c r="F161" s="31"/>
@@ -36516,7 +36652,7 @@
         <v>3787</v>
       </c>
       <c r="D162" s="31" t="s">
-        <v>4560</v>
+        <v>4557</v>
       </c>
       <c r="E162" s="31"/>
       <c r="F162" s="31"/>
@@ -36532,7 +36668,7 @@
         <v>3789</v>
       </c>
       <c r="D163" s="31" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
       <c r="E163" s="31"/>
       <c r="F163" s="31"/>
@@ -36548,7 +36684,7 @@
         <v>3789</v>
       </c>
       <c r="D164" s="31" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
       <c r="E164" s="31"/>
       <c r="F164" s="31"/>
@@ -36564,7 +36700,7 @@
         <v>3789</v>
       </c>
       <c r="D165" s="31" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
       <c r="E165" s="31"/>
       <c r="F165" s="31"/>
@@ -36580,7 +36716,7 @@
         <v>3789</v>
       </c>
       <c r="D166" s="31" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
       <c r="E166" s="31"/>
       <c r="F166" s="31"/>
@@ -36596,7 +36732,7 @@
         <v>3789</v>
       </c>
       <c r="D167" s="31" t="s">
-        <v>4561</v>
+        <v>4558</v>
       </c>
       <c r="E167" s="31"/>
       <c r="F167" s="31"/>
@@ -36612,7 +36748,7 @@
         <v>3791</v>
       </c>
       <c r="D168" s="31" t="s">
-        <v>4562</v>
+        <v>4559</v>
       </c>
       <c r="E168" s="31"/>
       <c r="F168" s="31"/>
@@ -36622,13 +36758,13 @@
         <v>3792</v>
       </c>
       <c r="B169" s="31" t="s">
-        <v>4563</v>
+        <v>4560</v>
       </c>
       <c r="C169" s="31" t="s">
         <v>3793</v>
       </c>
       <c r="D169" s="31" t="s">
-        <v>4564</v>
+        <v>4561</v>
       </c>
       <c r="E169" s="31"/>
       <c r="F169" s="31"/>
@@ -36644,7 +36780,7 @@
         <v>3795</v>
       </c>
       <c r="D170" s="31" t="s">
-        <v>4569</v>
+        <v>4566</v>
       </c>
       <c r="E170" s="31"/>
       <c r="F170" s="31"/>
@@ -36660,7 +36796,7 @@
         <v>3797</v>
       </c>
       <c r="D171" s="31" t="s">
-        <v>4568</v>
+        <v>4565</v>
       </c>
       <c r="E171" s="31"/>
       <c r="F171" s="31"/>
@@ -36676,7 +36812,7 @@
         <v>3799</v>
       </c>
       <c r="D172" s="31" t="s">
-        <v>4567</v>
+        <v>4564</v>
       </c>
       <c r="E172" s="31"/>
       <c r="F172" s="31"/>
@@ -36692,7 +36828,7 @@
         <v>3801</v>
       </c>
       <c r="D173" s="31" t="s">
-        <v>4566</v>
+        <v>4563</v>
       </c>
       <c r="E173" s="31"/>
       <c r="F173" s="31"/>
@@ -36708,7 +36844,7 @@
         <v>3803</v>
       </c>
       <c r="D174" s="31" t="s">
-        <v>4565</v>
+        <v>4562</v>
       </c>
       <c r="E174" s="31"/>
       <c r="F174" s="31"/>
@@ -36724,7 +36860,7 @@
         <v>3805</v>
       </c>
       <c r="D175" s="31" t="s">
-        <v>4575</v>
+        <v>4572</v>
       </c>
       <c r="E175" s="31"/>
       <c r="F175" s="31"/>
@@ -36740,7 +36876,7 @@
         <v>3807</v>
       </c>
       <c r="D176" s="31" t="s">
-        <v>4570</v>
+        <v>4567</v>
       </c>
       <c r="E176" s="31"/>
       <c r="F176" s="31"/>
@@ -36756,7 +36892,7 @@
         <v>3809</v>
       </c>
       <c r="D177" s="31" t="s">
-        <v>4571</v>
+        <v>4568</v>
       </c>
       <c r="E177" s="31"/>
       <c r="F177" s="31"/>
@@ -36772,7 +36908,7 @@
         <v>3795</v>
       </c>
       <c r="D178" s="31" t="s">
-        <v>4569</v>
+        <v>4566</v>
       </c>
       <c r="E178" s="31"/>
       <c r="F178" s="31"/>
@@ -36788,7 +36924,7 @@
         <v>3803</v>
       </c>
       <c r="D179" s="31" t="s">
-        <v>4565</v>
+        <v>4562</v>
       </c>
       <c r="E179" s="31"/>
       <c r="F179" s="31"/>
@@ -36804,7 +36940,7 @@
         <v>3807</v>
       </c>
       <c r="D180" s="31" t="s">
-        <v>4570</v>
+        <v>4567</v>
       </c>
       <c r="E180" s="31"/>
       <c r="F180" s="31"/>
@@ -36820,7 +36956,7 @@
         <v>3809</v>
       </c>
       <c r="D181" s="31" t="s">
-        <v>4571</v>
+        <v>4568</v>
       </c>
       <c r="E181" s="31"/>
       <c r="F181" s="31"/>
@@ -36836,7 +36972,7 @@
         <v>3811</v>
       </c>
       <c r="D182" s="31" t="s">
-        <v>4572</v>
+        <v>4569</v>
       </c>
       <c r="E182" s="31"/>
       <c r="F182" s="31"/>
@@ -36846,13 +36982,13 @@
         <v>3812</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>4573</v>
+        <v>4570</v>
       </c>
       <c r="C183" s="31" t="s">
         <v>3813</v>
       </c>
       <c r="D183" s="31" t="s">
-        <v>4574</v>
+        <v>4571</v>
       </c>
       <c r="E183" s="31"/>
       <c r="F183" s="31"/>
@@ -36864,7 +37000,7 @@
         <v>3813</v>
       </c>
       <c r="D184" s="31" t="s">
-        <v>4574</v>
+        <v>4571</v>
       </c>
       <c r="E184" s="31"/>
       <c r="F184" s="31"/>
@@ -36928,7 +37064,7 @@
         <v>3818</v>
       </c>
       <c r="D189" s="31" t="s">
-        <v>4576</v>
+        <v>4573</v>
       </c>
       <c r="E189" s="31"/>
       <c r="F189" s="31"/>
@@ -36944,7 +37080,7 @@
         <v>3820</v>
       </c>
       <c r="D190" s="31" t="s">
-        <v>4577</v>
+        <v>4574</v>
       </c>
       <c r="E190" s="31"/>
       <c r="F190" s="31"/>
@@ -37064,7 +37200,7 @@
         <v>3828</v>
       </c>
       <c r="D198" s="31" t="s">
-        <v>4791</v>
+        <v>4788</v>
       </c>
       <c r="E198" s="31"/>
       <c r="F198" s="31"/>
@@ -37080,7 +37216,7 @@
         <v>3828</v>
       </c>
       <c r="D199" s="66" t="s">
-        <v>4791</v>
+        <v>4788</v>
       </c>
       <c r="E199" s="31"/>
       <c r="F199" s="31"/>
@@ -37144,7 +37280,7 @@
         <v>3833</v>
       </c>
       <c r="D203" s="31" t="s">
-        <v>4792</v>
+        <v>4789</v>
       </c>
       <c r="E203" s="31"/>
       <c r="F203" s="31"/>
@@ -37160,7 +37296,7 @@
         <v>3835</v>
       </c>
       <c r="D204" s="31" t="s">
-        <v>4793</v>
+        <v>4790</v>
       </c>
       <c r="E204" s="31"/>
       <c r="F204" s="31"/>
@@ -37176,7 +37312,7 @@
         <v>3835</v>
       </c>
       <c r="D205" s="66" t="s">
-        <v>4793</v>
+        <v>4790</v>
       </c>
       <c r="E205" s="31"/>
       <c r="F205" s="31"/>
@@ -37192,7 +37328,7 @@
         <v>3835</v>
       </c>
       <c r="D206" s="66" t="s">
-        <v>4793</v>
+        <v>4790</v>
       </c>
       <c r="E206" s="31"/>
       <c r="F206" s="31"/>
@@ -37208,7 +37344,7 @@
         <v>3838</v>
       </c>
       <c r="D207" s="31" t="s">
-        <v>4794</v>
+        <v>4791</v>
       </c>
       <c r="E207" s="31"/>
       <c r="F207" s="31"/>
@@ -37224,7 +37360,7 @@
         <v>3840</v>
       </c>
       <c r="D208" s="31" t="s">
-        <v>4795</v>
+        <v>4792</v>
       </c>
       <c r="E208" s="31"/>
       <c r="F208" s="31"/>
@@ -37240,7 +37376,7 @@
         <v>3840</v>
       </c>
       <c r="D209" s="66" t="s">
-        <v>4795</v>
+        <v>4792</v>
       </c>
       <c r="E209" s="31"/>
       <c r="F209" s="31"/>
@@ -37902,7 +38038,7 @@
       </c>
       <c r="C263" s="31"/>
       <c r="D263" s="31" t="s">
-        <v>4498</v>
+        <v>4496</v>
       </c>
       <c r="E263" s="31"/>
       <c r="F263" s="31"/>
@@ -38280,7 +38416,7 @@
         <v>3942</v>
       </c>
       <c r="B287" s="31" t="s">
-        <v>4534</v>
+        <v>4532</v>
       </c>
       <c r="C287" s="31" t="s">
         <v>3943</v>
@@ -38850,7 +38986,7 @@
         <v>2787</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>4558</v>
+        <v>4556</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>3343</v>
@@ -39629,7 +39765,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>4578</v>
+        <v>4575</v>
       </c>
       <c r="B1" t="s">
         <v>1589</v>
@@ -39640,12 +39776,12 @@
         <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>4579</v>
+        <v>4576</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4580</v>
+        <v>4577</v>
       </c>
       <c r="B3" t="s">
         <v>2754</v>
@@ -39656,7 +39792,7 @@
         <v>2755</v>
       </c>
       <c r="B4" t="s">
-        <v>4581</v>
+        <v>4578</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -39664,46 +39800,46 @@
         <v>2757</v>
       </c>
       <c r="B5" t="s">
-        <v>4582</v>
+        <v>4579</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>4583</v>
+        <v>4580</v>
       </c>
       <c r="B6" t="s">
-        <v>4584</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>4585</v>
+        <v>4582</v>
       </c>
       <c r="B7" t="s">
-        <v>4586</v>
+        <v>4583</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>4587</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>4588</v>
+        <v>4585</v>
       </c>
       <c r="B9" t="s">
-        <v>4589</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>4590</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>4591</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -39711,87 +39847,87 @@
         <v>1169</v>
       </c>
       <c r="B12" t="s">
-        <v>4592</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>4593</v>
+        <v>4590</v>
       </c>
       <c r="B13" t="s">
-        <v>4594</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>4595</v>
+        <v>4592</v>
       </c>
       <c r="B14" t="s">
-        <v>4596</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>4597</v>
+        <v>4594</v>
       </c>
       <c r="B15" t="s">
-        <v>4598</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>4599</v>
+        <v>4596</v>
       </c>
       <c r="B16" t="s">
-        <v>4600</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>4601</v>
+        <v>4598</v>
       </c>
       <c r="B17" t="s">
-        <v>4602</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>4603</v>
+        <v>4600</v>
       </c>
       <c r="B18" t="s">
-        <v>4604</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>4605</v>
+        <v>4602</v>
       </c>
       <c r="B19" t="s">
-        <v>4606</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>4605</v>
+        <v>4602</v>
       </c>
       <c r="B20" t="s">
-        <v>4606</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>4605</v>
+        <v>4602</v>
       </c>
       <c r="B21" t="s">
-        <v>4606</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>4605</v>
+        <v>4602</v>
       </c>
       <c r="B22" t="s">
-        <v>4606</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -39799,7 +39935,7 @@
         <v>3899</v>
       </c>
       <c r="B23" t="s">
-        <v>4607</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -39807,7 +39943,7 @@
         <v>2769</v>
       </c>
       <c r="B24" t="s">
-        <v>4608</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -39815,7 +39951,7 @@
         <v>2771</v>
       </c>
       <c r="B25" t="s">
-        <v>4609</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -39823,15 +39959,15 @@
         <v>2773</v>
       </c>
       <c r="B26" t="s">
-        <v>4610</v>
+        <v>4607</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>4611</v>
+        <v>4608</v>
       </c>
       <c r="B27" t="s">
-        <v>4612</v>
+        <v>4609</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -39839,31 +39975,31 @@
         <v>188</v>
       </c>
       <c r="B28" t="s">
-        <v>4613</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>4614</v>
+        <v>4611</v>
       </c>
       <c r="B29" t="s">
-        <v>4615</v>
+        <v>4612</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>4616</v>
+        <v>4613</v>
       </c>
       <c r="B30" t="s">
-        <v>4617</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>4618</v>
+        <v>4615</v>
       </c>
       <c r="B31" t="s">
-        <v>4619</v>
+        <v>4616</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -39871,15 +40007,15 @@
         <v>2785</v>
       </c>
       <c r="B32" t="s">
-        <v>4620</v>
+        <v>4617</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>4621</v>
+        <v>4618</v>
       </c>
       <c r="B33" t="s">
-        <v>4622</v>
+        <v>4619</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -39887,31 +40023,31 @@
         <v>161</v>
       </c>
       <c r="B34" t="s">
-        <v>4623</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>4624</v>
+        <v>4621</v>
       </c>
       <c r="B35" t="s">
-        <v>4625</v>
+        <v>4622</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>4626</v>
+        <v>4623</v>
       </c>
       <c r="B36" t="s">
-        <v>4627</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>4628</v>
+        <v>4625</v>
       </c>
       <c r="B37" t="s">
-        <v>4627</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -39919,60 +40055,60 @@
         <v>2792</v>
       </c>
       <c r="B38" t="s">
-        <v>4629</v>
+        <v>4626</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>4630</v>
+        <v>4627</v>
       </c>
       <c r="B39" t="s">
-        <v>4629</v>
+        <v>4626</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>4631</v>
+        <v>4628</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>4632</v>
+        <v>4629</v>
       </c>
       <c r="B41" t="s">
-        <v>4633</v>
+        <v>4630</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>4634</v>
+        <v>4631</v>
       </c>
       <c r="B42" t="s">
-        <v>4635</v>
+        <v>4632</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>4636</v>
+        <v>4633</v>
       </c>
       <c r="B43" t="s">
-        <v>4637</v>
+        <v>4634</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>4638</v>
+        <v>4635</v>
       </c>
       <c r="B44" t="s">
-        <v>4639</v>
+        <v>4636</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>4640</v>
+        <v>4637</v>
       </c>
       <c r="B45" t="s">
-        <v>4641</v>
+        <v>4638</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -39980,143 +40116,143 @@
         <v>2795</v>
       </c>
       <c r="B46" t="s">
-        <v>4642</v>
+        <v>4639</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>4643</v>
+        <v>4640</v>
       </c>
       <c r="B47" t="s">
-        <v>4644</v>
+        <v>4641</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>4645</v>
+        <v>4642</v>
       </c>
       <c r="B48" t="s">
-        <v>4646</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>4647</v>
+        <v>4644</v>
       </c>
       <c r="B49" t="s">
-        <v>4648</v>
+        <v>4645</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>4649</v>
+        <v>4646</v>
       </c>
       <c r="B50" t="s">
-        <v>4650</v>
+        <v>4647</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>4651</v>
+        <v>4648</v>
       </c>
       <c r="B51" t="s">
-        <v>4652</v>
+        <v>4649</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>4653</v>
+        <v>4650</v>
       </c>
       <c r="B52" t="s">
-        <v>4654</v>
+        <v>4651</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>4655</v>
+        <v>4652</v>
       </c>
       <c r="B53" t="s">
-        <v>4656</v>
+        <v>4653</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>4657</v>
+        <v>4654</v>
       </c>
       <c r="B54" t="s">
-        <v>4658</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>4659</v>
+        <v>4656</v>
       </c>
       <c r="B55" t="s">
-        <v>4660</v>
+        <v>4657</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>4661</v>
+        <v>4658</v>
       </c>
       <c r="B56" t="s">
-        <v>4658</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>4662</v>
+        <v>4659</v>
       </c>
       <c r="B57" t="s">
-        <v>4663</v>
+        <v>4660</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>4664</v>
+        <v>4661</v>
       </c>
       <c r="B58" t="s">
-        <v>4665</v>
+        <v>4662</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>4666</v>
+        <v>4663</v>
       </c>
       <c r="B59" t="s">
-        <v>4667</v>
+        <v>4664</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>4668</v>
+        <v>4665</v>
       </c>
       <c r="B60" t="s">
-        <v>4669</v>
+        <v>4666</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>4670</v>
+        <v>4667</v>
       </c>
       <c r="B61" t="s">
-        <v>4671</v>
+        <v>4668</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>4672</v>
+        <v>4669</v>
       </c>
       <c r="B62" t="s">
-        <v>4673</v>
+        <v>4670</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>4674</v>
+        <v>4671</v>
       </c>
       <c r="B63" t="s">
-        <v>4675</v>
+        <v>4672</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -40124,39 +40260,39 @@
         <v>2821</v>
       </c>
       <c r="B64" t="s">
-        <v>4676</v>
+        <v>4673</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>4677</v>
+        <v>4674</v>
       </c>
       <c r="B65" t="s">
-        <v>4678</v>
+        <v>4675</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>4679</v>
+        <v>4676</v>
       </c>
       <c r="B66" t="s">
-        <v>4680</v>
+        <v>4677</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>4681</v>
+        <v>4678</v>
       </c>
       <c r="B67" t="s">
-        <v>4682</v>
+        <v>4679</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>4683</v>
+        <v>4680</v>
       </c>
       <c r="B68" t="s">
-        <v>4684</v>
+        <v>4681</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -40164,7 +40300,7 @@
         <v>2831</v>
       </c>
       <c r="B69" t="s">
-        <v>4685</v>
+        <v>4682</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -40172,23 +40308,23 @@
         <v>2833</v>
       </c>
       <c r="B70" t="s">
-        <v>4686</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>4687</v>
+        <v>4684</v>
       </c>
       <c r="B71" t="s">
-        <v>4688</v>
+        <v>4685</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>4689</v>
+        <v>4686</v>
       </c>
       <c r="B72" t="s">
-        <v>4690</v>
+        <v>4687</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -40196,7 +40332,7 @@
         <v>2839</v>
       </c>
       <c r="B73" t="s">
-        <v>4691</v>
+        <v>4688</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -40204,7 +40340,7 @@
         <v>2841</v>
       </c>
       <c r="B74" t="s">
-        <v>4692</v>
+        <v>4689</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -40214,173 +40350,173 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>4693</v>
+        <v>4690</v>
       </c>
       <c r="B76" t="s">
-        <v>4694</v>
+        <v>4691</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>4695</v>
+        <v>4692</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>4696</v>
+        <v>4693</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>4697</v>
+        <v>4694</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>4698</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>4699</v>
+        <v>4696</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>4700</v>
+        <v>4697</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>4701</v>
+        <v>4698</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>4702</v>
+        <v>4699</v>
       </c>
       <c r="B84" t="s">
-        <v>4703</v>
+        <v>4700</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>4704</v>
+        <v>4701</v>
       </c>
       <c r="B85" t="s">
-        <v>4705</v>
+        <v>4702</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>4706</v>
+        <v>4703</v>
       </c>
       <c r="B86" t="s">
-        <v>4707</v>
+        <v>4704</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>4708</v>
+        <v>4705</v>
       </c>
       <c r="B87" t="s">
-        <v>4709</v>
+        <v>4706</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>4710</v>
+        <v>4707</v>
       </c>
       <c r="B88" t="s">
-        <v>4711</v>
+        <v>4708</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>4710</v>
+        <v>4707</v>
       </c>
       <c r="B89" t="s">
-        <v>4712</v>
+        <v>4709</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>4713</v>
+        <v>4710</v>
       </c>
       <c r="B90" t="s">
-        <v>4714</v>
+        <v>4711</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>4715</v>
+        <v>4712</v>
       </c>
       <c r="B91" t="s">
-        <v>4716</v>
+        <v>4713</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>4717</v>
+        <v>4714</v>
       </c>
       <c r="B92" t="s">
-        <v>4718</v>
+        <v>4715</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>4719</v>
+        <v>4716</v>
       </c>
       <c r="B93" t="s">
-        <v>4720</v>
+        <v>4717</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>4721</v>
+        <v>4718</v>
       </c>
       <c r="B94" t="s">
-        <v>4722</v>
+        <v>4719</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>4723</v>
+        <v>4720</v>
       </c>
       <c r="B95" t="s">
-        <v>4724</v>
+        <v>4721</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>4725</v>
+        <v>4722</v>
       </c>
       <c r="B96" t="s">
-        <v>4726</v>
+        <v>4723</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>4727</v>
+        <v>4724</v>
       </c>
       <c r="B97" t="s">
-        <v>4728</v>
+        <v>4725</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>4729</v>
+        <v>4726</v>
       </c>
       <c r="B98" t="s">
-        <v>4730</v>
+        <v>4727</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>4731</v>
+        <v>4728</v>
       </c>
       <c r="B99" t="s">
-        <v>4730</v>
+        <v>4727</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -40388,15 +40524,15 @@
         <v>3764</v>
       </c>
       <c r="B100" t="s">
-        <v>4732</v>
+        <v>4729</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>4733</v>
+        <v>4730</v>
       </c>
       <c r="B101" t="s">
-        <v>4734</v>
+        <v>4731</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -40406,10 +40542,10 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>4735</v>
+        <v>4732</v>
       </c>
       <c r="B103" t="s">
-        <v>4736</v>
+        <v>4733</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -40417,7 +40553,7 @@
         <v>2863</v>
       </c>
       <c r="B104" t="s">
-        <v>4736</v>
+        <v>4733</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -40425,47 +40561,47 @@
         <v>2864</v>
       </c>
       <c r="B105" t="s">
-        <v>4736</v>
+        <v>4733</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>4737</v>
+        <v>4734</v>
       </c>
       <c r="B106" t="s">
-        <v>4738</v>
+        <v>4735</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>4739</v>
+        <v>4736</v>
       </c>
       <c r="B107" t="s">
-        <v>4740</v>
+        <v>4737</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>4741</v>
+        <v>4738</v>
       </c>
       <c r="B108" t="s">
-        <v>4742</v>
+        <v>4739</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>4743</v>
+        <v>4740</v>
       </c>
       <c r="B109" t="s">
-        <v>4744</v>
+        <v>4741</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>4745</v>
+        <v>4742</v>
       </c>
       <c r="B110" t="s">
-        <v>4746</v>
+        <v>4743</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -40473,38 +40609,38 @@
         <v>2870</v>
       </c>
       <c r="B111" t="s">
-        <v>4747</v>
+        <v>4744</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>4748</v>
+        <v>4745</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>4749</v>
+        <v>4746</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>4750</v>
+        <v>4747</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>4751</v>
+        <v>4748</v>
       </c>
       <c r="B115" t="s">
-        <v>4752</v>
+        <v>4749</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>4753</v>
+        <v>4750</v>
       </c>
       <c r="B116" t="s">
-        <v>4754</v>
+        <v>4751</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -40512,7 +40648,7 @@
         <v>2878</v>
       </c>
       <c r="B117" t="s">
-        <v>4755</v>
+        <v>4752</v>
       </c>
     </row>
   </sheetData>
@@ -41563,7 +41699,7 @@
         <v>1426</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>4470</v>
+        <v>4469</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14" t="s">
@@ -41696,7 +41832,7 @@
         <v>1436</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>4481</v>
+        <v>4479</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="18" t="s">
@@ -41981,7 +42117,7 @@
         <v>1452</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>4471</v>
+        <v>4470</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14" t="s">

</xml_diff>

<commit_message>
Slime events are all done!
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -15669,7 +15669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -20455,8 +20455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D63" sqref="A63:D63"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>

</xml_diff>

<commit_message>
Ultimate proofreading for chapter 10
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7329" uniqueCount="5205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7280" uniqueCount="5213">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -15956,6 +15956,30 @@
   </si>
   <si>
     <t>E2: Queen's Illusions</t>
+  </si>
+  <si>
+    <t>我慢できずにしごき始めてしま った。</t>
+  </si>
+  <si>
+    <t>メイドのサキュバスに斬りかかった</t>
+  </si>
+  <si>
+    <t>Don't hold back and start masturbating</t>
+  </si>
+  <si>
+    <t>Swing your sword at the maid succubus</t>
+  </si>
+  <si>
+    <t>技術の指輪</t>
+  </si>
+  <si>
+    <t>Skill Ring</t>
+  </si>
+  <si>
+    <t>Increases Skill when held.</t>
+  </si>
+  <si>
+    <t>[UNKNOWN]</t>
   </si>
 </sst>
 </file>
@@ -16794,10 +16818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ50"/>
+  <dimension ref="A1:BZ52"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -16828,24 +16852,12 @@
       <c r="L1" s="45"/>
     </row>
     <row r="2" spans="1:78" ht="15.9">
-      <c r="A2" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="59" t="s">
-        <v>2151</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>2187</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>5197</v>
-      </c>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="77"/>
       <c r="H2" s="85"/>
       <c r="I2" s="45"/>
@@ -17025,374 +17037,266 @@
       <c r="K5" s="59"/>
     </row>
     <row r="6" spans="1:78">
-      <c r="E6" s="56"/>
+      <c r="A6" s="59" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>907</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>5205</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>5207</v>
+      </c>
       <c r="F6" s="57"/>
     </row>
     <row r="7" spans="1:78">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59" t="s">
+        <v>5206</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>5208</v>
+      </c>
+      <c r="F7" s="55"/>
+    </row>
+    <row r="8" spans="1:78">
+      <c r="E8" s="56"/>
+    </row>
+    <row r="9" spans="1:78">
+      <c r="A9" s="37" t="s">
         <v>4397</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="55"/>
-    </row>
-    <row r="8" spans="1:78">
-      <c r="A8" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>2167</v>
-      </c>
-      <c r="E8" s="56"/>
-    </row>
-    <row r="9" spans="1:78">
-      <c r="A9" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>1458</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>2166</v>
-      </c>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:78">
-      <c r="A10" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C10" s="59" t="s">
-        <v>1575</v>
-      </c>
-      <c r="D10" s="59" t="s">
-        <v>5198</v>
-      </c>
+      <c r="A10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="56"/>
     </row>
     <row r="11" spans="1:78">
-      <c r="A11" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B11" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>1576</v>
-      </c>
-      <c r="D11" s="59" t="s">
-        <v>5199</v>
-      </c>
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
     </row>
     <row r="12" spans="1:78">
-      <c r="A12" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>2222</v>
-      </c>
-      <c r="D12" s="59" t="s">
-        <v>2484</v>
-      </c>
-      <c r="E12" s="59"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
     </row>
     <row r="13" spans="1:78">
-      <c r="A13" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B13" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C13" s="59" t="s">
-        <v>1514</v>
-      </c>
-      <c r="D13" s="59" t="s">
-        <v>4857</v>
-      </c>
+      <c r="A13" s="59"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
     </row>
     <row r="14" spans="1:78">
-      <c r="A14" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B14" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C14" s="59" t="s">
-        <v>1511</v>
-      </c>
-      <c r="D14" s="59" t="s">
-        <v>4858</v>
-      </c>
+      <c r="A14" s="59"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
     </row>
     <row r="15" spans="1:78">
-      <c r="A15" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C15" s="59" t="s">
-        <v>1412</v>
-      </c>
-      <c r="D15" s="59" t="s">
-        <v>2230</v>
-      </c>
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
     </row>
     <row r="16" spans="1:78">
-      <c r="A16" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B16" s="59" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C16" s="59" t="s">
-        <v>1578</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>5200</v>
-      </c>
+      <c r="A16" s="59"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B17" s="59" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>1580</v>
-      </c>
-      <c r="D17" s="59" t="s">
-        <v>5201</v>
-      </c>
+      <c r="A17" s="59"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="59" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B18" s="59" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C18" s="59" t="s">
-        <v>1582</v>
-      </c>
-      <c r="D18" s="59" t="s">
-        <v>5202</v>
-      </c>
+      <c r="A18" s="59"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="59" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B19" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>1514</v>
-      </c>
-      <c r="D19" s="59" t="s">
-        <v>4857</v>
-      </c>
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="59" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B20" s="59" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>1511</v>
-      </c>
-      <c r="D20" s="59" t="s">
-        <v>4858</v>
-      </c>
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
     </row>
     <row r="21" spans="1:6" s="59" customFormat="1">
-      <c r="A21" s="59" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B21" s="59" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C21" s="59" t="s">
-        <v>1412</v>
-      </c>
-      <c r="D21" s="59" t="s">
-        <v>2230</v>
-      </c>
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="59" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B22" s="59" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C22" s="59" t="s">
-        <v>1584</v>
-      </c>
-      <c r="D22" s="59" t="s">
-        <v>5203</v>
-      </c>
-      <c r="E22" s="59"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
       <c r="F22" s="59"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="59" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B23" s="59" t="s">
-        <v>1411</v>
-      </c>
-      <c r="C23" s="59" t="s">
-        <v>1586</v>
-      </c>
-      <c r="D23" s="59" t="s">
-        <v>5204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15">
-      <c r="A24" s="58"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="45"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="59"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.9">
-      <c r="A26" s="45"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="77"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+    </row>
+    <row r="26" spans="1:6" ht="15">
+      <c r="A26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="45"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="59"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.9">
+      <c r="A28" s="45"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="77"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="37" t="s">
         <v>4848</v>
       </c>
-      <c r="D27" s="55"/>
-      <c r="E27" s="59"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="60"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="66"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="59"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="60"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="66"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="59"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="68" t="s">
         <v>2505</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="59"/>
-    </row>
-    <row r="31" spans="1:6" ht="15">
-      <c r="A31" s="70"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-    </row>
-    <row r="32" spans="1:6" ht="15">
-      <c r="A32" s="69" t="s">
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="59"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.9">
+      <c r="A33" s="13" t="s">
+        <v>5209</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>5212</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>5210</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>5211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15">
+      <c r="A34" s="69" t="s">
         <v>5168</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-    </row>
-    <row r="33" spans="1:4" ht="15">
-      <c r="A33" s="71"/>
-      <c r="B33" s="70"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="72"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="59"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="59"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+    </row>
+    <row r="35" spans="1:4" ht="15">
+      <c r="A35" s="71"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="68" t="s">
-        <v>5138</v>
-      </c>
+      <c r="A38" s="59"/>
       <c r="B38" s="59"/>
       <c r="C38" s="59"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="68"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-    </row>
-    <row r="40" spans="1:4" ht="15">
-      <c r="A40" s="37" t="s">
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="68" t="s">
+        <v>5138</v>
+      </c>
+      <c r="B40" s="59"/>
+      <c r="C40" s="59"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="68"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+    </row>
+    <row r="42" spans="1:4" ht="15">
+      <c r="A42" s="37" t="s">
         <v>3421</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="37" t="s">
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="37" t="s">
         <v>5181</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-    </row>
-    <row r="42" spans="1:4" ht="15">
-      <c r="A42" s="72"/>
-      <c r="B42" s="73"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="72"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.9">
-      <c r="A43" s="77"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.9">
-      <c r="A44" s="77"/>
-      <c r="B44" s="77"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+    </row>
+    <row r="44" spans="1:4" ht="15">
+      <c r="A44" s="72"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
     </row>
     <row r="45" spans="1:4" ht="15.9">
       <c r="A45" s="77"/>
@@ -17412,23 +17316,35 @@
       <c r="C47" s="77"/>
       <c r="D47" s="77"/>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
+    <row r="48" spans="1:4" ht="15.9">
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.9">
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="77"/>
+      <c r="D49" s="77"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="45"/>
       <c r="B50" s="45"/>
       <c r="C50" s="45"/>
       <c r="D50" s="45"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="45"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="45"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18147,7 +18063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A115" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
@@ -21032,10 +20948,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G203"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178"/>
+    <sheetView topLeftCell="A128" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D142" sqref="A142:D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -23955,357 +23871,351 @@
       <c r="F141" s="14"/>
       <c r="G141" s="14"/>
     </row>
-    <row r="142" spans="1:7" ht="15.9">
+    <row r="142" spans="1:7" s="58" customFormat="1" ht="15.9">
       <c r="A142" s="13" t="s">
-        <v>674</v>
-      </c>
-      <c r="B142" s="13" t="s">
-        <v>675</v>
-      </c>
+        <v>5209</v>
+      </c>
+      <c r="B142" s="13"/>
       <c r="C142" s="10" t="s">
-        <v>1965</v>
+        <v>5210</v>
       </c>
       <c r="D142" s="10" t="s">
-        <v>2051</v>
-      </c>
-      <c r="E142" s="14" t="s">
-        <v>676</v>
-      </c>
-      <c r="F142" s="14" t="s">
-        <v>677</v>
-      </c>
-      <c r="G142" s="14"/>
+        <v>5211</v>
+      </c>
+      <c r="E142" s="59"/>
+      <c r="F142" s="59"/>
+      <c r="G142" s="59"/>
     </row>
     <row r="143" spans="1:7" ht="15.9">
       <c r="A143" s="13" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="E143" s="14" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="F143" s="14" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="G143" s="14"/>
     </row>
     <row r="144" spans="1:7" ht="15.9">
       <c r="A144" s="13" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="E144" s="14" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="F144" s="14" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="G144" s="14"/>
     </row>
     <row r="145" spans="1:7" ht="15.9">
       <c r="A145" s="13" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="D145" s="10" t="s">
-        <v>2427</v>
+        <v>2053</v>
       </c>
       <c r="E145" s="14" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="F145" s="14" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="G145" s="14"/>
     </row>
     <row r="146" spans="1:7" ht="15.9">
       <c r="A146" s="13" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C146" s="10" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="D146" s="10" t="s">
-        <v>2429</v>
-      </c>
-      <c r="E146" s="18" t="s">
-        <v>692</v>
+        <v>2427</v>
+      </c>
+      <c r="E146" s="14" t="s">
+        <v>688</v>
       </c>
       <c r="F146" s="14" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="G146" s="14"/>
     </row>
     <row r="147" spans="1:7" ht="15.9">
       <c r="A147" s="13" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="D147" s="10" t="s">
-        <v>2428</v>
-      </c>
-      <c r="E147" s="14" t="s">
-        <v>696</v>
+        <v>2429</v>
+      </c>
+      <c r="E147" s="18" t="s">
+        <v>692</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="G147" s="14"/>
     </row>
     <row r="148" spans="1:7" ht="15.9">
       <c r="A148" s="13" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>2061</v>
+        <v>2428</v>
       </c>
       <c r="E148" s="14" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="F148" s="14" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="G148" s="14"/>
     </row>
     <row r="149" spans="1:7" ht="15.9">
       <c r="A149" s="13" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="E149" s="14" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="F149" s="14" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="G149" s="14"/>
     </row>
     <row r="150" spans="1:7" ht="15.9">
       <c r="A150" s="13" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="D150" s="10" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="E150" s="14" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="F150" s="14" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="G150" s="14"/>
     </row>
     <row r="151" spans="1:7" ht="15.9">
       <c r="A151" s="13" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="D151" s="10" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="E151" s="14" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="F151" s="14" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="G151" s="14"/>
     </row>
     <row r="152" spans="1:7" ht="15.9">
       <c r="A152" s="13" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="D152" s="10" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="E152" s="14" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="F152" s="14" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="G152" s="14"/>
     </row>
     <row r="153" spans="1:7" ht="15.9">
       <c r="A153" s="13" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>2470</v>
+        <v>1975</v>
       </c>
       <c r="D153" s="10" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="E153" s="14" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="F153" s="14" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="G153" s="14"/>
     </row>
     <row r="154" spans="1:7" ht="15.9">
       <c r="A154" s="13" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="C154" s="10" t="s">
-        <v>1976</v>
+        <v>2470</v>
       </c>
       <c r="D154" s="10" t="s">
-        <v>2067</v>
-      </c>
-      <c r="E154" s="18" t="s">
-        <v>724</v>
+        <v>2066</v>
+      </c>
+      <c r="E154" s="14" t="s">
+        <v>720</v>
       </c>
       <c r="F154" s="14" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="G154" s="14"/>
     </row>
     <row r="155" spans="1:7" ht="15.9">
       <c r="A155" s="13" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>699</v>
+        <v>723</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="D155" s="10" t="s">
-        <v>2061</v>
-      </c>
-      <c r="E155" s="14" t="s">
-        <v>727</v>
+        <v>2067</v>
+      </c>
+      <c r="E155" s="18" t="s">
+        <v>724</v>
       </c>
       <c r="F155" s="14" t="s">
-        <v>701</v>
+        <v>725</v>
       </c>
       <c r="G155" s="14"/>
     </row>
     <row r="156" spans="1:7" ht="15.9">
       <c r="A156" s="13" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>729</v>
+        <v>699</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="D156" s="10" t="s">
-        <v>2054</v>
+        <v>2061</v>
       </c>
       <c r="E156" s="14" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="F156" s="14" t="s">
-        <v>731</v>
+        <v>701</v>
       </c>
       <c r="G156" s="14"/>
     </row>
     <row r="157" spans="1:7" ht="15.9">
       <c r="A157" s="13" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="D157" s="10" t="s">
-        <v>2430</v>
+        <v>2054</v>
       </c>
       <c r="E157" s="14" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="F157" s="14" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="G157" s="14"/>
     </row>
     <row r="158" spans="1:7" ht="15.9">
       <c r="A158" s="13" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B158" s="13" t="s">
         <v>733</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="D158" s="10" t="s">
         <v>2430</v>
       </c>
       <c r="E158" s="14" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="F158" s="14" t="s">
         <v>735</v>
@@ -24314,187 +24224,187 @@
     </row>
     <row r="159" spans="1:7" ht="15.9">
       <c r="A159" s="13" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="E159" s="14" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="F159" s="14" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="G159" s="14"/>
     </row>
     <row r="160" spans="1:7" ht="15.9">
       <c r="A160" s="13" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="D160" s="10" t="s">
-        <v>2068</v>
+        <v>2431</v>
       </c>
       <c r="E160" s="14" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="F160" s="14" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G160" s="14"/>
     </row>
     <row r="161" spans="1:7" ht="15.9">
       <c r="A161" s="13" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="D161" s="10" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="E161" s="14" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="F161" s="14" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="G161" s="14"/>
     </row>
     <row r="162" spans="1:7" ht="15.9">
       <c r="A162" s="13" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="D162" s="10" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="E162" s="14" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="F162" s="14" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="G162" s="14"/>
     </row>
     <row r="163" spans="1:7" ht="15.9">
       <c r="A163" s="13" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="D163" s="10" t="s">
-        <v>2070</v>
+        <v>2071</v>
       </c>
       <c r="E163" s="14" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="F163" s="14" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="G163" s="14"/>
     </row>
     <row r="164" spans="1:7" ht="15.9">
       <c r="A164" s="13" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="D164" s="10" t="s">
-        <v>2060</v>
+        <v>2070</v>
       </c>
       <c r="E164" s="14" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="F164" s="14" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="G164" s="14"/>
     </row>
     <row r="165" spans="1:7" ht="15.9">
       <c r="A165" s="13" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="D165" s="10" t="s">
-        <v>2432</v>
+        <v>2060</v>
       </c>
       <c r="E165" s="14" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="F165" s="14" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="G165" s="14"/>
     </row>
     <row r="166" spans="1:7" ht="15.9">
       <c r="A166" s="13" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C166" s="10" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="D166" s="10" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="E166" s="14" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="F166" s="14" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="G166" s="14"/>
     </row>
     <row r="167" spans="1:7" ht="15.9">
       <c r="A167" s="13" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="B167" s="13" t="s">
         <v>765</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>2433</v>
       </c>
       <c r="E167" s="14" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="F167" s="14" t="s">
         <v>767</v>
@@ -24503,99 +24413,101 @@
     </row>
     <row r="168" spans="1:7" ht="15.9">
       <c r="A168" s="13" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>3356</v>
+        <v>1989</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>2055</v>
+        <v>2433</v>
       </c>
       <c r="E168" s="14" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="F168" s="14" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="G168" s="14"/>
     </row>
     <row r="169" spans="1:7" ht="15.9">
       <c r="A169" s="13" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>1990</v>
+        <v>3356</v>
       </c>
       <c r="D169" s="10" t="s">
-        <v>2434</v>
+        <v>2055</v>
       </c>
       <c r="E169" s="14" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="F169" s="14" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="G169" s="14"/>
     </row>
     <row r="170" spans="1:7" ht="15.9">
       <c r="A170" s="13" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="D170" s="10" t="s">
-        <v>2437</v>
+        <v>2434</v>
       </c>
       <c r="E170" s="14" t="s">
-        <v>780</v>
-      </c>
-      <c r="F170" s="14"/>
+        <v>776</v>
+      </c>
+      <c r="F170" s="14" t="s">
+        <v>777</v>
+      </c>
       <c r="G170" s="14"/>
     </row>
     <row r="171" spans="1:7" ht="15.9">
       <c r="A171" s="13" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="D171" s="10" t="s">
-        <v>2436</v>
+        <v>2437</v>
       </c>
       <c r="E171" s="14" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="F171" s="14"/>
       <c r="G171" s="14"/>
     </row>
     <row r="172" spans="1:7" ht="15.9">
       <c r="A172" s="13" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>3355</v>
+        <v>1992</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>2435</v>
+        <v>2436</v>
       </c>
       <c r="E172" s="14" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="F172" s="14"/>
       <c r="G172" s="14"/>
@@ -24605,13 +24517,13 @@
         <v>784</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C173" s="10" t="s">
         <v>3355</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>2460</v>
+        <v>2435</v>
       </c>
       <c r="E173" s="14" t="s">
         <v>786</v>
@@ -24621,38 +24533,38 @@
     </row>
     <row r="174" spans="1:7" ht="15.9">
       <c r="A174" s="13" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>1900</v>
+        <v>3355</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>4406</v>
+        <v>2460</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="F174" s="14"/>
       <c r="G174" s="14"/>
     </row>
     <row r="175" spans="1:7" ht="15.9">
       <c r="A175" s="13" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>1993</v>
+        <v>1900</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>2459</v>
+        <v>4406</v>
       </c>
       <c r="E175" s="14" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="F175" s="14"/>
       <c r="G175" s="14"/>
@@ -24662,13 +24574,13 @@
         <v>791</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>2461</v>
+        <v>2459</v>
       </c>
       <c r="E176" s="14" t="s">
         <v>793</v>
@@ -24678,572 +24590,591 @@
     </row>
     <row r="177" spans="1:7" ht="15.9">
       <c r="A177" s="13" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C177" s="10" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="E177" s="14" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
     </row>
     <row r="178" spans="1:7" ht="15.9">
       <c r="A178" s="13" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="C178" s="10" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>2438</v>
+        <v>2462</v>
       </c>
       <c r="E178" s="14" t="s">
-        <v>800</v>
-      </c>
-      <c r="F178" s="14" t="s">
-        <v>801</v>
-      </c>
+        <v>797</v>
+      </c>
+      <c r="F178" s="14"/>
       <c r="G178" s="14"/>
     </row>
     <row r="179" spans="1:7" ht="15.9">
       <c r="A179" s="13" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>2439</v>
-      </c>
-      <c r="E179" s="16" t="s">
-        <v>804</v>
+        <v>2438</v>
+      </c>
+      <c r="E179" s="14" t="s">
+        <v>800</v>
       </c>
       <c r="F179" s="14" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="G179" s="14"/>
     </row>
     <row r="180" spans="1:7" ht="15.9">
       <c r="A180" s="13" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C180" s="10" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="E180" s="16" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="F180" s="14" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="G180" s="14"/>
     </row>
     <row r="181" spans="1:7" ht="15.9">
       <c r="A181" s="13" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>2441</v>
-      </c>
-      <c r="E181" s="14" t="s">
-        <v>812</v>
+        <v>2440</v>
+      </c>
+      <c r="E181" s="16" t="s">
+        <v>808</v>
       </c>
       <c r="F181" s="14" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="G181" s="14"/>
     </row>
     <row r="182" spans="1:7" ht="15.9">
       <c r="A182" s="13" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>3397</v>
+        <v>2441</v>
       </c>
       <c r="E182" s="14" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="F182" s="14" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="G182" s="14"/>
     </row>
     <row r="183" spans="1:7" ht="15.9">
       <c r="A183" s="13" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>3354</v>
+        <v>2000</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>2444</v>
+        <v>3397</v>
       </c>
       <c r="E183" s="14" t="s">
-        <v>820</v>
-      </c>
-      <c r="F183" s="16" t="s">
-        <v>821</v>
+        <v>816</v>
+      </c>
+      <c r="F183" s="14" t="s">
+        <v>817</v>
       </c>
       <c r="G183" s="14"/>
     </row>
     <row r="184" spans="1:7" ht="15.9">
       <c r="A184" s="13" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>2001</v>
+        <v>3354</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>2443</v>
+        <v>2444</v>
       </c>
       <c r="E184" s="14" t="s">
-        <v>824</v>
-      </c>
-      <c r="F184" s="14" t="s">
-        <v>825</v>
+        <v>820</v>
+      </c>
+      <c r="F184" s="16" t="s">
+        <v>821</v>
       </c>
       <c r="G184" s="14"/>
     </row>
     <row r="185" spans="1:7" ht="15.9">
       <c r="A185" s="13" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>2442</v>
+        <v>2443</v>
       </c>
       <c r="E185" s="14" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="F185" s="14" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="G185" s="14"/>
     </row>
     <row r="186" spans="1:7" ht="15.9">
       <c r="A186" s="13" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>3396</v>
+        <v>2002</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>3398</v>
+        <v>2442</v>
       </c>
       <c r="E186" s="14" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="F186" s="14" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="G186" s="14"/>
     </row>
     <row r="187" spans="1:7" ht="15.9">
       <c r="A187" s="13" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>2003</v>
+        <v>3396</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>2445</v>
+        <v>3398</v>
       </c>
       <c r="E187" s="14" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="F187" s="14" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="G187" s="14"/>
     </row>
     <row r="188" spans="1:7" ht="15.9">
       <c r="A188" s="13" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="E188" s="14" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="F188" s="14" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="G188" s="14"/>
     </row>
     <row r="189" spans="1:7" ht="15.9">
       <c r="A189" s="13" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>3353</v>
+        <v>2004</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="E189" s="14" t="s">
-        <v>844</v>
-      </c>
-      <c r="F189" s="16" t="s">
-        <v>845</v>
+        <v>840</v>
+      </c>
+      <c r="F189" s="14" t="s">
+        <v>841</v>
       </c>
       <c r="G189" s="14"/>
     </row>
     <row r="190" spans="1:7" ht="15.9">
       <c r="A190" s="13" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="C190" s="10" t="s">
-        <v>2005</v>
+        <v>3353</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>3344</v>
+        <v>2447</v>
       </c>
       <c r="E190" s="14" t="s">
-        <v>848</v>
-      </c>
-      <c r="F190" s="14" t="s">
-        <v>849</v>
+        <v>844</v>
+      </c>
+      <c r="F190" s="16" t="s">
+        <v>845</v>
       </c>
       <c r="G190" s="14"/>
     </row>
     <row r="191" spans="1:7" ht="15.9">
       <c r="A191" s="13" t="s">
+        <v>846</v>
+      </c>
+      <c r="B191" s="13" t="s">
+        <v>847</v>
+      </c>
+      <c r="C191" s="10" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D191" s="10" t="s">
+        <v>3344</v>
+      </c>
+      <c r="E191" s="14" t="s">
+        <v>848</v>
+      </c>
+      <c r="F191" s="14" t="s">
+        <v>849</v>
+      </c>
+      <c r="G191" s="14"/>
+    </row>
+    <row r="192" spans="1:7" ht="15.9">
+      <c r="A192" s="13" t="s">
         <v>850</v>
       </c>
-      <c r="B191" s="13" t="s">
+      <c r="B192" s="13" t="s">
         <v>851</v>
-      </c>
-      <c r="C191" s="10" t="s">
-        <v>2006</v>
-      </c>
-      <c r="D191" s="10" t="s">
-        <v>2056</v>
-      </c>
-      <c r="E191" s="14" t="s">
-        <v>852</v>
-      </c>
-      <c r="F191" s="14" t="s">
-        <v>853</v>
-      </c>
-      <c r="G191" s="14" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" s="8" customFormat="1" ht="15.9">
-      <c r="A192" s="19" t="s">
-        <v>850</v>
-      </c>
-      <c r="B192" s="19" t="s">
-        <v>855</v>
       </c>
       <c r="C192" s="10" t="s">
         <v>2006</v>
       </c>
       <c r="D192" s="10" t="s">
+        <v>2056</v>
+      </c>
+      <c r="E192" s="14" t="s">
+        <v>852</v>
+      </c>
+      <c r="F192" s="14" t="s">
+        <v>853</v>
+      </c>
+      <c r="G192" s="14" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" s="8" customFormat="1" ht="15.9">
+      <c r="A193" s="19" t="s">
+        <v>850</v>
+      </c>
+      <c r="B193" s="19" t="s">
+        <v>855</v>
+      </c>
+      <c r="C193" s="10" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D193" s="10" t="s">
         <v>2059</v>
       </c>
-      <c r="E192" s="18" t="s">
+      <c r="E193" s="18" t="s">
         <v>852</v>
       </c>
-      <c r="F192" s="18" t="s">
+      <c r="F193" s="18" t="s">
         <v>856</v>
       </c>
-      <c r="G192" s="18" t="s">
+      <c r="G193" s="18" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" ht="15.9">
-      <c r="A193" s="13" t="s">
-        <v>858</v>
-      </c>
-      <c r="B193" s="13" t="s">
-        <v>859</v>
-      </c>
-      <c r="C193" s="10" t="s">
-        <v>2007</v>
-      </c>
-      <c r="D193" s="10" t="s">
-        <v>2448</v>
-      </c>
-      <c r="E193" s="14" t="s">
-        <v>860</v>
-      </c>
-      <c r="F193" s="14" t="s">
-        <v>861</v>
-      </c>
-      <c r="G193" s="14"/>
     </row>
     <row r="194" spans="1:7" ht="15.9">
       <c r="A194" s="13" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="E194" s="14" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="F194" s="14" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="G194" s="14"/>
     </row>
     <row r="195" spans="1:7" ht="15.9">
       <c r="A195" s="13" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D195" s="10" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="E195" s="14" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="F195" s="14" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="G195" s="14"/>
     </row>
     <row r="196" spans="1:7" ht="15.9">
       <c r="A196" s="13" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="C196" s="10" t="s">
-        <v>3414</v>
+        <v>2009</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>3416</v>
+        <v>2450</v>
       </c>
       <c r="E196" s="14" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="F196" s="14" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="G196" s="14"/>
     </row>
     <row r="197" spans="1:7" ht="15.9">
       <c r="A197" s="13" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C197" s="10" t="s">
-        <v>3415</v>
+        <v>3414</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>3417</v>
+        <v>3416</v>
       </c>
       <c r="E197" s="14" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="F197" s="14" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="G197" s="14"/>
     </row>
     <row r="198" spans="1:7" ht="15.9">
       <c r="A198" s="13" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="C198" s="10" t="s">
-        <v>2010</v>
+        <v>3415</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>2463</v>
+        <v>3417</v>
       </c>
       <c r="E198" s="14" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="F198" s="14" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="G198" s="14"/>
     </row>
     <row r="199" spans="1:7" ht="15.9">
       <c r="A199" s="13" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="E199" s="14" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="F199" s="14" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="G199" s="14"/>
     </row>
     <row r="200" spans="1:7" ht="15.9">
       <c r="A200" s="13" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C200" s="10" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D200" s="10" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="E200" s="14" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="F200" s="14" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="G200" s="14"/>
     </row>
     <row r="201" spans="1:7" ht="15.9">
       <c r="A201" s="13" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="C201" s="10" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D201" s="10" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="E201" s="14" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="F201" s="14" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="G201" s="14"/>
     </row>
     <row r="202" spans="1:7" ht="15.9">
       <c r="A202" s="13" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="C202" s="10" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>3365</v>
+        <v>2466</v>
       </c>
       <c r="E202" s="14" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="F202" s="14" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="G202" s="14"/>
     </row>
     <row r="203" spans="1:7" ht="15.9">
       <c r="A203" s="13" t="s">
+        <v>893</v>
+      </c>
+      <c r="B203" s="13" t="s">
+        <v>894</v>
+      </c>
+      <c r="C203" s="10" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D203" s="10" t="s">
+        <v>3365</v>
+      </c>
+      <c r="E203" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="F203" s="14" t="s">
+        <v>896</v>
+      </c>
+      <c r="G203" s="14"/>
+    </row>
+    <row r="204" spans="1:7" ht="15.9">
+      <c r="A204" s="13" t="s">
         <v>897</v>
       </c>
-      <c r="B203" s="13" t="s">
+      <c r="B204" s="13" t="s">
         <v>898</v>
       </c>
-      <c r="C203" s="10" t="s">
+      <c r="C204" s="10" t="s">
         <v>3363</v>
       </c>
-      <c r="D203" s="10" t="s">
+      <c r="D204" s="10" t="s">
         <v>3364</v>
       </c>
-      <c r="E203" s="14" t="s">
+      <c r="E204" s="14" t="s">
         <v>899</v>
       </c>
-      <c r="F203" s="14" t="s">
+      <c r="F204" s="14" t="s">
         <v>900</v>
       </c>
-      <c r="G203" s="14"/>
+      <c r="G204" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -25255,10 +25186,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+      <selection activeCell="A92" sqref="A92:E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -26734,45 +26665,45 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="29.15">
-      <c r="A92" s="14" t="s">
+    <row r="92" spans="1:6" s="58" customFormat="1" ht="15">
+      <c r="A92" s="59" t="s">
         <v>1070</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="59" t="s">
         <v>907</v>
       </c>
-      <c r="C92" s="24" t="s">
+      <c r="C92" s="59" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D92" s="59" t="s">
+        <v>5205</v>
+      </c>
+      <c r="E92" s="59" t="s">
+        <v>5207</v>
+      </c>
+      <c r="F92" s="59"/>
+    </row>
+    <row r="93" spans="1:6" s="58" customFormat="1" ht="15">
+      <c r="A93" s="59"/>
+      <c r="B93" s="59"/>
+      <c r="C93" s="59"/>
+      <c r="D93" s="59" t="s">
+        <v>5206</v>
+      </c>
+      <c r="E93" s="59" t="s">
+        <v>5208</v>
+      </c>
+      <c r="F93" s="59"/>
+    </row>
+    <row r="94" spans="1:6" ht="29.15">
+      <c r="A94" s="14" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>907</v>
+      </c>
+      <c r="C94" s="24" t="s">
         <v>2057</v>
-      </c>
-      <c r="D92" s="59" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E92" s="59" t="s">
-        <v>5195</v>
-      </c>
-      <c r="F92" s="14" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="15">
-      <c r="A93" s="14"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="59" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E93" s="59" t="s">
-        <v>5193</v>
-      </c>
-      <c r="F93" s="14" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="15">
-      <c r="A94" s="14"/>
-      <c r="B94" s="14"/>
-      <c r="C94" s="14" t="s">
-        <v>2058</v>
       </c>
       <c r="D94" s="59" t="s">
         <v>1076</v>
@@ -26785,66 +26716,96 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="15">
-      <c r="A95" s="14" t="s">
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="59" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E95" s="59" t="s">
+        <v>5193</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15">
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14" t="s">
+        <v>2058</v>
+      </c>
+      <c r="D96" s="59" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E96" s="59" t="s">
+        <v>5195</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="15">
+      <c r="A97" s="14" t="s">
         <v>1080</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B97" s="14" t="s">
         <v>902</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C97" s="14" t="s">
         <v>1081</v>
       </c>
-      <c r="D95" s="14" t="s">
+      <c r="D97" s="14" t="s">
         <v>1082</v>
       </c>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14" t="s">
+      <c r="E97" s="14"/>
+      <c r="F97" s="14" t="s">
         <v>1083</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15">
-      <c r="A97" s="31" t="s">
+    <row r="99" spans="1:6" ht="15">
+      <c r="A99" s="31" t="s">
         <v>3928</v>
       </c>
-      <c r="B97" s="31" t="s">
+      <c r="B99" s="31" t="s">
         <v>1948</v>
       </c>
-      <c r="C97" s="31"/>
-      <c r="D97" s="31" t="s">
-        <v>3929</v>
-      </c>
-      <c r="E97" s="31" t="s">
-        <v>3934</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15">
-      <c r="A98" s="31"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="31"/>
-      <c r="D98" s="31" t="s">
-        <v>3930</v>
-      </c>
-      <c r="E98" s="31" t="s">
-        <v>3932</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="15">
-      <c r="A99" s="31"/>
-      <c r="B99" s="31"/>
       <c r="C99" s="31"/>
       <c r="D99" s="31" t="s">
-        <v>3931</v>
+        <v>3929</v>
       </c>
       <c r="E99" s="31" t="s">
-        <v>3933</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15">
+        <v>3934</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15">
       <c r="A100" s="31"/>
       <c r="B100" s="31"/>
       <c r="C100" s="31"/>
-      <c r="D100" s="31"/>
-      <c r="E100" s="31"/>
+      <c r="D100" s="31" t="s">
+        <v>3930</v>
+      </c>
+      <c r="E100" s="31" t="s">
+        <v>3932</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15">
+      <c r="A101" s="31"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="31"/>
+      <c r="D101" s="31" t="s">
+        <v>3931</v>
+      </c>
+      <c r="E101" s="31" t="s">
+        <v>3933</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="15">
+      <c r="A102" s="31"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="31"/>
+      <c r="D102" s="31"/>
+      <c r="E102" s="31"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -26858,7 +26819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chapter 11 update translation
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -16826,8 +16826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BZ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -34351,8 +34351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>

</xml_diff>

<commit_message>
First side quest chapter scene done
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -39,7 +39,7 @@
     <sheet name="常見生詞" sheetId="19" r:id="rId25"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'names-名前'!$A$1:$H$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'names-名前'!$A$1:$H$81</definedName>
     <definedName name="skill" localSheetId="4">'Skills-スキル'!$A$1:$G$303</definedName>
     <definedName name="state" localSheetId="8">Sheet2!$A$1:$C$117</definedName>
     <definedName name="Unit_Command_1" localSheetId="5">'Unit Command'!$F$21:$F$70</definedName>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7322" uniqueCount="5242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7329" uniqueCount="5247">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16026,9 +16026,6 @@
     <t>A class that can raise ally stats. Incredibly weak.</t>
   </si>
   <si>
-    <t>sent this item to the convoy?</t>
-  </si>
-  <si>
     <t>Send this item to the convoy?</t>
   </si>
   <si>
@@ -16066,6 +16063,24 @@
   </si>
   <si>
     <t>to receive that.</t>
+  </si>
+  <si>
+    <t>病院の少女</t>
+  </si>
+  <si>
+    <t>Characters</t>
+  </si>
+  <si>
+    <t>Girl in Infirmary</t>
+  </si>
+  <si>
+    <t>村の治癒師</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girl in Infirmary </t>
+  </si>
+  <si>
+    <t>Village Doctor</t>
   </si>
 </sst>
 </file>
@@ -16384,7 +16399,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyAlignment="1">
@@ -16538,6 +16553,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16905,10 +16922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ69"/>
+  <dimension ref="A1:BZ70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -16955,8 +16972,10 @@
       <c r="L2" s="44"/>
     </row>
     <row r="3" spans="1:78" s="77" customFormat="1" ht="15.9">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
+      <c r="A3" s="37" t="s">
+        <v>5242</v>
+      </c>
+      <c r="B3" s="44"/>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
       <c r="E3" s="57"/>
@@ -17035,9 +17054,13 @@
       <c r="BZ3" s="55"/>
     </row>
     <row r="4" spans="1:78" ht="15.9">
-      <c r="A4" s="57"/>
+      <c r="A4" s="57" t="s">
+        <v>5241</v>
+      </c>
       <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="C4" s="57" t="s">
+        <v>5243</v>
+      </c>
       <c r="D4" s="56"/>
       <c r="E4" s="56"/>
       <c r="F4" s="57"/>
@@ -17115,9 +17138,13 @@
       <c r="BZ4" s="54"/>
     </row>
     <row r="5" spans="1:78" ht="16.3" customHeight="1">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
+      <c r="A5" s="57" t="s">
+        <v>5244</v>
+      </c>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57" t="s">
+        <v>5246</v>
+      </c>
       <c r="D5" s="56"/>
       <c r="E5" s="56"/>
       <c r="F5" s="79"/>
@@ -17127,25 +17154,22 @@
       <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:78" ht="15.9">
-      <c r="A6" s="56" t="s">
-        <v>5225</v>
-      </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="57" t="s">
+        <v>3153</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>5228</v>
+      </c>
       <c r="F6" s="82"/>
       <c r="H6" s="73"/>
       <c r="I6" s="75"/>
     </row>
     <row r="7" spans="1:78" ht="15.9">
-      <c r="A7" s="57" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B7" s="57" t="s">
-        <v>1101</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>2503</v>
-      </c>
+      <c r="A7" s="92" t="s">
+        <v>5225</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
       <c r="D7" s="55"/>
       <c r="E7" s="84"/>
       <c r="F7" s="79"/>
@@ -17153,12 +17177,14 @@
       <c r="I7" s="75"/>
     </row>
     <row r="8" spans="1:78" ht="15.9">
-      <c r="A8" s="55"/>
-      <c r="B8" s="55" t="s">
-        <v>5231</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>5230</v>
+      <c r="A8" s="57" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>2503</v>
       </c>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
@@ -17167,27 +17193,29 @@
       <c r="I8" s="75"/>
     </row>
     <row r="9" spans="1:78" ht="15.9">
-      <c r="A9" s="57"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55" t="s">
+        <v>5230</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>5229</v>
+      </c>
       <c r="D9" s="56"/>
       <c r="E9" s="56"/>
       <c r="H9" s="73"/>
       <c r="I9" s="75"/>
     </row>
     <row r="10" spans="1:78" ht="15.9">
-      <c r="A10" s="55"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="55"/>
       <c r="E10" s="84"/>
       <c r="H10" s="73"/>
       <c r="I10" s="75"/>
     </row>
     <row r="11" spans="1:78" ht="15.9">
-      <c r="A11" s="55" t="s">
-        <v>2562</v>
-      </c>
+      <c r="A11" s="55"/>
       <c r="B11" s="55"/>
       <c r="C11" s="55"/>
       <c r="D11" s="55"/>
@@ -17196,12 +17224,10 @@
       <c r="I11" s="75"/>
     </row>
     <row r="12" spans="1:78" ht="15.9">
-      <c r="A12" s="55" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B12" s="55" t="s">
+      <c r="A12" s="91" t="s">
         <v>2562</v>
       </c>
+      <c r="B12" s="55"/>
       <c r="C12" s="55"/>
       <c r="D12" s="55"/>
       <c r="E12" s="84"/>
@@ -17210,14 +17236,12 @@
     </row>
     <row r="13" spans="1:78" ht="15.9">
       <c r="A13" s="55" t="s">
-        <v>5234</v>
+        <v>1229</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>5233</v>
-      </c>
-      <c r="C13" s="55" t="s">
-        <v>5235</v>
-      </c>
+        <v>2562</v>
+      </c>
+      <c r="C13" s="55"/>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
       <c r="H13" s="73"/>
@@ -17225,37 +17249,39 @@
     </row>
     <row r="14" spans="1:78" ht="15.9">
       <c r="A14" s="55" t="s">
-        <v>1238</v>
+        <v>5233</v>
       </c>
       <c r="B14" s="55" t="s">
-        <v>3334</v>
-      </c>
-      <c r="C14" s="55"/>
+        <v>5232</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>5234</v>
+      </c>
       <c r="D14" s="55"/>
       <c r="E14" s="55"/>
       <c r="H14" s="73"/>
       <c r="I14" s="75"/>
     </row>
-    <row r="15" spans="1:78" ht="43.75">
-      <c r="A15" s="55"/>
-      <c r="B15" s="90" t="s">
-        <v>5236</v>
-      </c>
-      <c r="C15" s="90" t="s">
-        <v>5237</v>
-      </c>
+    <row r="15" spans="1:78" ht="15.9">
+      <c r="A15" s="55" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>3334</v>
+      </c>
+      <c r="C15" s="55"/>
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="H15" s="73"/>
       <c r="I15" s="75"/>
     </row>
-    <row r="16" spans="1:78" s="57" customFormat="1" ht="15.9">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56" t="s">
-        <v>5238</v>
-      </c>
-      <c r="C16" s="57" t="s">
-        <v>5240</v>
+    <row r="16" spans="1:78" s="57" customFormat="1" ht="43.75">
+      <c r="A16" s="55"/>
+      <c r="B16" s="90" t="s">
+        <v>5235</v>
+      </c>
+      <c r="C16" s="90" t="s">
+        <v>5236</v>
       </c>
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
@@ -17265,10 +17291,10 @@
     <row r="17" spans="1:9" s="57" customFormat="1" ht="15.9">
       <c r="A17" s="56"/>
       <c r="B17" s="56" t="s">
+        <v>5237</v>
+      </c>
+      <c r="C17" s="57" t="s">
         <v>5239</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>5241</v>
       </c>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
@@ -17276,27 +17302,29 @@
       <c r="I17" s="75"/>
     </row>
     <row r="18" spans="1:9" s="57" customFormat="1" ht="15.9">
-      <c r="A18" s="55"/>
-      <c r="B18" s="90"/>
-      <c r="C18" s="90"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56" t="s">
+        <v>5238</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>5240</v>
+      </c>
       <c r="D18" s="55"/>
       <c r="E18" s="55"/>
       <c r="H18" s="73"/>
       <c r="I18" s="75"/>
     </row>
     <row r="19" spans="1:9" ht="15.9">
-      <c r="A19" s="57"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="57"/>
       <c r="E19" s="55"/>
       <c r="H19" s="73"/>
       <c r="I19" s="75"/>
     </row>
     <row r="20" spans="1:9" ht="15.9">
-      <c r="A20" s="57" t="s">
-        <v>2505</v>
-      </c>
+      <c r="A20" s="57"/>
       <c r="B20" s="57"/>
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
@@ -17305,9 +17333,11 @@
       <c r="I20" s="75"/>
     </row>
     <row r="21" spans="1:9" ht="15.9">
-      <c r="C21" s="57" t="s">
-        <v>2084</v>
-      </c>
+      <c r="A21" s="37" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
       <c r="D21" s="57" t="s">
         <v>5226</v>
       </c>
@@ -17316,17 +17346,11 @@
       <c r="I21" s="75"/>
     </row>
     <row r="22" spans="1:9" ht="15.9">
-      <c r="A22" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>1911</v>
+      <c r="C22" s="57" t="s">
+        <v>2084</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>5232</v>
+        <v>5231</v>
       </c>
       <c r="E22" s="55"/>
       <c r="H22" s="73"/>
@@ -17334,14 +17358,12 @@
     </row>
     <row r="23" spans="1:9" ht="15.9">
       <c r="A23" s="13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>1912</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
         <v>2048</v>
       </c>
@@ -17350,6 +17372,15 @@
       <c r="I23" s="75"/>
     </row>
     <row r="24" spans="1:9" s="57" customFormat="1" ht="15.9">
+      <c r="A24" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>1912</v>
+      </c>
       <c r="E24" s="55"/>
       <c r="F24" s="31"/>
       <c r="H24" s="73"/>
@@ -17363,20 +17394,13 @@
       <c r="E25" s="55"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="57" t="s">
-        <v>3153</v>
-      </c>
-      <c r="B26" s="57" t="s">
-        <v>5228</v>
-      </c>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="57"/>
       <c r="D26" s="57"/>
       <c r="E26" s="55"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="55"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
       <c r="D27" s="54"/>
       <c r="E27" s="55"/>
       <c r="F27" s="57"/>
@@ -17410,9 +17434,7 @@
       <c r="E31" s="55"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="55" t="s">
-        <v>5229</v>
-      </c>
+      <c r="A32" s="55"/>
       <c r="B32" s="55"/>
       <c r="C32" s="55"/>
       <c r="D32" s="54"/>
@@ -17432,9 +17454,9 @@
       <c r="D34" s="55"/>
       <c r="E34" s="55"/>
     </row>
-    <row r="35" spans="1:5" ht="15.9">
-      <c r="A35" s="82"/>
-      <c r="B35" s="83"/>
+    <row r="35" spans="1:5">
+      <c r="A35" s="55"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="55"/>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
@@ -17442,28 +17464,28 @@
     <row r="36" spans="1:5" ht="15.9">
       <c r="A36" s="82"/>
       <c r="B36" s="83"/>
-      <c r="C36" s="88"/>
+      <c r="C36" s="55"/>
       <c r="D36" s="88"/>
       <c r="E36" s="55"/>
     </row>
     <row r="37" spans="1:5" ht="15.9">
       <c r="A37" s="82"/>
       <c r="B37" s="83"/>
-      <c r="C37" s="55"/>
+      <c r="C37" s="88"/>
       <c r="D37" s="55"/>
       <c r="E37" s="55"/>
     </row>
     <row r="38" spans="1:5" ht="15.9">
       <c r="A38" s="82"/>
       <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
+      <c r="C38" s="55"/>
       <c r="D38" s="83"/>
       <c r="E38" s="55"/>
     </row>
     <row r="39" spans="1:5" ht="15.9">
       <c r="A39" s="82"/>
       <c r="B39" s="83"/>
-      <c r="C39" s="85"/>
+      <c r="C39" s="83"/>
       <c r="D39" s="85"/>
       <c r="E39" s="55"/>
     </row>
@@ -17477,13 +17499,13 @@
     <row r="41" spans="1:5" ht="15.9">
       <c r="A41" s="82"/>
       <c r="B41" s="83"/>
-      <c r="C41" s="55"/>
+      <c r="C41" s="85"/>
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="55"/>
-      <c r="B42" s="55"/>
+    <row r="42" spans="1:5" ht="15.9">
+      <c r="A42" s="82"/>
+      <c r="B42" s="83"/>
       <c r="C42" s="55"/>
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
@@ -17503,7 +17525,7 @@
       <c r="E44" s="55"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="89"/>
+      <c r="A45" s="55"/>
       <c r="B45" s="55"/>
       <c r="C45" s="55"/>
       <c r="D45" s="55"/>
@@ -17516,32 +17538,32 @@
       <c r="D46" s="55"/>
       <c r="E46" s="55"/>
     </row>
-    <row r="47" spans="1:5" ht="15">
-      <c r="A47" s="55"/>
-      <c r="B47" s="87"/>
-      <c r="C47" s="87"/>
+    <row r="47" spans="1:5">
+      <c r="A47" s="89"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" ht="15">
       <c r="A48" s="55"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="87"/>
       <c r="D48" s="55"/>
       <c r="E48" s="55"/>
     </row>
-    <row r="49" spans="1:6" ht="15">
-      <c r="A49" s="85"/>
-      <c r="B49" s="86"/>
+    <row r="49" spans="1:6">
+      <c r="A49" s="55"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="55"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55"/>
       <c r="F49" s="57"/>
     </row>
     <row r="50" spans="1:6" ht="15.9">
-      <c r="A50" s="83"/>
-      <c r="B50" s="83"/>
-      <c r="C50" s="83"/>
+      <c r="A50" s="85"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="55"/>
       <c r="D50" s="83"/>
       <c r="E50" s="55"/>
     </row>
@@ -17573,10 +17595,10 @@
       <c r="D54" s="83"/>
       <c r="E54" s="55"/>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="55"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
+    <row r="55" spans="1:6" ht="15.9">
+      <c r="A55" s="83"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="83"/>
       <c r="D55" s="55"/>
       <c r="E55" s="55"/>
     </row>
@@ -17672,11 +17694,16 @@
       <c r="E68" s="55"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="77"/>
-      <c r="B69" s="77"/>
-      <c r="C69" s="77"/>
+      <c r="A69" s="55"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="55"/>
       <c r="D69" s="77"/>
       <c r="E69" s="77"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="77"/>
+      <c r="B70" s="77"/>
+      <c r="C70" s="77"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32926,7 +32953,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
@@ -33974,18 +34001,18 @@
     </row>
     <row r="37" spans="1:3" ht="15">
       <c r="B37" t="s">
-        <v>5238</v>
+        <v>5237</v>
       </c>
       <c r="C37" s="57" t="s">
-        <v>5240</v>
+        <v>5239</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="B38" t="s">
-        <v>5239</v>
+        <v>5238</v>
       </c>
       <c r="C38" s="57" t="s">
-        <v>5241</v>
+        <v>5240</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.6">
@@ -34685,10 +34712,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F81" sqref="A81:F81"/>
+    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="C20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -35079,41 +35106,33 @@
       </c>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="15">
-      <c r="A20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14" t="s">
-        <v>1951</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="14"/>
-    </row>
-    <row r="21" spans="1:8" ht="15">
-      <c r="A21" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14" t="s">
-        <v>2170</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" s="14"/>
+    <row r="20" spans="1:8" s="56" customFormat="1" ht="15">
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57" t="s">
+        <v>5244</v>
+      </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57" t="s">
+        <v>5246</v>
+      </c>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+    </row>
+    <row r="21" spans="1:8" s="56" customFormat="1" ht="15">
+      <c r="A21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57" t="s">
+        <v>5241</v>
+      </c>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57" t="s">
+        <v>5245</v>
+      </c>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
     </row>
     <row r="22" spans="1:8" ht="15">
       <c r="A22" s="14" t="s">
@@ -35121,15 +35140,15 @@
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H22" s="14"/>
     </row>
@@ -35139,15 +35158,15 @@
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>1953</v>
+        <v>2170</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H23" s="14"/>
     </row>
@@ -35157,15 +35176,15 @@
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H24" s="14"/>
     </row>
@@ -35175,14 +35194,15 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14" t="s">
-        <v>1956</v>
-      </c>
+        <v>1953</v>
+      </c>
+      <c r="F25" s="14"/>
       <c r="G25" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H25" s="14"/>
     </row>
@@ -35192,15 +35212,15 @@
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14" t="s">
-        <v>2629</v>
+        <v>1955</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H26" s="14"/>
     </row>
@@ -35210,15 +35230,14 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14" t="s">
-        <v>2171</v>
-      </c>
-      <c r="F27" s="14"/>
+        <v>1956</v>
+      </c>
       <c r="G27" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H27" s="14"/>
     </row>
@@ -35228,127 +35247,115 @@
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14" t="s">
-        <v>2172</v>
+        <v>2629</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29" spans="1:8" ht="15">
+      <c r="A29" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14" t="s">
+        <v>2171</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" ht="15">
+      <c r="A30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="14"/>
-    </row>
-    <row r="29" spans="1:8" ht="15">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31" t="s">
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" ht="15">
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31" t="s">
+      <c r="D31" s="31"/>
+      <c r="E31" s="31" t="s">
         <v>2198</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="1:8" s="56" customFormat="1" ht="15">
-      <c r="A30" s="57"/>
-      <c r="B30" s="57" t="s">
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+    </row>
+    <row r="32" spans="1:8" s="56" customFormat="1" ht="15">
+      <c r="A32" s="57"/>
+      <c r="B32" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C32" s="57" t="s">
         <v>5118</v>
       </c>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57" t="s">
+      <c r="D32" s="57"/>
+      <c r="E32" s="57" t="s">
         <v>5119</v>
       </c>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-    </row>
-    <row r="31" spans="1:8" s="56" customFormat="1" ht="15">
-      <c r="A31" s="57"/>
-      <c r="B31" s="57" t="s">
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+    </row>
+    <row r="33" spans="1:8" s="56" customFormat="1" ht="15">
+      <c r="A33" s="57"/>
+      <c r="B33" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C33" s="57" t="s">
         <v>5109</v>
       </c>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57" t="s">
+      <c r="D33" s="57"/>
+      <c r="E33" s="57" t="s">
         <v>5110</v>
       </c>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-    </row>
-    <row r="32" spans="1:8" ht="15">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31" t="s">
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+    </row>
+    <row r="34" spans="1:8" ht="15">
+      <c r="A34" s="31"/>
+      <c r="B34" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C34" s="31" t="s">
         <v>3373</v>
       </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31" t="s">
+      <c r="D34" s="31"/>
+      <c r="E34" s="31" t="s">
         <v>3374</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-    </row>
-    <row r="33" spans="1:8" ht="15">
-      <c r="A33" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>2113</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>2174</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>2209</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H33" s="14"/>
-    </row>
-    <row r="34" spans="1:8" ht="15">
-      <c r="A34" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>2114</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>2175</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>2208</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H34" s="14"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
     </row>
     <row r="35" spans="1:8" ht="15">
       <c r="A35" s="14" t="s">
@@ -35358,15 +35365,19 @@
         <v>63</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="14"/>
+        <v>64</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>2113</v>
+      </c>
       <c r="E35" s="14" t="s">
-        <v>2176</v>
-      </c>
-      <c r="F35" s="14"/>
+        <v>2174</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>2209</v>
+      </c>
       <c r="G35" s="14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H35" s="14"/>
     </row>
@@ -35375,22 +35386,22 @@
         <v>62</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>2644</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>71</v>
+        <v>2208</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="H36" s="14"/>
     </row>
@@ -35399,22 +35410,18 @@
         <v>62</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>2116</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D37" s="14"/>
       <c r="E37" s="14" t="s">
-        <v>2178</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>4736</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>73</v>
+        <v>2176</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="H37" s="14"/>
     </row>
@@ -35426,41 +35433,45 @@
         <v>7</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>2179</v>
+        <v>2177</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>2488</v>
+        <v>2644</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="15">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31" t="s">
+      <c r="A39" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="31" t="s">
-        <v>2647</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>2645</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>3353</v>
-      </c>
-      <c r="F39" s="31" t="s">
-        <v>2646</v>
-      </c>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
+      <c r="C39" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>4736</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="15">
       <c r="A40" s="14" t="s">
@@ -35470,67 +35481,63 @@
         <v>7</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>4661</v>
+        <v>2488</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="15">
-      <c r="A41" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>2119</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>2183</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>4737</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H41" s="14"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>2647</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>2645</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>3353</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>2646</v>
+      </c>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
     </row>
     <row r="42" spans="1:8" ht="15">
       <c r="A42" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>2183</v>
+        <v>2180</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>2496</v>
+        <v>4661</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H42" s="14"/>
     </row>
@@ -35542,19 +35549,19 @@
         <v>23</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>2467</v>
+        <v>2183</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>2489</v>
+        <v>4737</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H43" s="14"/>
     </row>
@@ -35566,19 +35573,19 @@
         <v>23</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>2181</v>
+        <v>2183</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>4738</v>
+        <v>2496</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H44" s="14"/>
     </row>
@@ -35590,19 +35597,19 @@
         <v>23</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>2182</v>
+        <v>2467</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>5185</v>
+        <v>2489</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H45" s="14"/>
     </row>
@@ -35611,22 +35618,22 @@
         <v>62</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>2173</v>
+        <v>2181</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>2490</v>
+        <v>4738</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H46" s="14"/>
     </row>
@@ -35635,22 +35642,22 @@
         <v>62</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>2184</v>
-      </c>
-      <c r="F47" s="31" t="s">
-        <v>3356</v>
-      </c>
-      <c r="G47" s="27" t="s">
-        <v>89</v>
+        <v>2182</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>5185</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="H47" s="14"/>
     </row>
@@ -35662,19 +35669,19 @@
         <v>10</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>2185</v>
-      </c>
-      <c r="F48" s="31" t="s">
-        <v>3355</v>
+        <v>2173</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>2490</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H48" s="14"/>
     </row>
@@ -35686,19 +35693,19 @@
         <v>10</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>2186</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>4739</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>93</v>
+        <v>2184</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>3356</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="H49" s="14"/>
     </row>
@@ -35707,22 +35714,22 @@
         <v>62</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>3301</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>3425</v>
+        <v>2185</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>3355</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H50" s="14"/>
     </row>
@@ -35731,22 +35738,22 @@
         <v>62</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>2199</v>
+        <v>2186</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>2491</v>
+        <v>4739</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H51" s="14"/>
     </row>
@@ -35758,19 +35765,19 @@
         <v>15</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>3369</v>
+        <v>3301</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>2492</v>
+        <v>3425</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H52" s="14"/>
     </row>
@@ -35782,19 +35789,19 @@
         <v>15</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>2493</v>
+        <v>2491</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H53" s="14"/>
     </row>
@@ -35806,19 +35813,19 @@
         <v>15</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>2205</v>
+        <v>3369</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H54" s="14"/>
     </row>
@@ -35830,19 +35837,19 @@
         <v>15</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>2198</v>
+        <v>2200</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>3382</v>
+        <v>2493</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H55" s="14"/>
     </row>
@@ -35851,22 +35858,22 @@
         <v>62</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>2201</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>4733</v>
+        <v>2205</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>2494</v>
       </c>
       <c r="G56" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H56" s="14"/>
     </row>
@@ -35875,22 +35882,22 @@
         <v>62</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>1835</v>
+        <v>2133</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>2202</v>
+        <v>2198</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>4734</v>
+        <v>3382</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H57" s="14"/>
     </row>
@@ -35899,22 +35906,22 @@
         <v>62</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="F58" s="31" t="s">
-        <v>3357</v>
+        <v>4733</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H58" s="14"/>
     </row>
@@ -35926,19 +35933,19 @@
         <v>109</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>2136</v>
+        <v>1835</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>2495</v>
+        <v>4734</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H59" s="14"/>
     </row>
@@ -35950,19 +35957,19 @@
         <v>109</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>3370</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>4735</v>
+        <v>2202</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>3357</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H60" s="14"/>
     </row>
@@ -35974,19 +35981,19 @@
         <v>109</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>2138</v>
+        <v>2136</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>4296</v>
+        <v>2495</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H61" s="14"/>
     </row>
@@ -35995,46 +36002,46 @@
         <v>62</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>2139</v>
+        <v>2137</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>2191</v>
-      </c>
-      <c r="F62" s="57" t="s">
-        <v>4849</v>
+        <v>3370</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>4735</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="15">
       <c r="A63" s="14" t="s">
-        <v>1836</v>
+        <v>62</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>1837</v>
+        <v>2138</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>3922</v>
+        <v>2204</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>4760</v>
+        <v>4296</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H63" s="14"/>
     </row>
@@ -36046,43 +36053,43 @@
         <v>118</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>3922</v>
+        <v>2191</v>
       </c>
       <c r="F64" s="57" t="s">
-        <v>4761</v>
+        <v>4849</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H64" s="14"/>
     </row>
     <row r="65" spans="1:8" ht="15">
       <c r="A65" s="14" t="s">
-        <v>62</v>
+        <v>1836</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>118</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>2141</v>
+        <v>1837</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>2197</v>
-      </c>
-      <c r="F65" s="57" t="s">
-        <v>4844</v>
+        <v>3922</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>4760</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H65" s="14"/>
     </row>
@@ -36094,19 +36101,19 @@
         <v>118</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>2196</v>
-      </c>
-      <c r="F66" s="14" t="s">
-        <v>4841</v>
+        <v>3922</v>
+      </c>
+      <c r="F66" s="57" t="s">
+        <v>4761</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H66" s="14"/>
     </row>
@@ -36118,19 +36125,19 @@
         <v>118</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>2143</v>
+        <v>2141</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>4762</v>
-      </c>
-      <c r="F67" s="14" t="s">
-        <v>4825</v>
+        <v>2197</v>
+      </c>
+      <c r="F67" s="57" t="s">
+        <v>4844</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H67" s="14"/>
     </row>
@@ -36139,22 +36146,22 @@
         <v>62</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>1838</v>
+        <v>118</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>2144</v>
+        <v>2142</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>2180</v>
+        <v>2196</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>4826</v>
+        <v>4841</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="H68" s="14"/>
     </row>
@@ -36166,19 +36173,19 @@
         <v>118</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>2145</v>
+        <v>2143</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>2192</v>
+        <v>4762</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>4842</v>
+        <v>4825</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H69" s="14"/>
     </row>
@@ -36187,22 +36194,22 @@
         <v>62</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>131</v>
+        <v>1838</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>2146</v>
+        <v>2144</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>2193</v>
+        <v>2180</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>4887</v>
+        <v>4826</v>
       </c>
       <c r="G70" s="14" t="s">
-        <v>133</v>
+        <v>77</v>
       </c>
       <c r="H70" s="14"/>
     </row>
@@ -36211,22 +36218,22 @@
         <v>62</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>2194</v>
-      </c>
-      <c r="F71" s="57" t="s">
-        <v>4887</v>
+        <v>2192</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>4842</v>
       </c>
       <c r="G71" s="14" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H71" s="14"/>
     </row>
@@ -36238,19 +36245,19 @@
         <v>131</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>2195</v>
+        <v>2193</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>4889</v>
+        <v>4887</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H72" s="14"/>
     </row>
@@ -36262,19 +36269,19 @@
         <v>131</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>2148</v>
+        <v>2146</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>2190</v>
+        <v>2194</v>
       </c>
       <c r="F73" s="57" t="s">
-        <v>4888</v>
+        <v>4887</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H73" s="14"/>
     </row>
@@ -36286,19 +36293,19 @@
         <v>131</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>2149</v>
+        <v>2147</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>5145</v>
+        <v>2195</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>4890</v>
+        <v>4889</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H74" s="14"/>
     </row>
@@ -36310,19 +36317,19 @@
         <v>131</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>2150</v>
+        <v>2148</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>2188</v>
-      </c>
-      <c r="F75" s="14" t="s">
-        <v>4891</v>
+        <v>2190</v>
+      </c>
+      <c r="F75" s="57" t="s">
+        <v>4888</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H75" s="14"/>
     </row>
@@ -36331,18 +36338,22 @@
         <v>62</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D76" s="14"/>
+        <v>140</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>2149</v>
+      </c>
       <c r="E76" s="14" t="s">
-        <v>2189</v>
-      </c>
-      <c r="F76" s="14"/>
+        <v>5145</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>4890</v>
+      </c>
       <c r="G76" s="14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H76" s="14"/>
     </row>
@@ -36351,22 +36362,22 @@
         <v>62</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>2187</v>
+        <v>2188</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>5172</v>
+        <v>4891</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H77" s="14"/>
     </row>
@@ -36375,22 +36386,18 @@
         <v>62</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>2152</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D78" s="14"/>
       <c r="E78" s="14" t="s">
-        <v>2206</v>
-      </c>
-      <c r="F78" s="14" t="s">
-        <v>3445</v>
-      </c>
+        <v>2189</v>
+      </c>
+      <c r="F78" s="14"/>
       <c r="G78" s="14" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H78" s="14"/>
     </row>
@@ -36399,56 +36406,104 @@
         <v>62</v>
       </c>
       <c r="B79" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>2151</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>2187</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>5172</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="H79" s="14"/>
+    </row>
+    <row r="80" spans="1:8" ht="15">
+      <c r="A80" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C80" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>2152</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>2206</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>3445</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="H80" s="14"/>
+    </row>
+    <row r="81" spans="1:8" ht="15">
+      <c r="A81" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C81" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D81" s="14" t="s">
         <v>2153</v>
       </c>
-      <c r="E79" s="14" t="s">
+      <c r="E81" s="14" t="s">
         <v>2207</v>
       </c>
-      <c r="F79" s="14" t="s">
+      <c r="F81" s="14" t="s">
         <v>4829</v>
       </c>
-      <c r="G79" s="14" t="s">
+      <c r="G81" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H79" s="14"/>
-    </row>
-    <row r="80" spans="1:8" ht="15">
-      <c r="C80" s="64" t="s">
+      <c r="H81" s="14"/>
+    </row>
+    <row r="82" spans="1:8" ht="15">
+      <c r="C82" s="64" t="s">
         <v>5186</v>
       </c>
-      <c r="D80" s="64"/>
-      <c r="E80" s="64" t="s">
+      <c r="D82" s="64"/>
+      <c r="E82" s="64" t="s">
         <v>5187</v>
       </c>
-      <c r="F80" s="57" t="s">
+      <c r="F82" s="57" t="s">
         <v>4828</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="15">
-      <c r="B81" s="57" t="s">
+    <row r="83" spans="1:8" ht="15">
+      <c r="B83" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>5204</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D83" t="s">
         <v>5205</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E83" t="s">
         <v>5206</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F83" t="s">
         <v>5207</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H79"/>
+  <autoFilter ref="A1:H81"/>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
First sidequest 90% done!
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -16071,9 +16071,6 @@
     <t>Characters</t>
   </si>
   <si>
-    <t>Girl in Infirmary</t>
-  </si>
-  <si>
     <t>村の治癒師</t>
   </si>
   <si>
@@ -16081,6 +16078,9 @@
   </si>
   <si>
     <t>Village Doctor</t>
+  </si>
+  <si>
+    <t>Infirmary Girl</t>
   </si>
 </sst>
 </file>
@@ -16925,7 +16925,7 @@
   <dimension ref="A1:BZ70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -17059,7 +17059,7 @@
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="57" t="s">
-        <v>5243</v>
+        <v>5246</v>
       </c>
       <c r="D4" s="56"/>
       <c r="E4" s="56"/>
@@ -17139,11 +17139,11 @@
     </row>
     <row r="5" spans="1:78" ht="16.3" customHeight="1">
       <c r="A5" s="57" t="s">
-        <v>5244</v>
+        <v>5243</v>
       </c>
       <c r="B5" s="57"/>
       <c r="C5" s="57" t="s">
-        <v>5246</v>
+        <v>5245</v>
       </c>
       <c r="D5" s="56"/>
       <c r="E5" s="56"/>
@@ -35110,11 +35110,11 @@
       <c r="A20" s="57"/>
       <c r="B20" s="57"/>
       <c r="C20" s="57" t="s">
-        <v>5244</v>
+        <v>5243</v>
       </c>
       <c r="D20" s="57"/>
       <c r="E20" s="57" t="s">
-        <v>5246</v>
+        <v>5245</v>
       </c>
       <c r="F20" s="57"/>
       <c r="G20" s="57"/>
@@ -35128,7 +35128,7 @@
       </c>
       <c r="D21" s="57"/>
       <c r="E21" s="57" t="s">
-        <v>5245</v>
+        <v>5244</v>
       </c>
       <c r="F21" s="57"/>
       <c r="G21" s="57"/>

</xml_diff>

<commit_message>
Next side quest translation in progress!
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7329" uniqueCount="5247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7331" uniqueCount="5249">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16081,6 +16081,12 @@
   </si>
   <si>
     <t>Infirmary Girl</t>
+  </si>
+  <si>
+    <t>盗賊団長</t>
+  </si>
+  <si>
+    <t>Bandit Leader</t>
   </si>
 </sst>
 </file>
@@ -16922,10 +16928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ70"/>
+  <dimension ref="A1:BZ71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -17137,96 +17143,167 @@
       <c r="BY4" s="54"/>
       <c r="BZ4" s="54"/>
     </row>
-    <row r="5" spans="1:78" ht="16.3" customHeight="1">
+    <row r="5" spans="1:78" s="57" customFormat="1" ht="15.9">
       <c r="A5" s="57" t="s">
-        <v>5243</v>
-      </c>
-      <c r="B5" s="57"/>
+        <v>5247</v>
+      </c>
       <c r="C5" s="57" t="s">
-        <v>5245</v>
+        <v>5248</v>
       </c>
       <c r="D5" s="56"/>
       <c r="E5" s="56"/>
-      <c r="F5" s="79"/>
+      <c r="G5" s="83"/>
       <c r="H5" s="73"/>
       <c r="I5" s="75"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-    </row>
-    <row r="6" spans="1:78" ht="15.9">
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
+      <c r="AE5" s="54"/>
+      <c r="AF5" s="54"/>
+      <c r="AG5" s="54"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="54"/>
+      <c r="AJ5" s="54"/>
+      <c r="AK5" s="54"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="54"/>
+      <c r="AN5" s="54"/>
+      <c r="AO5" s="54"/>
+      <c r="AP5" s="54"/>
+      <c r="AQ5" s="54"/>
+      <c r="AR5" s="54"/>
+      <c r="AS5" s="54"/>
+      <c r="AT5" s="54"/>
+      <c r="AU5" s="54"/>
+      <c r="AV5" s="54"/>
+      <c r="AW5" s="54"/>
+      <c r="AX5" s="54"/>
+      <c r="AY5" s="54"/>
+      <c r="AZ5" s="54"/>
+      <c r="BA5" s="54"/>
+      <c r="BB5" s="54"/>
+      <c r="BC5" s="54"/>
+      <c r="BD5" s="54"/>
+      <c r="BE5" s="54"/>
+      <c r="BF5" s="54"/>
+      <c r="BG5" s="54"/>
+      <c r="BH5" s="54"/>
+      <c r="BI5" s="54"/>
+      <c r="BJ5" s="54"/>
+      <c r="BK5" s="54"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="54"/>
+      <c r="BN5" s="54"/>
+      <c r="BO5" s="54"/>
+      <c r="BP5" s="54"/>
+      <c r="BQ5" s="54"/>
+      <c r="BR5" s="54"/>
+      <c r="BS5" s="54"/>
+      <c r="BT5" s="54"/>
+      <c r="BU5" s="54"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="54"/>
+      <c r="BX5" s="54"/>
+      <c r="BY5" s="54"/>
+      <c r="BZ5" s="54"/>
+    </row>
+    <row r="6" spans="1:78" ht="16.3" customHeight="1">
       <c r="A6" s="57" t="s">
-        <v>3153</v>
-      </c>
+        <v>5243</v>
+      </c>
+      <c r="B6" s="57"/>
       <c r="C6" s="57" t="s">
-        <v>5228</v>
-      </c>
-      <c r="F6" s="82"/>
+        <v>5245</v>
+      </c>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="79"/>
       <c r="H6" s="73"/>
       <c r="I6" s="75"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
     </row>
     <row r="7" spans="1:78" ht="15.9">
-      <c r="A7" s="92" t="s">
-        <v>5225</v>
-      </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="79"/>
+      <c r="A7" s="57" t="s">
+        <v>3153</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>5228</v>
+      </c>
+      <c r="F7" s="82"/>
       <c r="H7" s="73"/>
       <c r="I7" s="75"/>
     </row>
     <row r="8" spans="1:78" ht="15.9">
-      <c r="A8" s="57" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>1101</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>2503</v>
-      </c>
+      <c r="A8" s="92" t="s">
+        <v>5225</v>
+      </c>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="79"/>
       <c r="H8" s="73"/>
       <c r="I8" s="75"/>
     </row>
     <row r="9" spans="1:78" ht="15.9">
-      <c r="A9" s="55"/>
-      <c r="B9" s="55" t="s">
-        <v>5230</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>5229</v>
-      </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
+      <c r="A9" s="57" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
       <c r="H9" s="73"/>
       <c r="I9" s="75"/>
     </row>
     <row r="10" spans="1:78" ht="15.9">
-      <c r="A10" s="57"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="84"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="55" t="s">
+        <v>5230</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>5229</v>
+      </c>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
       <c r="H10" s="73"/>
       <c r="I10" s="75"/>
     </row>
     <row r="11" spans="1:78" ht="15.9">
-      <c r="A11" s="55"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="55"/>
       <c r="E11" s="84"/>
       <c r="H11" s="73"/>
       <c r="I11" s="75"/>
     </row>
     <row r="12" spans="1:78" ht="15.9">
-      <c r="A12" s="91" t="s">
-        <v>2562</v>
-      </c>
+      <c r="A12" s="55"/>
       <c r="B12" s="55"/>
       <c r="C12" s="55"/>
       <c r="D12" s="55"/>
@@ -17235,28 +17312,24 @@
       <c r="I12" s="75"/>
     </row>
     <row r="13" spans="1:78" ht="15.9">
-      <c r="A13" s="55" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B13" s="55" t="s">
+      <c r="A13" s="91" t="s">
         <v>2562</v>
       </c>
+      <c r="B13" s="55"/>
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
+      <c r="E13" s="84"/>
       <c r="H13" s="73"/>
       <c r="I13" s="75"/>
     </row>
     <row r="14" spans="1:78" ht="15.9">
       <c r="A14" s="55" t="s">
-        <v>5233</v>
+        <v>1229</v>
       </c>
       <c r="B14" s="55" t="s">
-        <v>5232</v>
-      </c>
-      <c r="C14" s="55" t="s">
-        <v>5234</v>
-      </c>
+        <v>2562</v>
+      </c>
+      <c r="C14" s="55"/>
       <c r="D14" s="55"/>
       <c r="E14" s="55"/>
       <c r="H14" s="73"/>
@@ -17264,37 +17337,39 @@
     </row>
     <row r="15" spans="1:78" ht="15.9">
       <c r="A15" s="55" t="s">
-        <v>1238</v>
+        <v>5233</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>3334</v>
-      </c>
-      <c r="C15" s="55"/>
+        <v>5232</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>5234</v>
+      </c>
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="H15" s="73"/>
       <c r="I15" s="75"/>
     </row>
-    <row r="16" spans="1:78" s="57" customFormat="1" ht="43.75">
-      <c r="A16" s="55"/>
-      <c r="B16" s="90" t="s">
-        <v>5235</v>
-      </c>
-      <c r="C16" s="90" t="s">
-        <v>5236</v>
-      </c>
+    <row r="16" spans="1:78" ht="15.9">
+      <c r="A16" s="55" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>3334</v>
+      </c>
+      <c r="C16" s="55"/>
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
       <c r="H16" s="73"/>
       <c r="I16" s="75"/>
     </row>
-    <row r="17" spans="1:9" s="57" customFormat="1" ht="15.9">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56" t="s">
-        <v>5237</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>5239</v>
+    <row r="17" spans="1:9" s="57" customFormat="1" ht="43.75">
+      <c r="A17" s="55"/>
+      <c r="B17" s="90" t="s">
+        <v>5235</v>
+      </c>
+      <c r="C17" s="90" t="s">
+        <v>5236</v>
       </c>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
@@ -17304,94 +17379,100 @@
     <row r="18" spans="1:9" s="57" customFormat="1" ht="15.9">
       <c r="A18" s="56"/>
       <c r="B18" s="56" t="s">
-        <v>5238</v>
+        <v>5237</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>5240</v>
+        <v>5239</v>
       </c>
       <c r="D18" s="55"/>
       <c r="E18" s="55"/>
       <c r="H18" s="73"/>
       <c r="I18" s="75"/>
     </row>
-    <row r="19" spans="1:9" ht="15.9">
-      <c r="A19" s="55"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="57"/>
+    <row r="19" spans="1:9" s="57" customFormat="1" ht="15.9">
+      <c r="A19" s="56"/>
+      <c r="B19" s="56" t="s">
+        <v>5238</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>5240</v>
+      </c>
+      <c r="D19" s="55"/>
       <c r="E19" s="55"/>
       <c r="H19" s="73"/>
       <c r="I19" s="75"/>
     </row>
     <row r="20" spans="1:9" ht="15.9">
-      <c r="A20" s="57"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
       <c r="D20" s="57"/>
       <c r="E20" s="55"/>
       <c r="H20" s="73"/>
       <c r="I20" s="75"/>
     </row>
     <row r="21" spans="1:9" ht="15.9">
-      <c r="A21" s="37" t="s">
-        <v>2505</v>
-      </c>
+      <c r="A21" s="57"/>
       <c r="B21" s="57"/>
       <c r="C21" s="57"/>
-      <c r="D21" s="57" t="s">
-        <v>5226</v>
-      </c>
+      <c r="D21" s="57"/>
       <c r="E21" s="55"/>
       <c r="H21" s="73"/>
       <c r="I21" s="75"/>
     </row>
     <row r="22" spans="1:9" ht="15.9">
-      <c r="C22" s="57" t="s">
-        <v>2084</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>5231</v>
+      <c r="A22" s="37" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57" t="s">
+        <v>5226</v>
       </c>
       <c r="E22" s="55"/>
       <c r="H22" s="73"/>
       <c r="I22" s="75"/>
     </row>
     <row r="23" spans="1:9" ht="15.9">
-      <c r="A23" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="57" t="s">
+        <v>2084</v>
+      </c>
       <c r="D23" s="10" t="s">
-        <v>2048</v>
+        <v>5231</v>
       </c>
       <c r="E23" s="55"/>
       <c r="H23" s="73"/>
       <c r="I23" s="75"/>
     </row>
-    <row r="24" spans="1:9" s="57" customFormat="1" ht="15.9">
+    <row r="24" spans="1:9" ht="15.9">
       <c r="A24" s="13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>1912</v>
+        <v>363</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>2048</v>
       </c>
       <c r="E24" s="55"/>
-      <c r="F24" s="31"/>
       <c r="H24" s="73"/>
       <c r="I24" s="75"/>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
+    <row r="25" spans="1:9" s="57" customFormat="1" ht="15.9">
+      <c r="A25" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>1912</v>
+      </c>
       <c r="E25" s="55"/>
+      <c r="F25" s="31"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="75"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="57"/>
@@ -17401,16 +17482,16 @@
       <c r="E26" s="55"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="D27" s="54"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="55"/>
-      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="55"/>
+      <c r="F28" s="57"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="55"/>
@@ -17430,7 +17511,7 @@
       <c r="A31" s="55"/>
       <c r="B31" s="55"/>
       <c r="C31" s="55"/>
-      <c r="D31" s="54"/>
+      <c r="D31" s="55"/>
       <c r="E31" s="55"/>
     </row>
     <row r="32" spans="1:9">
@@ -17440,19 +17521,19 @@
       <c r="D32" s="54"/>
       <c r="E32" s="55"/>
     </row>
-    <row r="33" spans="1:5" ht="15.9">
+    <row r="33" spans="1:5">
       <c r="A33" s="55"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="83"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="D33" s="54"/>
+      <c r="E33" s="55"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.9">
       <c r="A34" s="55"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
+      <c r="E34" s="83"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="55"/>
@@ -17461,38 +17542,38 @@
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
     </row>
-    <row r="36" spans="1:5" ht="15.9">
-      <c r="A36" s="82"/>
-      <c r="B36" s="83"/>
+    <row r="36" spans="1:5">
+      <c r="A36" s="55"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="55"/>
-      <c r="D36" s="88"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="55"/>
     </row>
     <row r="37" spans="1:5" ht="15.9">
       <c r="A37" s="82"/>
       <c r="B37" s="83"/>
-      <c r="C37" s="88"/>
-      <c r="D37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="88"/>
       <c r="E37" s="55"/>
     </row>
     <row r="38" spans="1:5" ht="15.9">
       <c r="A38" s="82"/>
       <c r="B38" s="83"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="83"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="55"/>
       <c r="E38" s="55"/>
     </row>
     <row r="39" spans="1:5" ht="15.9">
       <c r="A39" s="82"/>
       <c r="B39" s="83"/>
-      <c r="C39" s="83"/>
-      <c r="D39" s="85"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="83"/>
       <c r="E39" s="55"/>
     </row>
     <row r="40" spans="1:5" ht="15.9">
       <c r="A40" s="82"/>
       <c r="B40" s="83"/>
-      <c r="C40" s="85"/>
+      <c r="C40" s="83"/>
       <c r="D40" s="85"/>
       <c r="E40" s="55"/>
     </row>
@@ -17500,19 +17581,19 @@
       <c r="A41" s="82"/>
       <c r="B41" s="83"/>
       <c r="C41" s="85"/>
-      <c r="D41" s="55"/>
+      <c r="D41" s="85"/>
       <c r="E41" s="55"/>
     </row>
     <row r="42" spans="1:5" ht="15.9">
       <c r="A42" s="82"/>
       <c r="B42" s="83"/>
-      <c r="C42" s="55"/>
+      <c r="C42" s="85"/>
       <c r="D42" s="55"/>
       <c r="E42" s="55"/>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="55"/>
-      <c r="B43" s="55"/>
+    <row r="43" spans="1:5" ht="15.9">
+      <c r="A43" s="82"/>
+      <c r="B43" s="83"/>
       <c r="C43" s="55"/>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
@@ -17532,7 +17613,7 @@
       <c r="E45" s="55"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="89"/>
+      <c r="A46" s="55"/>
       <c r="B46" s="55"/>
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
@@ -17545,32 +17626,32 @@
       <c r="D47" s="55"/>
       <c r="E47" s="55"/>
     </row>
-    <row r="48" spans="1:5" ht="15">
-      <c r="A48" s="55"/>
-      <c r="B48" s="87"/>
-      <c r="C48" s="87"/>
+    <row r="48" spans="1:5">
+      <c r="A48" s="89"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="55"/>
       <c r="D48" s="55"/>
       <c r="E48" s="55"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" ht="15">
       <c r="A49" s="55"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="87"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55"/>
-      <c r="F49" s="57"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.9">
-      <c r="A50" s="85"/>
-      <c r="B50" s="86"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="55"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="55"/>
-      <c r="D50" s="83"/>
+      <c r="D50" s="55"/>
       <c r="E50" s="55"/>
+      <c r="F50" s="57"/>
     </row>
     <row r="51" spans="1:6" ht="15.9">
-      <c r="A51" s="83"/>
-      <c r="B51" s="83"/>
-      <c r="C51" s="83"/>
+      <c r="A51" s="85"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="55"/>
       <c r="D51" s="83"/>
       <c r="E51" s="55"/>
     </row>
@@ -17599,13 +17680,13 @@
       <c r="A55" s="83"/>
       <c r="B55" s="83"/>
       <c r="C55" s="83"/>
-      <c r="D55" s="55"/>
+      <c r="D55" s="83"/>
       <c r="E55" s="55"/>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="55"/>
-      <c r="B56" s="55"/>
-      <c r="C56" s="55"/>
+    <row r="56" spans="1:6" ht="15.9">
+      <c r="A56" s="83"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="83"/>
       <c r="D56" s="55"/>
       <c r="E56" s="55"/>
     </row>
@@ -17697,13 +17778,20 @@
       <c r="A69" s="55"/>
       <c r="B69" s="55"/>
       <c r="C69" s="55"/>
-      <c r="D69" s="77"/>
-      <c r="E69" s="77"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="77"/>
-      <c r="B70" s="77"/>
-      <c r="C70" s="77"/>
+      <c r="A70" s="55"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="77"/>
+      <c r="E70" s="77"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="77"/>
+      <c r="B71" s="77"/>
+      <c r="C71" s="77"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bandit game over event
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7331" uniqueCount="5249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7333" uniqueCount="5249">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16928,10 +16928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ71"/>
+  <dimension ref="A1:BZ72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -17145,10 +17145,10 @@
     </row>
     <row r="5" spans="1:78" s="57" customFormat="1" ht="15.9">
       <c r="A5" s="57" t="s">
-        <v>5247</v>
+        <v>2722</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>5248</v>
+        <v>3159</v>
       </c>
       <c r="D5" s="56"/>
       <c r="E5" s="56"/>
@@ -17225,96 +17225,167 @@
       <c r="BY5" s="54"/>
       <c r="BZ5" s="54"/>
     </row>
-    <row r="6" spans="1:78" ht="16.3" customHeight="1">
+    <row r="6" spans="1:78" s="57" customFormat="1" ht="15.9">
       <c r="A6" s="57" t="s">
-        <v>5243</v>
-      </c>
-      <c r="B6" s="57"/>
+        <v>5247</v>
+      </c>
       <c r="C6" s="57" t="s">
-        <v>5245</v>
+        <v>5248</v>
       </c>
       <c r="D6" s="56"/>
       <c r="E6" s="56"/>
-      <c r="F6" s="79"/>
+      <c r="G6" s="83"/>
       <c r="H6" s="73"/>
       <c r="I6" s="75"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-    </row>
-    <row r="7" spans="1:78" ht="15.9">
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
+      <c r="X6" s="54"/>
+      <c r="Y6" s="54"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="54"/>
+      <c r="AC6" s="54"/>
+      <c r="AD6" s="54"/>
+      <c r="AE6" s="54"/>
+      <c r="AF6" s="54"/>
+      <c r="AG6" s="54"/>
+      <c r="AH6" s="54"/>
+      <c r="AI6" s="54"/>
+      <c r="AJ6" s="54"/>
+      <c r="AK6" s="54"/>
+      <c r="AL6" s="54"/>
+      <c r="AM6" s="54"/>
+      <c r="AN6" s="54"/>
+      <c r="AO6" s="54"/>
+      <c r="AP6" s="54"/>
+      <c r="AQ6" s="54"/>
+      <c r="AR6" s="54"/>
+      <c r="AS6" s="54"/>
+      <c r="AT6" s="54"/>
+      <c r="AU6" s="54"/>
+      <c r="AV6" s="54"/>
+      <c r="AW6" s="54"/>
+      <c r="AX6" s="54"/>
+      <c r="AY6" s="54"/>
+      <c r="AZ6" s="54"/>
+      <c r="BA6" s="54"/>
+      <c r="BB6" s="54"/>
+      <c r="BC6" s="54"/>
+      <c r="BD6" s="54"/>
+      <c r="BE6" s="54"/>
+      <c r="BF6" s="54"/>
+      <c r="BG6" s="54"/>
+      <c r="BH6" s="54"/>
+      <c r="BI6" s="54"/>
+      <c r="BJ6" s="54"/>
+      <c r="BK6" s="54"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="54"/>
+      <c r="BN6" s="54"/>
+      <c r="BO6" s="54"/>
+      <c r="BP6" s="54"/>
+      <c r="BQ6" s="54"/>
+      <c r="BR6" s="54"/>
+      <c r="BS6" s="54"/>
+      <c r="BT6" s="54"/>
+      <c r="BU6" s="54"/>
+      <c r="BV6" s="54"/>
+      <c r="BW6" s="54"/>
+      <c r="BX6" s="54"/>
+      <c r="BY6" s="54"/>
+      <c r="BZ6" s="54"/>
+    </row>
+    <row r="7" spans="1:78" ht="16.3" customHeight="1">
       <c r="A7" s="57" t="s">
-        <v>3153</v>
-      </c>
+        <v>5243</v>
+      </c>
+      <c r="B7" s="57"/>
       <c r="C7" s="57" t="s">
-        <v>5228</v>
-      </c>
-      <c r="F7" s="82"/>
+        <v>5245</v>
+      </c>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="79"/>
       <c r="H7" s="73"/>
       <c r="I7" s="75"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
     </row>
     <row r="8" spans="1:78" ht="15.9">
-      <c r="A8" s="92" t="s">
-        <v>5225</v>
-      </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="79"/>
+      <c r="A8" s="57" t="s">
+        <v>3153</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>5228</v>
+      </c>
+      <c r="F8" s="82"/>
       <c r="H8" s="73"/>
       <c r="I8" s="75"/>
     </row>
     <row r="9" spans="1:78" ht="15.9">
-      <c r="A9" s="57" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B9" s="57" t="s">
-        <v>1101</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>2503</v>
-      </c>
+      <c r="A9" s="92" t="s">
+        <v>5225</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="79"/>
       <c r="H9" s="73"/>
       <c r="I9" s="75"/>
     </row>
     <row r="10" spans="1:78" ht="15.9">
-      <c r="A10" s="55"/>
-      <c r="B10" s="55" t="s">
-        <v>5230</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>5229</v>
-      </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
+      <c r="A10" s="57" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
       <c r="H10" s="73"/>
       <c r="I10" s="75"/>
     </row>
     <row r="11" spans="1:78" ht="15.9">
-      <c r="A11" s="57"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="84"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55" t="s">
+        <v>5230</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>5229</v>
+      </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
       <c r="H11" s="73"/>
       <c r="I11" s="75"/>
     </row>
     <row r="12" spans="1:78" ht="15.9">
-      <c r="A12" s="55"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
       <c r="D12" s="55"/>
       <c r="E12" s="84"/>
       <c r="H12" s="73"/>
       <c r="I12" s="75"/>
     </row>
     <row r="13" spans="1:78" ht="15.9">
-      <c r="A13" s="91" t="s">
-        <v>2562</v>
-      </c>
+      <c r="A13" s="55"/>
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
@@ -17323,28 +17394,24 @@
       <c r="I13" s="75"/>
     </row>
     <row r="14" spans="1:78" ht="15.9">
-      <c r="A14" s="55" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B14" s="55" t="s">
+      <c r="A14" s="91" t="s">
         <v>2562</v>
       </c>
+      <c r="B14" s="55"/>
       <c r="C14" s="55"/>
       <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
+      <c r="E14" s="84"/>
       <c r="H14" s="73"/>
       <c r="I14" s="75"/>
     </row>
     <row r="15" spans="1:78" ht="15.9">
       <c r="A15" s="55" t="s">
-        <v>5233</v>
+        <v>1229</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>5232</v>
-      </c>
-      <c r="C15" s="55" t="s">
-        <v>5234</v>
-      </c>
+        <v>2562</v>
+      </c>
+      <c r="C15" s="55"/>
       <c r="D15" s="55"/>
       <c r="E15" s="55"/>
       <c r="H15" s="73"/>
@@ -17352,37 +17419,39 @@
     </row>
     <row r="16" spans="1:78" ht="15.9">
       <c r="A16" s="55" t="s">
-        <v>1238</v>
+        <v>5233</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>3334</v>
-      </c>
-      <c r="C16" s="55"/>
+        <v>5232</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>5234</v>
+      </c>
       <c r="D16" s="55"/>
       <c r="E16" s="55"/>
       <c r="H16" s="73"/>
       <c r="I16" s="75"/>
     </row>
-    <row r="17" spans="1:9" s="57" customFormat="1" ht="43.75">
-      <c r="A17" s="55"/>
-      <c r="B17" s="90" t="s">
-        <v>5235</v>
-      </c>
-      <c r="C17" s="90" t="s">
-        <v>5236</v>
-      </c>
+    <row r="17" spans="1:9" ht="15.9">
+      <c r="A17" s="55" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>3334</v>
+      </c>
+      <c r="C17" s="55"/>
       <c r="D17" s="55"/>
       <c r="E17" s="55"/>
       <c r="H17" s="73"/>
       <c r="I17" s="75"/>
     </row>
-    <row r="18" spans="1:9" s="57" customFormat="1" ht="15.9">
-      <c r="A18" s="56"/>
-      <c r="B18" s="56" t="s">
-        <v>5237</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>5239</v>
+    <row r="18" spans="1:9" s="57" customFormat="1" ht="43.75">
+      <c r="A18" s="55"/>
+      <c r="B18" s="90" t="s">
+        <v>5235</v>
+      </c>
+      <c r="C18" s="90" t="s">
+        <v>5236</v>
       </c>
       <c r="D18" s="55"/>
       <c r="E18" s="55"/>
@@ -17392,94 +17461,100 @@
     <row r="19" spans="1:9" s="57" customFormat="1" ht="15.9">
       <c r="A19" s="56"/>
       <c r="B19" s="56" t="s">
-        <v>5238</v>
+        <v>5237</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>5240</v>
+        <v>5239</v>
       </c>
       <c r="D19" s="55"/>
       <c r="E19" s="55"/>
       <c r="H19" s="73"/>
       <c r="I19" s="75"/>
     </row>
-    <row r="20" spans="1:9" ht="15.9">
-      <c r="A20" s="55"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="57"/>
+    <row r="20" spans="1:9" s="57" customFormat="1" ht="15.9">
+      <c r="A20" s="56"/>
+      <c r="B20" s="56" t="s">
+        <v>5238</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>5240</v>
+      </c>
+      <c r="D20" s="55"/>
       <c r="E20" s="55"/>
       <c r="H20" s="73"/>
       <c r="I20" s="75"/>
     </row>
     <row r="21" spans="1:9" ht="15.9">
-      <c r="A21" s="57"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
       <c r="D21" s="57"/>
       <c r="E21" s="55"/>
       <c r="H21" s="73"/>
       <c r="I21" s="75"/>
     </row>
     <row r="22" spans="1:9" ht="15.9">
-      <c r="A22" s="37" t="s">
-        <v>2505</v>
-      </c>
+      <c r="A22" s="57"/>
       <c r="B22" s="57"/>
       <c r="C22" s="57"/>
-      <c r="D22" s="57" t="s">
-        <v>5226</v>
-      </c>
+      <c r="D22" s="57"/>
       <c r="E22" s="55"/>
       <c r="H22" s="73"/>
       <c r="I22" s="75"/>
     </row>
     <row r="23" spans="1:9" ht="15.9">
-      <c r="C23" s="57" t="s">
-        <v>2084</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>5231</v>
+      <c r="A23" s="37" t="s">
+        <v>2505</v>
+      </c>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57" t="s">
+        <v>5226</v>
       </c>
       <c r="E23" s="55"/>
       <c r="H23" s="73"/>
       <c r="I23" s="75"/>
     </row>
     <row r="24" spans="1:9" ht="15.9">
-      <c r="A24" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="57" t="s">
+        <v>2084</v>
+      </c>
       <c r="D24" s="10" t="s">
-        <v>2048</v>
+        <v>5231</v>
       </c>
       <c r="E24" s="55"/>
       <c r="H24" s="73"/>
       <c r="I24" s="75"/>
     </row>
-    <row r="25" spans="1:9" s="57" customFormat="1" ht="15.9">
+    <row r="25" spans="1:9" ht="15.9">
       <c r="A25" s="13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>1912</v>
+        <v>363</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>2048</v>
       </c>
       <c r="E25" s="55"/>
-      <c r="F25" s="31"/>
       <c r="H25" s="73"/>
       <c r="I25" s="75"/>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
+    <row r="26" spans="1:9" s="57" customFormat="1" ht="15.9">
+      <c r="A26" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>1912</v>
+      </c>
       <c r="E26" s="55"/>
+      <c r="F26" s="31"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="75"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="57"/>
@@ -17489,16 +17564,16 @@
       <c r="E27" s="55"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="D28" s="54"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="55"/>
-      <c r="F28" s="57"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="55"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="55"/>
+      <c r="F29" s="57"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="55"/>
@@ -17518,7 +17593,7 @@
       <c r="A32" s="55"/>
       <c r="B32" s="55"/>
       <c r="C32" s="55"/>
-      <c r="D32" s="54"/>
+      <c r="D32" s="55"/>
       <c r="E32" s="55"/>
     </row>
     <row r="33" spans="1:5">
@@ -17528,19 +17603,19 @@
       <c r="D33" s="54"/>
       <c r="E33" s="55"/>
     </row>
-    <row r="34" spans="1:5" ht="15.9">
+    <row r="34" spans="1:5">
       <c r="A34" s="55"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="83"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="D34" s="54"/>
+      <c r="E34" s="55"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.9">
       <c r="A35" s="55"/>
       <c r="B35" s="55"/>
       <c r="C35" s="55"/>
       <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
+      <c r="E35" s="83"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="55"/>
@@ -17549,38 +17624,38 @@
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
     </row>
-    <row r="37" spans="1:5" ht="15.9">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
+    <row r="37" spans="1:5">
+      <c r="A37" s="55"/>
+      <c r="B37" s="55"/>
       <c r="C37" s="55"/>
-      <c r="D37" s="88"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="55"/>
     </row>
     <row r="38" spans="1:5" ht="15.9">
       <c r="A38" s="82"/>
       <c r="B38" s="83"/>
-      <c r="C38" s="88"/>
-      <c r="D38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="88"/>
       <c r="E38" s="55"/>
     </row>
     <row r="39" spans="1:5" ht="15.9">
       <c r="A39" s="82"/>
       <c r="B39" s="83"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="83"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="55"/>
       <c r="E39" s="55"/>
     </row>
     <row r="40" spans="1:5" ht="15.9">
       <c r="A40" s="82"/>
       <c r="B40" s="83"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="85"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="83"/>
       <c r="E40" s="55"/>
     </row>
     <row r="41" spans="1:5" ht="15.9">
       <c r="A41" s="82"/>
       <c r="B41" s="83"/>
-      <c r="C41" s="85"/>
+      <c r="C41" s="83"/>
       <c r="D41" s="85"/>
       <c r="E41" s="55"/>
     </row>
@@ -17588,19 +17663,19 @@
       <c r="A42" s="82"/>
       <c r="B42" s="83"/>
       <c r="C42" s="85"/>
-      <c r="D42" s="55"/>
+      <c r="D42" s="85"/>
       <c r="E42" s="55"/>
     </row>
     <row r="43" spans="1:5" ht="15.9">
       <c r="A43" s="82"/>
       <c r="B43" s="83"/>
-      <c r="C43" s="55"/>
+      <c r="C43" s="85"/>
       <c r="D43" s="55"/>
       <c r="E43" s="55"/>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="55"/>
-      <c r="B44" s="55"/>
+    <row r="44" spans="1:5" ht="15.9">
+      <c r="A44" s="82"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="55"/>
       <c r="D44" s="55"/>
       <c r="E44" s="55"/>
@@ -17620,7 +17695,7 @@
       <c r="E46" s="55"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="89"/>
+      <c r="A47" s="55"/>
       <c r="B47" s="55"/>
       <c r="C47" s="55"/>
       <c r="D47" s="55"/>
@@ -17633,32 +17708,32 @@
       <c r="D48" s="55"/>
       <c r="E48" s="55"/>
     </row>
-    <row r="49" spans="1:6" ht="15">
-      <c r="A49" s="55"/>
-      <c r="B49" s="87"/>
-      <c r="C49" s="87"/>
+    <row r="49" spans="1:6">
+      <c r="A49" s="89"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="55"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" ht="15">
       <c r="A50" s="55"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="87"/>
       <c r="D50" s="55"/>
       <c r="E50" s="55"/>
-      <c r="F50" s="57"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.9">
-      <c r="A51" s="85"/>
-      <c r="B51" s="86"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="55"/>
+      <c r="B51" s="55"/>
       <c r="C51" s="55"/>
-      <c r="D51" s="83"/>
+      <c r="D51" s="55"/>
       <c r="E51" s="55"/>
+      <c r="F51" s="57"/>
     </row>
     <row r="52" spans="1:6" ht="15.9">
-      <c r="A52" s="83"/>
-      <c r="B52" s="83"/>
-      <c r="C52" s="83"/>
+      <c r="A52" s="85"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="55"/>
       <c r="D52" s="83"/>
       <c r="E52" s="55"/>
     </row>
@@ -17687,13 +17762,13 @@
       <c r="A56" s="83"/>
       <c r="B56" s="83"/>
       <c r="C56" s="83"/>
-      <c r="D56" s="55"/>
+      <c r="D56" s="83"/>
       <c r="E56" s="55"/>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="55"/>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
+    <row r="57" spans="1:6" ht="15.9">
+      <c r="A57" s="83"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="83"/>
       <c r="D57" s="55"/>
       <c r="E57" s="55"/>
     </row>
@@ -17785,13 +17860,20 @@
       <c r="A70" s="55"/>
       <c r="B70" s="55"/>
       <c r="C70" s="55"/>
-      <c r="D70" s="77"/>
-      <c r="E70" s="77"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="77"/>
-      <c r="B71" s="77"/>
-      <c r="C71" s="77"/>
+      <c r="A71" s="55"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="77"/>
+      <c r="E71" s="77"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="77"/>
+      <c r="B72" s="77"/>
+      <c r="C72" s="77"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Giant proofreading! Thanks to all the playtesters so far!
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -45,7 +45,7 @@
     <definedName name="state" localSheetId="8">Sheet2!$A$1:$C$117</definedName>
     <definedName name="Unit_Command_1" localSheetId="5">'Unit Command'!$F$21:$F$70</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -16489,13 +16489,13 @@
     <t>Bring your face closer…</t>
   </si>
   <si>
-    <t>Resist ｔemptation</t>
-  </si>
-  <si>
     <t>回復を得意とする。レシナの街でメンバーに加入した。</t>
   </si>
   <si>
     <t>Skilled at healing others. Joined the group at the town of Reshina.</t>
+  </si>
+  <si>
+    <t>Bandit Lacky</t>
   </si>
 </sst>
 </file>
@@ -17445,8 +17445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BZ102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -17745,7 +17745,7 @@
         <v>5225</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>2621</v>
+        <v>5377</v>
       </c>
       <c r="D6" s="56"/>
       <c r="E6" s="56"/>
@@ -18047,13 +18047,13 @@
         <v>39</v>
       </c>
       <c r="B16" s="107" t="s">
-        <v>5376</v>
+        <v>5375</v>
       </c>
       <c r="C16" s="57" t="s">
         <v>2168</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>5377</v>
+        <v>5376</v>
       </c>
       <c r="E16" s="83"/>
       <c r="F16" s="79"/>
@@ -18663,7 +18663,7 @@
         <v>934</v>
       </c>
       <c r="D63" s="102" t="s">
-        <v>5375</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="57" customFormat="1" ht="15.9">
@@ -18711,9 +18711,6 @@
       <c r="B68" s="67"/>
       <c r="C68" s="67"/>
       <c r="D68" s="67"/>
-      <c r="E68" s="93" t="s">
-        <v>5329</v>
-      </c>
     </row>
     <row r="69" spans="1:5" ht="15">
       <c r="A69" s="67" t="s">
@@ -18729,7 +18726,7 @@
         <v>5257</v>
       </c>
       <c r="E69" s="93" t="s">
-        <v>5330</v>
+        <v>5329</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15">
@@ -18740,7 +18737,7 @@
         <v>4261</v>
       </c>
       <c r="E70" s="93" t="s">
-        <v>5329</v>
+        <v>5330</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15">
@@ -18753,7 +18750,7 @@
         <v>5257</v>
       </c>
       <c r="E71" s="93" t="s">
-        <v>5330</v>
+        <v>5329</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15">
@@ -18763,16 +18760,16 @@
       <c r="D72" s="73" t="s">
         <v>4261</v>
       </c>
-      <c r="E72" s="67"/>
+      <c r="E72" s="93" t="s">
+        <v>5330</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="15">
       <c r="A73" s="67"/>
       <c r="B73" s="67"/>
       <c r="C73" s="67"/>
       <c r="D73" s="67"/>
-      <c r="E73" s="93" t="s">
-        <v>5331</v>
-      </c>
+      <c r="E73" s="67"/>
     </row>
     <row r="74" spans="1:5" ht="15">
       <c r="A74" s="67" t="s">
@@ -18788,7 +18785,7 @@
         <v>5259</v>
       </c>
       <c r="E74" s="93" t="s">
-        <v>4273</v>
+        <v>5331</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15">
@@ -18799,7 +18796,7 @@
         <v>5260</v>
       </c>
       <c r="E75" s="93" t="s">
-        <v>5331</v>
+        <v>4273</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15">
@@ -18812,7 +18809,7 @@
         <v>5259</v>
       </c>
       <c r="E76" s="93" t="s">
-        <v>4273</v>
+        <v>5331</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15">
@@ -18822,7 +18819,9 @@
       <c r="D77" s="73" t="s">
         <v>5260</v>
       </c>
-      <c r="E77" s="55"/>
+      <c r="E77" s="93" t="s">
+        <v>4273</v>
+      </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="87"/>
@@ -37538,13 +37537,13 @@
         <v>39</v>
       </c>
       <c r="D17" s="107" t="s">
-        <v>5376</v>
+        <v>5375</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>2168</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>5377</v>
+        <v>5376</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Updated names for iroji
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -17514,7 +17514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BZ120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -37521,8 +37521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F123" sqref="B112:F123"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>

</xml_diff>

<commit_message>
Black Market Translation Update
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7646" uniqueCount="5395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7649" uniqueCount="5397">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16520,6 +16520,12 @@
   </si>
   <si>
     <t>Remia</t>
+  </si>
+  <si>
+    <t>side4</t>
+  </si>
+  <si>
+    <t>Black Marketeer</t>
   </si>
 </sst>
 </file>
@@ -36912,10 +36918,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H125"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+      <selection activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
@@ -38800,6 +38806,17 @@
       </c>
       <c r="E125" s="57" t="s">
         <v>5394</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="B127" s="57" t="s">
+        <v>5395</v>
+      </c>
+      <c r="C127" s="57" t="s">
+        <v>5239</v>
+      </c>
+      <c r="E127" s="57" t="s">
+        <v>5396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big Black Market translation
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7649" uniqueCount="5397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7651" uniqueCount="5398">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16526,6 +16526,9 @@
   </si>
   <si>
     <t>Black Marketeer</t>
+  </si>
+  <si>
+    <t>Aphrodisiac Succubus</t>
   </si>
 </sst>
 </file>
@@ -36918,10 +36921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
@@ -38817,6 +38820,14 @@
       </c>
       <c r="E127" s="57" t="s">
         <v>5396</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="C128" s="57" t="s">
+        <v>5237</v>
+      </c>
+      <c r="E128" s="57" t="s">
+        <v>5397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aphrodisiac succubus done. Perfume Succubus Translation
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7651" uniqueCount="5398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7653" uniqueCount="5399">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16529,6 +16529,9 @@
   </si>
   <si>
     <t>Aphrodisiac Succubus</t>
+  </si>
+  <si>
+    <t>Perfume Succubus</t>
   </si>
 </sst>
 </file>
@@ -36921,10 +36924,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
@@ -38828,6 +38831,14 @@
       </c>
       <c r="E128" s="57" t="s">
         <v>5397</v>
+      </c>
+    </row>
+    <row r="129" spans="3:5">
+      <c r="C129" s="57" t="s">
+        <v>5235</v>
+      </c>
+      <c r="E129" s="57" t="s">
+        <v>5398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update is ready to go!
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="23" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7692" uniqueCount="5434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7756" uniqueCount="5461">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16637,6 +16637,87 @@
   </si>
   <si>
     <t>Lotion Succubus</t>
+  </si>
+  <si>
+    <t>吸精の牢屋</t>
+  </si>
+  <si>
+    <t>The Semen Squeezing Jailhouse</t>
+  </si>
+  <si>
+    <t>ドレインサキュバスの施設から兵士たちを救い出そう</t>
+  </si>
+  <si>
+    <t>Free the soldiers from the Drain Succubus facility!</t>
+  </si>
+  <si>
+    <t>Chapters</t>
+  </si>
+  <si>
+    <t>クエスト</t>
+  </si>
+  <si>
+    <t>Subquests</t>
+  </si>
+  <si>
+    <t>Side 5</t>
+  </si>
+  <si>
+    <t>サキュバスに命を吸い取られた成れの果て。</t>
+  </si>
+  <si>
+    <t>A former shell of one who's life was drained by succubus.</t>
+  </si>
+  <si>
+    <t>山積みの骨</t>
+  </si>
+  <si>
+    <t>吸いつくされた兵士たちの骨。 スケル卜ンを生み出す。</t>
+  </si>
+  <si>
+    <t>サキュバスの偉い魔。 空を飛んで襲ってくる。</t>
+  </si>
+  <si>
+    <t>ドレイ ン乳魔</t>
+  </si>
+  <si>
+    <t>パイズリで男の レべルを吸うサキュバス。</t>
+  </si>
+  <si>
+    <t>王国の兵士</t>
+  </si>
+  <si>
+    <t>Drain Imp</t>
+  </si>
+  <si>
+    <t>Boob Drain Succubus</t>
+  </si>
+  <si>
+    <t>A demon valued by all succubi. Flies high in the air.</t>
+  </si>
+  <si>
+    <t>ドレインを得意とするインプ。 力と速さを吸ってくる。</t>
+  </si>
+  <si>
+    <t>ドレインを得意とするインプ。 HPと守備カを吸ってくる。</t>
+  </si>
+  <si>
+    <t>An imp proficient at draining. Saps away at Str and Spd.</t>
+  </si>
+  <si>
+    <t>An imp proficient at draining. Saps away at HP and Def.</t>
+  </si>
+  <si>
+    <t>A succubus who uses paizuri to drain the levels of men.</t>
+  </si>
+  <si>
+    <t>Royal Guard</t>
+  </si>
+  <si>
+    <t>Pile of Bones</t>
+  </si>
+  <si>
+    <t>The bones of dried up soldiers. Spawns skeletons.</t>
   </si>
 </sst>
 </file>
@@ -17590,8 +17671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BZ120"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E28" sqref="A20:E28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -18160,7 +18241,9 @@
       <c r="J19" s="55"/>
     </row>
     <row r="20" spans="1:10" ht="15.9">
-      <c r="A20" s="57"/>
+      <c r="A20" s="57" t="s">
+        <v>5441</v>
+      </c>
       <c r="B20" s="57"/>
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
@@ -18173,10 +18256,18 @@
     </row>
     <row r="21" spans="1:10" ht="15.9">
       <c r="A21" s="57"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
+      <c r="B21" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>5442</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>2163</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>5443</v>
+      </c>
       <c r="F21" s="57"/>
       <c r="G21" s="55"/>
       <c r="H21" s="81"/>
@@ -18184,6 +18275,18 @@
       <c r="J21" s="55"/>
     </row>
     <row r="22" spans="1:10" s="57" customFormat="1" ht="15.9">
+      <c r="B22" s="57" t="s">
+        <v>2674</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>5446</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>2847</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>5452</v>
+      </c>
       <c r="G22" s="55"/>
       <c r="H22" s="81"/>
       <c r="I22" s="82"/>
@@ -18191,10 +18294,18 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
+      <c r="B23" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>5453</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>5450</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>5455</v>
+      </c>
       <c r="G23" s="55"/>
       <c r="H23" s="55"/>
       <c r="I23" s="55"/>
@@ -18202,10 +18313,18 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="57"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
+      <c r="B24" s="57" t="s">
+        <v>5447</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>5448</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>5451</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>5457</v>
+      </c>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="55"/>
@@ -18213,24 +18332,44 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
+      <c r="B25" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>5454</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>5450</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>5456</v>
+      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
+      <c r="B26" s="57" t="s">
+        <v>5449</v>
+      </c>
       <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
+      <c r="D26" s="57" t="s">
+        <v>5458</v>
+      </c>
       <c r="E26" s="57"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="57"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
+      <c r="B27" s="57" t="s">
+        <v>5444</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>5445</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>5459</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>5460</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="57"/>
@@ -18287,8 +18426,12 @@
       <c r="E36" s="55"/>
     </row>
     <row r="37" spans="1:6" ht="15">
-      <c r="A37" s="57"/>
-      <c r="B37" s="57"/>
+      <c r="A37" s="57" t="s">
+        <v>5439</v>
+      </c>
+      <c r="B37" s="57" t="s">
+        <v>5440</v>
+      </c>
       <c r="C37" s="57"/>
       <c r="D37" s="56"/>
       <c r="E37" s="55"/>
@@ -18316,18 +18459,26 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="88" t="s">
-        <v>2554</v>
+        <v>5438</v>
       </c>
       <c r="B41" s="55"/>
       <c r="C41" s="55"/>
       <c r="D41" s="55"/>
       <c r="E41" s="55"/>
     </row>
-    <row r="42" spans="1:6" s="57" customFormat="1">
-      <c r="A42" s="55"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
+    <row r="42" spans="1:6" s="57" customFormat="1" ht="15">
+      <c r="A42" s="56" t="s">
+        <v>5434</v>
+      </c>
+      <c r="B42" s="57" t="s">
+        <v>5435</v>
+      </c>
+      <c r="C42" s="56" t="s">
+        <v>5436</v>
+      </c>
+      <c r="D42" s="56" t="s">
+        <v>5437</v>
+      </c>
       <c r="E42" s="55"/>
     </row>
     <row r="43" spans="1:6" s="57" customFormat="1">
@@ -18345,10 +18496,6 @@
       <c r="E44" s="55"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="55"/>
-      <c r="B45" s="87"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="55"/>
       <c r="E45" s="55"/>
     </row>
     <row r="46" spans="1:6" ht="15">
@@ -35328,7 +35475,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.15"/>
@@ -35520,7 +35667,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="A2:D17"/>
+      <selection activeCell="D18" sqref="A18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15"/>
@@ -35870,7 +36017,18 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15">
-      <c r="B18" s="14"/>
+      <c r="A18" t="s">
+        <v>5434</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>5435</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5436</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5437</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15">
       <c r="B19" s="14"/>
@@ -37047,10 +37205,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView topLeftCell="B127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F143" sqref="B136:F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
@@ -39049,6 +39207,103 @@
       </c>
       <c r="F133" s="57" t="s">
         <v>5407</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="B136" s="57" t="s">
+        <v>5441</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="C137" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D137" s="57" t="s">
+        <v>5442</v>
+      </c>
+      <c r="E137" s="57" t="s">
+        <v>2163</v>
+      </c>
+      <c r="F137" s="57" t="s">
+        <v>5443</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="C138" s="57" t="s">
+        <v>2674</v>
+      </c>
+      <c r="D138" s="57" t="s">
+        <v>5446</v>
+      </c>
+      <c r="E138" s="57" t="s">
+        <v>2847</v>
+      </c>
+      <c r="F138" s="57" t="s">
+        <v>5452</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="C139" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="D139" s="57" t="s">
+        <v>5453</v>
+      </c>
+      <c r="E139" s="57" t="s">
+        <v>5450</v>
+      </c>
+      <c r="F139" s="57" t="s">
+        <v>5455</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="C140" s="57" t="s">
+        <v>5447</v>
+      </c>
+      <c r="D140" s="57" t="s">
+        <v>5448</v>
+      </c>
+      <c r="E140" s="57" t="s">
+        <v>5451</v>
+      </c>
+      <c r="F140" s="57" t="s">
+        <v>5457</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="C141" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="D141" s="57" t="s">
+        <v>5454</v>
+      </c>
+      <c r="E141" s="57" t="s">
+        <v>5450</v>
+      </c>
+      <c r="F141" s="57" t="s">
+        <v>5456</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="C142" s="57" t="s">
+        <v>5449</v>
+      </c>
+      <c r="E142" s="57" t="s">
+        <v>5458</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="C143" s="57" t="s">
+        <v>5444</v>
+      </c>
+      <c r="D143" s="57" t="s">
+        <v>5445</v>
+      </c>
+      <c r="E143" s="57" t="s">
+        <v>5459</v>
+      </c>
+      <c r="F143" s="57" t="s">
+        <v>5460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All current playtesting fixes
</commit_message>
<xml_diff>
--- a/固有名詞 (Literally everything else).xlsx
+++ b/固有名詞 (Literally everything else).xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7756" uniqueCount="5461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7728" uniqueCount="5460">
   <si>
     <t>カテゴリ</t>
   </si>
@@ -16537,9 +16537,6 @@
     <t>A succubus adept at Level Drain.</t>
   </si>
   <si>
-    <t>A succubus who uses aphrodasiacs to seduce men.</t>
-  </si>
-  <si>
     <t>媚藁を使って男を誘惑してくるサキュバス</t>
   </si>
   <si>
@@ -16654,12 +16651,6 @@
     <t>Chapters</t>
   </si>
   <si>
-    <t>クエスト</t>
-  </si>
-  <si>
-    <t>Subquests</t>
-  </si>
-  <si>
     <t>Side 5</t>
   </si>
   <si>
@@ -16718,6 +16709,12 @@
   </si>
   <si>
     <t>The bones of dried up soldiers. Spawns skeletons.</t>
+  </si>
+  <si>
+    <t>Side4</t>
+  </si>
+  <si>
+    <t>A succubus who uses aphrodisiacs to seduce men.</t>
   </si>
 </sst>
 </file>
@@ -17672,7 +17669,7 @@
   <dimension ref="A1:BZ120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.6"/>
@@ -18123,7 +18120,7 @@
     </row>
     <row r="9" spans="1:78" ht="15.9">
       <c r="A9" s="109" t="s">
-        <v>5430</v>
+        <v>5429</v>
       </c>
       <c r="B9" s="57"/>
       <c r="C9" s="57"/>
@@ -18241,9 +18238,7 @@
       <c r="J19" s="55"/>
     </row>
     <row r="20" spans="1:10" ht="15.9">
-      <c r="A20" s="57" t="s">
-        <v>5441</v>
-      </c>
+      <c r="A20" s="57"/>
       <c r="B20" s="57"/>
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
@@ -18255,18 +18250,20 @@
       <c r="J20" s="55"/>
     </row>
     <row r="21" spans="1:10" ht="15.9">
-      <c r="A21" s="57"/>
+      <c r="A21" s="57" t="s">
+        <v>5458</v>
+      </c>
       <c r="B21" s="57" t="s">
-        <v>29</v>
+        <v>5237</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>5442</v>
+        <v>5400</v>
       </c>
       <c r="D21" s="57" t="s">
-        <v>2163</v>
+        <v>5432</v>
       </c>
       <c r="E21" s="57" t="s">
-        <v>5443</v>
+        <v>5459</v>
       </c>
       <c r="F21" s="57"/>
       <c r="G21" s="55"/>
@@ -18275,18 +18272,6 @@
       <c r="J21" s="55"/>
     </row>
     <row r="22" spans="1:10" s="57" customFormat="1" ht="15.9">
-      <c r="B22" s="57" t="s">
-        <v>2674</v>
-      </c>
-      <c r="C22" s="57" t="s">
-        <v>5446</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>2847</v>
-      </c>
-      <c r="E22" s="57" t="s">
-        <v>5452</v>
-      </c>
       <c r="G22" s="55"/>
       <c r="H22" s="81"/>
       <c r="I22" s="82"/>
@@ -18294,18 +18279,10 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="57"/>
-      <c r="B23" s="57" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>5453</v>
-      </c>
-      <c r="D23" s="57" t="s">
-        <v>5450</v>
-      </c>
-      <c r="E23" s="57" t="s">
-        <v>5455</v>
-      </c>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
       <c r="G23" s="55"/>
       <c r="H23" s="55"/>
       <c r="I23" s="55"/>
@@ -18313,18 +18290,10 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="57"/>
-      <c r="B24" s="57" t="s">
-        <v>5447</v>
-      </c>
-      <c r="C24" s="57" t="s">
-        <v>5448</v>
-      </c>
-      <c r="D24" s="57" t="s">
-        <v>5451</v>
-      </c>
-      <c r="E24" s="57" t="s">
-        <v>5457</v>
-      </c>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
       <c r="G24" s="55"/>
       <c r="H24" s="55"/>
       <c r="I24" s="55"/>
@@ -18332,44 +18301,24 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="57"/>
-      <c r="B25" s="57" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="57" t="s">
-        <v>5454</v>
-      </c>
-      <c r="D25" s="57" t="s">
-        <v>5450</v>
-      </c>
-      <c r="E25" s="57" t="s">
-        <v>5456</v>
-      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="57"/>
-      <c r="B26" s="57" t="s">
-        <v>5449</v>
-      </c>
+      <c r="B26" s="57"/>
       <c r="C26" s="57"/>
-      <c r="D26" s="57" t="s">
-        <v>5458</v>
-      </c>
+      <c r="D26" s="57"/>
       <c r="E26" s="57"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="57"/>
-      <c r="B27" s="57" t="s">
-        <v>5444</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>5445</v>
-      </c>
-      <c r="D27" s="57" t="s">
-        <v>5459</v>
-      </c>
-      <c r="E27" s="57" t="s">
-        <v>5460</v>
-      </c>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="57"/>
@@ -18426,12 +18375,8 @@
       <c r="E36" s="55"/>
     </row>
     <row r="37" spans="1:6" ht="15">
-      <c r="A37" s="57" t="s">
-        <v>5439</v>
-      </c>
-      <c r="B37" s="57" t="s">
-        <v>5440</v>
-      </c>
+      <c r="A37" s="57"/>
+      <c r="B37" s="57"/>
       <c r="C37" s="57"/>
       <c r="D37" s="56"/>
       <c r="E37" s="55"/>
@@ -18459,7 +18404,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="88" t="s">
-        <v>5438</v>
+        <v>5437</v>
       </c>
       <c r="B41" s="55"/>
       <c r="C41" s="55"/>
@@ -18467,18 +18412,9 @@
       <c r="E41" s="55"/>
     </row>
     <row r="42" spans="1:6" s="57" customFormat="1" ht="15">
-      <c r="A42" s="56" t="s">
-        <v>5434</v>
-      </c>
-      <c r="B42" s="57" t="s">
-        <v>5435</v>
-      </c>
-      <c r="C42" s="56" t="s">
-        <v>5436</v>
-      </c>
-      <c r="D42" s="56" t="s">
-        <v>5437</v>
-      </c>
+      <c r="A42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
       <c r="E42" s="55"/>
     </row>
     <row r="43" spans="1:6" s="57" customFormat="1">
@@ -23027,16 +22963,16 @@
     </row>
     <row r="15" spans="1:7" s="56" customFormat="1" ht="15.9">
       <c r="A15" s="13" t="s">
+        <v>5417</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>5418</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="10" t="s">
         <v>5419</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>5420</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>5421</v>
       </c>
       <c r="E15" s="57"/>
       <c r="F15" s="57"/>
@@ -36018,16 +35954,16 @@
     </row>
     <row r="18" spans="1:6" ht="15">
       <c r="A18" t="s">
+        <v>5433</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>5434</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="C18" t="s">
         <v>5435</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>5436</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5437</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15">
@@ -37207,8 +37143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView topLeftCell="B127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F143" sqref="B136:F143"/>
+    <sheetView topLeftCell="B121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
@@ -39107,27 +39043,27 @@
         <v>2674</v>
       </c>
       <c r="D126" s="57" t="s">
-        <v>5406</v>
+        <v>5405</v>
       </c>
       <c r="E126" s="57" t="s">
         <v>2847</v>
       </c>
       <c r="F126" s="57" t="s">
-        <v>5407</v>
+        <v>5406</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="C127" s="57" t="s">
+        <v>5413</v>
+      </c>
+      <c r="D127" s="57" t="s">
+        <v>5415</v>
+      </c>
+      <c r="E127" s="57" t="s">
         <v>5414</v>
       </c>
-      <c r="D127" s="57" t="s">
+      <c r="F127" s="57" t="s">
         <v>5416</v>
-      </c>
-      <c r="E127" s="57" t="s">
-        <v>5415</v>
-      </c>
-      <c r="F127" s="57" t="s">
-        <v>5417</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -39138,13 +39074,13 @@
         <v>5239</v>
       </c>
       <c r="D129" s="57" t="s">
-        <v>5402</v>
+        <v>5401</v>
       </c>
       <c r="E129" s="57" t="s">
         <v>5396</v>
       </c>
       <c r="F129" s="57" t="s">
-        <v>5403</v>
+        <v>5402</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -39152,13 +39088,13 @@
         <v>5237</v>
       </c>
       <c r="D130" s="57" t="s">
-        <v>5401</v>
+        <v>5400</v>
       </c>
       <c r="E130" s="57" t="s">
-        <v>5433</v>
+        <v>5432</v>
       </c>
       <c r="F130" s="57" t="s">
-        <v>5400</v>
+        <v>5459</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -39166,52 +39102,52 @@
         <v>5235</v>
       </c>
       <c r="D131" s="57" t="s">
-        <v>5404</v>
+        <v>5403</v>
       </c>
       <c r="E131" s="57" t="s">
         <v>5397</v>
       </c>
       <c r="F131" s="57" t="s">
-        <v>5405</v>
+        <v>5404</v>
       </c>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="57" t="s">
+        <v>5408</v>
+      </c>
+      <c r="B132" s="57" t="s">
         <v>5409</v>
       </c>
-      <c r="B132" s="57" t="s">
+      <c r="C132" s="57" t="s">
+        <v>5407</v>
+      </c>
+      <c r="D132" s="57" t="s">
+        <v>5411</v>
+      </c>
+      <c r="E132" s="57" t="s">
         <v>5410</v>
       </c>
-      <c r="C132" s="57" t="s">
-        <v>5408</v>
-      </c>
-      <c r="D132" s="57" t="s">
+      <c r="F132" s="57" t="s">
         <v>5412</v>
-      </c>
-      <c r="E132" s="57" t="s">
-        <v>5411</v>
-      </c>
-      <c r="F132" s="57" t="s">
-        <v>5413</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="57" t="s">
+        <v>5430</v>
+      </c>
+      <c r="D133" s="57" t="s">
+        <v>5405</v>
+      </c>
+      <c r="E133" s="57" t="s">
         <v>5431</v>
       </c>
-      <c r="D133" s="57" t="s">
+      <c r="F133" s="57" t="s">
         <v>5406</v>
-      </c>
-      <c r="E133" s="57" t="s">
-        <v>5432</v>
-      </c>
-      <c r="F133" s="57" t="s">
-        <v>5407</v>
       </c>
     </row>
     <row r="136" spans="1:6">
       <c r="B136" s="57" t="s">
-        <v>5441</v>
+        <v>5438</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -39219,13 +39155,13 @@
         <v>29</v>
       </c>
       <c r="D137" s="57" t="s">
-        <v>5442</v>
+        <v>5439</v>
       </c>
       <c r="E137" s="57" t="s">
         <v>2163</v>
       </c>
       <c r="F137" s="57" t="s">
-        <v>5443</v>
+        <v>5440</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -39233,13 +39169,13 @@
         <v>2674</v>
       </c>
       <c r="D138" s="57" t="s">
-        <v>5446</v>
+        <v>5443</v>
       </c>
       <c r="E138" s="57" t="s">
         <v>2847</v>
       </c>
       <c r="F138" s="57" t="s">
-        <v>5452</v>
+        <v>5449</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -39247,27 +39183,27 @@
         <v>121</v>
       </c>
       <c r="D139" s="57" t="s">
-        <v>5453</v>
+        <v>5450</v>
       </c>
       <c r="E139" s="57" t="s">
-        <v>5450</v>
+        <v>5447</v>
       </c>
       <c r="F139" s="57" t="s">
-        <v>5455</v>
+        <v>5452</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="C140" s="57" t="s">
-        <v>5447</v>
+        <v>5444</v>
       </c>
       <c r="D140" s="57" t="s">
+        <v>5445</v>
+      </c>
+      <c r="E140" s="57" t="s">
         <v>5448</v>
       </c>
-      <c r="E140" s="57" t="s">
-        <v>5451</v>
-      </c>
       <c r="F140" s="57" t="s">
-        <v>5457</v>
+        <v>5454</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -39275,35 +39211,35 @@
         <v>121</v>
       </c>
       <c r="D141" s="57" t="s">
-        <v>5454</v>
+        <v>5451</v>
       </c>
       <c r="E141" s="57" t="s">
-        <v>5450</v>
+        <v>5447</v>
       </c>
       <c r="F141" s="57" t="s">
-        <v>5456</v>
+        <v>5453</v>
       </c>
     </row>
     <row r="142" spans="1:6">
       <c r="C142" s="57" t="s">
-        <v>5449</v>
+        <v>5446</v>
       </c>
       <c r="E142" s="57" t="s">
-        <v>5458</v>
+        <v>5455</v>
       </c>
     </row>
     <row r="143" spans="1:6">
       <c r="C143" s="57" t="s">
-        <v>5444</v>
+        <v>5441</v>
       </c>
       <c r="D143" s="57" t="s">
-        <v>5445</v>
+        <v>5442</v>
       </c>
       <c r="E143" s="57" t="s">
-        <v>5459</v>
+        <v>5456</v>
       </c>
       <c r="F143" s="57" t="s">
-        <v>5460</v>
+        <v>5457</v>
       </c>
     </row>
   </sheetData>
@@ -43261,7 +43197,7 @@
         <v>3819</v>
       </c>
       <c r="B249" s="57" t="s">
-        <v>5422</v>
+        <v>5421</v>
       </c>
       <c r="C249" s="31"/>
       <c r="D249" s="31"/>
@@ -43273,7 +43209,7 @@
         <v>3820</v>
       </c>
       <c r="B250" s="57" t="s">
-        <v>5423</v>
+        <v>5422</v>
       </c>
       <c r="C250" s="31"/>
       <c r="D250" s="31"/>
@@ -43285,7 +43221,7 @@
         <v>3821</v>
       </c>
       <c r="B251" s="57" t="s">
-        <v>5424</v>
+        <v>5423</v>
       </c>
       <c r="C251" s="31"/>
       <c r="D251" s="31"/>
@@ -43297,7 +43233,7 @@
         <v>3822</v>
       </c>
       <c r="B252" s="57" t="s">
-        <v>5425</v>
+        <v>5424</v>
       </c>
       <c r="C252" s="31"/>
       <c r="D252" s="31"/>
@@ -43309,7 +43245,7 @@
         <v>3823</v>
       </c>
       <c r="B253" s="57" t="s">
-        <v>5426</v>
+        <v>5425</v>
       </c>
       <c r="C253" s="31"/>
       <c r="D253" s="31"/>
@@ -43321,7 +43257,7 @@
         <v>3824</v>
       </c>
       <c r="B254" s="57" t="s">
-        <v>5427</v>
+        <v>5426</v>
       </c>
       <c r="C254" s="31"/>
       <c r="D254" s="31"/>
@@ -43333,7 +43269,7 @@
         <v>3825</v>
       </c>
       <c r="B255" s="57" t="s">
-        <v>5428</v>
+        <v>5427</v>
       </c>
       <c r="C255" s="31"/>
       <c r="D255" s="31"/>
@@ -43345,7 +43281,7 @@
         <v>3826</v>
       </c>
       <c r="B256" s="57" t="s">
-        <v>5429</v>
+        <v>5428</v>
       </c>
       <c r="C256" s="31"/>
       <c r="D256" s="31"/>

</xml_diff>